<commit_message>
Filled in my section of costing summary
</commit_message>
<xml_diff>
--- a/Report/Costings summary.xlsx
+++ b/Report/Costings summary.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jocelyn\Desktop\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CSC3600\Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{5E4DC56D-9765-4B01-871B-1B1DEA424785}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9390" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Greg" sheetId="2" r:id="rId1"/>
@@ -18,7 +19,7 @@
     <sheet name="Isaac" sheetId="8" r:id="rId4"/>
     <sheet name="Total Hrs" sheetId="10" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="179017" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -102,7 +103,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -218,90 +219,90 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:I15" totalsRowShown="0">
-  <autoFilter ref="A1:I15"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:I15" totalsRowShown="0">
+  <autoFilter ref="A1:I15" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="Column1" dataDxfId="4"/>
-    <tableColumn id="2" name="Initialising"/>
-    <tableColumn id="3" name="Discover and understand the details of the problem"/>
-    <tableColumn id="4" name="Create the project plan."/>
-    <tableColumn id="5" name="Design Components"/>
-    <tableColumn id="6" name="Implement and Test"/>
-    <tableColumn id="7" name="Monitoring and Controlling"/>
-    <tableColumn id="8" name="Deploy"/>
-    <tableColumn id="9" name="Weekly Total"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Column1" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Initialising"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Discover and understand the details of the problem"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Create the project plan."/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Design Components"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Implement and Test"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Monitoring and Controlling"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Deploy"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Weekly Total"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A1:I15" totalsRowShown="0">
-  <autoFilter ref="A1:I15"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table13" displayName="Table13" ref="A1:I15" totalsRowShown="0">
+  <autoFilter ref="A1:I15" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="Column1" dataDxfId="3"/>
-    <tableColumn id="2" name="Initialising"/>
-    <tableColumn id="3" name="Discover and understand the details of the problem"/>
-    <tableColumn id="4" name="Create the project plan."/>
-    <tableColumn id="5" name="Design Components"/>
-    <tableColumn id="6" name="Implement and Test"/>
-    <tableColumn id="7" name="Monitoring and Controlling"/>
-    <tableColumn id="8" name="Deploy"/>
-    <tableColumn id="9" name="Weekly Total"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Column1" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Initialising"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Discover and understand the details of the problem"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Create the project plan."/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Design Components"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Implement and Test"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Monitoring and Controlling"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Deploy"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Weekly Total"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table134" displayName="Table134" ref="A1:I15" totalsRowShown="0">
-  <autoFilter ref="A1:I15"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table134" displayName="Table134" ref="A1:I15" totalsRowShown="0">
+  <autoFilter ref="A1:I15" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="Column1" dataDxfId="2"/>
-    <tableColumn id="2" name="Initialising"/>
-    <tableColumn id="3" name="Discover and understand the details of the problem"/>
-    <tableColumn id="4" name="Create the project plan."/>
-    <tableColumn id="5" name="Design Components"/>
-    <tableColumn id="6" name="Implement and Test"/>
-    <tableColumn id="7" name="Monitoring and Controlling"/>
-    <tableColumn id="8" name="Deploy"/>
-    <tableColumn id="9" name="Weekly Total"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Column1" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Initialising"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Discover and understand the details of the problem"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Create the project plan."/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Design Components"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Implement and Test"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Monitoring and Controlling"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Deploy"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="Weekly Total"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table1345" displayName="Table1345" ref="A1:I15" totalsRowShown="0">
-  <autoFilter ref="A1:I15"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table1345" displayName="Table1345" ref="A1:I15" totalsRowShown="0">
+  <autoFilter ref="A1:I15" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="Column1" dataDxfId="1"/>
-    <tableColumn id="2" name="Initialising"/>
-    <tableColumn id="3" name="Discover and understand the details of the problem"/>
-    <tableColumn id="4" name="Create the project plan."/>
-    <tableColumn id="5" name="Design Components"/>
-    <tableColumn id="6" name="Implement and Test"/>
-    <tableColumn id="7" name="Monitoring and Controlling"/>
-    <tableColumn id="8" name="Deploy"/>
-    <tableColumn id="9" name="Weekly Total"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Column1" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Initialising"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Discover and understand the details of the problem"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Create the project plan."/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Design Components"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Implement and Test"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="Monitoring and Controlling"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="Deploy"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0300-000009000000}" name="Weekly Total"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table13456" displayName="Table13456" ref="A1:I15" totalsRowShown="0">
-  <autoFilter ref="A1:I15"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table13456" displayName="Table13456" ref="A1:I15" totalsRowShown="0">
+  <autoFilter ref="A1:I15" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="Column1" dataDxfId="0"/>
-    <tableColumn id="2" name="Initialising"/>
-    <tableColumn id="3" name="Discover and understand the details of the problem"/>
-    <tableColumn id="4" name="Create the project plan."/>
-    <tableColumn id="5" name="Design Components"/>
-    <tableColumn id="6" name="Implement and Test"/>
-    <tableColumn id="7" name="Monitoring and Controlling"/>
-    <tableColumn id="8" name="Deploy"/>
-    <tableColumn id="9" name="Weekly Total"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Column1" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Initialising"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Discover and understand the details of the problem"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Create the project plan."/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="Design Components"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0400-000006000000}" name="Implement and Test"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0400-000007000000}" name="Monitoring and Controlling"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0400-000008000000}" name="Deploy"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0400-000009000000}" name="Weekly Total"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -569,25 +570,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" customWidth="1"/>
-    <col min="3" max="3" width="45.88671875" customWidth="1"/>
-    <col min="4" max="4" width="22.6640625" customWidth="1"/>
-    <col min="5" max="6" width="19.6640625" customWidth="1"/>
-    <col min="7" max="7" width="25.6640625" customWidth="1"/>
-    <col min="9" max="9" width="13.77734375" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
+    <col min="3" max="3" width="45.85546875" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" customWidth="1"/>
+    <col min="5" max="6" width="19.7109375" customWidth="1"/>
+    <col min="7" max="7" width="25.7109375" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -616,7 +617,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -634,7 +635,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -652,7 +653,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -670,7 +671,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
@@ -682,7 +683,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
@@ -694,7 +695,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -712,7 +713,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -730,7 +731,7 @@
         <v>10.5</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -745,7 +746,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
@@ -763,7 +764,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
@@ -778,7 +779,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
@@ -793,7 +794,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
@@ -802,12 +803,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>21</v>
       </c>
@@ -844,7 +845,7 @@
         <v>106.5</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -854,25 +855,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" customWidth="1"/>
-    <col min="3" max="3" width="45.88671875" customWidth="1"/>
-    <col min="4" max="4" width="22.6640625" customWidth="1"/>
-    <col min="5" max="6" width="19.6640625" customWidth="1"/>
-    <col min="7" max="7" width="25.6640625" customWidth="1"/>
-    <col min="9" max="9" width="13.77734375" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
+    <col min="3" max="3" width="45.85546875" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" customWidth="1"/>
+    <col min="5" max="6" width="19.7109375" customWidth="1"/>
+    <col min="7" max="7" width="25.7109375" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -901,7 +902,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -910,7 +911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -919,7 +920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -928,7 +929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
@@ -937,7 +938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
@@ -946,7 +947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -955,7 +956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -964,7 +965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -973,7 +974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
@@ -982,7 +983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
@@ -991,7 +992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
@@ -1000,7 +1001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
@@ -1009,12 +1010,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>21</v>
       </c>
@@ -1051,7 +1052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -1061,25 +1062,25 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" customWidth="1"/>
-    <col min="3" max="3" width="45.88671875" customWidth="1"/>
-    <col min="4" max="4" width="22.6640625" customWidth="1"/>
-    <col min="5" max="6" width="19.6640625" customWidth="1"/>
-    <col min="7" max="7" width="25.6640625" customWidth="1"/>
-    <col min="9" max="9" width="13.77734375" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
+    <col min="3" max="3" width="45.85546875" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" customWidth="1"/>
+    <col min="5" max="6" width="19.7109375" customWidth="1"/>
+    <col min="7" max="7" width="25.7109375" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -1108,106 +1109,178 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>2.5</v>
+      </c>
       <c r="I2">
         <f>SUM(B2:H2)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
       <c r="I3">
         <f t="shared" ref="I3:I13" si="0">SUM(B3:H3)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="D4">
+        <v>9.5</v>
+      </c>
       <c r="I4">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="B5">
+        <v>0.5</v>
+      </c>
+      <c r="D5">
+        <v>6</v>
+      </c>
       <c r="I5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
       <c r="I6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="B7">
+        <v>0.5</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
       <c r="I7">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="C8">
+        <v>1.5</v>
+      </c>
+      <c r="E8">
+        <v>7</v>
+      </c>
+      <c r="F8">
+        <v>3</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
       <c r="I8">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <v>4</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
       <c r="I9">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="E10">
+        <v>4</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
       <c r="I10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="E11">
+        <v>5</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
       <c r="I11">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="E12">
+        <v>3.5</v>
+      </c>
+      <c r="F12">
+        <v>0.5</v>
+      </c>
       <c r="I12">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
@@ -1216,38 +1289,38 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B15" s="1">
         <f t="shared" ref="B15:H15" si="1">SUM(B2:B14)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C15" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D15" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>15.5</v>
       </c>
       <c r="E15" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>28.5</v>
       </c>
       <c r="F15" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>9.5</v>
       </c>
       <c r="G15" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" s="1">
         <f t="shared" si="1"/>
@@ -1255,10 +1328,10 @@
       </c>
       <c r="I15" s="1">
         <f>SUM(I2:I14)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+        <v>71.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -1268,25 +1341,25 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" customWidth="1"/>
-    <col min="3" max="3" width="45.88671875" customWidth="1"/>
-    <col min="4" max="4" width="22.6640625" customWidth="1"/>
-    <col min="5" max="6" width="19.6640625" customWidth="1"/>
-    <col min="7" max="7" width="25.6640625" customWidth="1"/>
-    <col min="9" max="9" width="13.77734375" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
+    <col min="3" max="3" width="45.85546875" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" customWidth="1"/>
+    <col min="5" max="6" width="19.7109375" customWidth="1"/>
+    <col min="7" max="7" width="25.7109375" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -1315,7 +1388,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1324,7 +1397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -1333,7 +1406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -1342,7 +1415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
@@ -1351,7 +1424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
@@ -1360,7 +1433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -1369,7 +1442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -1378,7 +1451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -1387,7 +1460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
@@ -1396,7 +1469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
@@ -1405,7 +1478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
@@ -1414,7 +1487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
@@ -1423,12 +1496,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>21</v>
       </c>
@@ -1465,7 +1538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -1475,25 +1548,25 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" customWidth="1"/>
-    <col min="3" max="3" width="45.88671875" customWidth="1"/>
-    <col min="4" max="4" width="22.6640625" customWidth="1"/>
-    <col min="5" max="6" width="19.6640625" customWidth="1"/>
-    <col min="7" max="7" width="25.6640625" customWidth="1"/>
-    <col min="9" max="9" width="13.77734375" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
+    <col min="3" max="3" width="45.85546875" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" customWidth="1"/>
+    <col min="5" max="6" width="19.7109375" customWidth="1"/>
+    <col min="7" max="7" width="25.7109375" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -1522,17 +1595,17 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B2">
         <f>Table1[[#This Row],[Initialising]]+Table13[[#This Row],[Initialising]]+Table134[[#This Row],[Initialising]]+Table1345[[#This Row],[Initialising]]</f>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C2">
         <f>Table1[[#This Row],[Discover and understand the details of the problem]]+Table13[[#This Row],[Discover and understand the details of the problem]]+Table134[[#This Row],[Discover and understand the details of the problem]]+Table1345[[#This Row],[Discover and understand the details of the problem]]</f>
-        <v>1</v>
+        <v>3.5</v>
       </c>
       <c r="D2">
         <f>Table1[[#This Row],[Create the project plan.]]+Table13[[#This Row],[Create the project plan.]]+Table134[[#This Row],[Create the project plan.]]+Table1345[[#This Row],[Create the project plan.]]</f>
@@ -1556,10 +1629,10 @@
       </c>
       <c r="I2">
         <f>SUM(B2:H2)</f>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+        <v>19.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -1569,7 +1642,7 @@
       </c>
       <c r="C3">
         <f>Table1[[#This Row],[Discover and understand the details of the problem]]+Table13[[#This Row],[Discover and understand the details of the problem]]+Table134[[#This Row],[Discover and understand the details of the problem]]+Table1345[[#This Row],[Discover and understand the details of the problem]]</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D3">
         <f>Table1[[#This Row],[Create the project plan.]]+Table13[[#This Row],[Create the project plan.]]+Table134[[#This Row],[Create the project plan.]]+Table1345[[#This Row],[Create the project plan.]]</f>
@@ -1577,11 +1650,11 @@
       </c>
       <c r="E3">
         <f>Table1[[#This Row],[Design Components]]+Table13[[#This Row],[Design Components]]+Table134[[#This Row],[Design Components]]+Table1345[[#This Row],[Design Components]]</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F3">
         <f>Table1[[#This Row],[Implement and Test]]+Table13[[#This Row],[Implement and Test]]+Table134[[#This Row],[Implement and Test]]+Table1345[[#This Row],[Implement and Test]]</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G3">
         <f>Table1[[#This Row],[Monitoring and Controlling]]+Table13[[#This Row],[Monitoring and Controlling]]+Table134[[#This Row],[Monitoring and Controlling]]+Table1345[[#This Row],[Monitoring and Controlling]]</f>
@@ -1593,10 +1666,10 @@
       </c>
       <c r="I3">
         <f t="shared" ref="I3:I13" si="0">SUM(B3:H3)</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -1610,7 +1683,7 @@
       </c>
       <c r="D4">
         <f>Table1[[#This Row],[Create the project plan.]]+Table13[[#This Row],[Create the project plan.]]+Table134[[#This Row],[Create the project plan.]]+Table1345[[#This Row],[Create the project plan.]]</f>
-        <v>3</v>
+        <v>12.5</v>
       </c>
       <c r="E4">
         <f>Table1[[#This Row],[Design Components]]+Table13[[#This Row],[Design Components]]+Table134[[#This Row],[Design Components]]+Table1345[[#This Row],[Design Components]]</f>
@@ -1630,16 +1703,16 @@
       </c>
       <c r="I4">
         <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+        <v>16.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B5">
         <f>Table1[[#This Row],[Initialising]]+Table13[[#This Row],[Initialising]]+Table134[[#This Row],[Initialising]]+Table1345[[#This Row],[Initialising]]</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="C5">
         <f>Table1[[#This Row],[Discover and understand the details of the problem]]+Table13[[#This Row],[Discover and understand the details of the problem]]+Table134[[#This Row],[Discover and understand the details of the problem]]+Table1345[[#This Row],[Discover and understand the details of the problem]]</f>
@@ -1647,7 +1720,7 @@
       </c>
       <c r="D5">
         <f>Table1[[#This Row],[Create the project plan.]]+Table13[[#This Row],[Create the project plan.]]+Table134[[#This Row],[Create the project plan.]]+Table1345[[#This Row],[Create the project plan.]]</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E5">
         <f>Table1[[#This Row],[Design Components]]+Table13[[#This Row],[Design Components]]+Table134[[#This Row],[Design Components]]+Table1345[[#This Row],[Design Components]]</f>
@@ -1667,16 +1740,16 @@
       </c>
       <c r="I5">
         <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+        <v>18.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B6">
         <f>Table1[[#This Row],[Initialising]]+Table13[[#This Row],[Initialising]]+Table134[[#This Row],[Initialising]]+Table1345[[#This Row],[Initialising]]</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C6">
         <f>Table1[[#This Row],[Discover and understand the details of the problem]]+Table13[[#This Row],[Discover and understand the details of the problem]]+Table134[[#This Row],[Discover and understand the details of the problem]]+Table1345[[#This Row],[Discover and understand the details of the problem]]</f>
@@ -1704,20 +1777,20 @@
       </c>
       <c r="I6">
         <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B7">
         <f>Table1[[#This Row],[Initialising]]+Table13[[#This Row],[Initialising]]+Table134[[#This Row],[Initialising]]+Table1345[[#This Row],[Initialising]]</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="C7">
         <f>Table1[[#This Row],[Discover and understand the details of the problem]]+Table13[[#This Row],[Discover and understand the details of the problem]]+Table134[[#This Row],[Discover and understand the details of the problem]]+Table1345[[#This Row],[Discover and understand the details of the problem]]</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D7">
         <f>Table1[[#This Row],[Create the project plan.]]+Table13[[#This Row],[Create the project plan.]]+Table134[[#This Row],[Create the project plan.]]+Table1345[[#This Row],[Create the project plan.]]</f>
@@ -1741,10 +1814,10 @@
       </c>
       <c r="I7">
         <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -1754,7 +1827,7 @@
       </c>
       <c r="C8">
         <f>Table1[[#This Row],[Discover and understand the details of the problem]]+Table13[[#This Row],[Discover and understand the details of the problem]]+Table134[[#This Row],[Discover and understand the details of the problem]]+Table1345[[#This Row],[Discover and understand the details of the problem]]</f>
-        <v>2</v>
+        <v>3.5</v>
       </c>
       <c r="D8">
         <f>Table1[[#This Row],[Create the project plan.]]+Table13[[#This Row],[Create the project plan.]]+Table134[[#This Row],[Create the project plan.]]+Table1345[[#This Row],[Create the project plan.]]</f>
@@ -1762,15 +1835,15 @@
       </c>
       <c r="E8">
         <f>Table1[[#This Row],[Design Components]]+Table13[[#This Row],[Design Components]]+Table134[[#This Row],[Design Components]]+Table1345[[#This Row],[Design Components]]</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F8">
         <f>Table1[[#This Row],[Implement and Test]]+Table13[[#This Row],[Implement and Test]]+Table134[[#This Row],[Implement and Test]]+Table1345[[#This Row],[Implement and Test]]</f>
-        <v>7.5</v>
+        <v>10.5</v>
       </c>
       <c r="G8">
         <f>Table1[[#This Row],[Monitoring and Controlling]]+Table13[[#This Row],[Monitoring and Controlling]]+Table134[[#This Row],[Monitoring and Controlling]]+Table1345[[#This Row],[Monitoring and Controlling]]</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H8">
         <f>Table1[[#This Row],[Deploy]]+Table13[[#This Row],[Deploy]]+Table134[[#This Row],[Deploy]]+Table1345[[#This Row],[Deploy]]</f>
@@ -1778,10 +1851,10 @@
       </c>
       <c r="I8">
         <f t="shared" si="0"/>
-        <v>10.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -1791,7 +1864,7 @@
       </c>
       <c r="C9">
         <f>Table1[[#This Row],[Discover and understand the details of the problem]]+Table13[[#This Row],[Discover and understand the details of the problem]]+Table134[[#This Row],[Discover and understand the details of the problem]]+Table1345[[#This Row],[Discover and understand the details of the problem]]</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D9">
         <f>Table1[[#This Row],[Create the project plan.]]+Table13[[#This Row],[Create the project plan.]]+Table134[[#This Row],[Create the project plan.]]+Table1345[[#This Row],[Create the project plan.]]</f>
@@ -1799,11 +1872,11 @@
       </c>
       <c r="E9">
         <f>Table1[[#This Row],[Design Components]]+Table13[[#This Row],[Design Components]]+Table134[[#This Row],[Design Components]]+Table1345[[#This Row],[Design Components]]</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F9">
         <f>Table1[[#This Row],[Implement and Test]]+Table13[[#This Row],[Implement and Test]]+Table134[[#This Row],[Implement and Test]]+Table1345[[#This Row],[Implement and Test]]</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G9">
         <f>Table1[[#This Row],[Monitoring and Controlling]]+Table13[[#This Row],[Monitoring and Controlling]]+Table134[[#This Row],[Monitoring and Controlling]]+Table1345[[#This Row],[Monitoring and Controlling]]</f>
@@ -1815,10 +1888,10 @@
       </c>
       <c r="I9">
         <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
@@ -1836,11 +1909,11 @@
       </c>
       <c r="E10">
         <f>Table1[[#This Row],[Design Components]]+Table13[[#This Row],[Design Components]]+Table134[[#This Row],[Design Components]]+Table1345[[#This Row],[Design Components]]</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F10">
         <f>Table1[[#This Row],[Implement and Test]]+Table13[[#This Row],[Implement and Test]]+Table134[[#This Row],[Implement and Test]]+Table1345[[#This Row],[Implement and Test]]</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G10">
         <f>Table1[[#This Row],[Monitoring and Controlling]]+Table13[[#This Row],[Monitoring and Controlling]]+Table134[[#This Row],[Monitoring and Controlling]]+Table1345[[#This Row],[Monitoring and Controlling]]</f>
@@ -1852,10 +1925,10 @@
       </c>
       <c r="I10">
         <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
@@ -1873,11 +1946,11 @@
       </c>
       <c r="E11">
         <f>Table1[[#This Row],[Design Components]]+Table13[[#This Row],[Design Components]]+Table134[[#This Row],[Design Components]]+Table1345[[#This Row],[Design Components]]</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F11">
         <f>Table1[[#This Row],[Implement and Test]]+Table13[[#This Row],[Implement and Test]]+Table134[[#This Row],[Implement and Test]]+Table1345[[#This Row],[Implement and Test]]</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G11">
         <f>Table1[[#This Row],[Monitoring and Controlling]]+Table13[[#This Row],[Monitoring and Controlling]]+Table134[[#This Row],[Monitoring and Controlling]]+Table1345[[#This Row],[Monitoring and Controlling]]</f>
@@ -1889,10 +1962,10 @@
       </c>
       <c r="I11">
         <f t="shared" si="0"/>
-        <v>8.5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+        <v>14.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
@@ -1910,11 +1983,11 @@
       </c>
       <c r="E12">
         <f>Table1[[#This Row],[Design Components]]+Table13[[#This Row],[Design Components]]+Table134[[#This Row],[Design Components]]+Table1345[[#This Row],[Design Components]]</f>
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="F12">
         <f>Table1[[#This Row],[Implement and Test]]+Table13[[#This Row],[Implement and Test]]+Table134[[#This Row],[Implement and Test]]+Table1345[[#This Row],[Implement and Test]]</f>
-        <v>8</v>
+        <v>8.5</v>
       </c>
       <c r="G12">
         <f>Table1[[#This Row],[Monitoring and Controlling]]+Table13[[#This Row],[Monitoring and Controlling]]+Table134[[#This Row],[Monitoring and Controlling]]+Table1345[[#This Row],[Monitoring and Controlling]]</f>
@@ -1926,10 +1999,10 @@
       </c>
       <c r="I12">
         <f t="shared" si="0"/>
-        <v>8.5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
@@ -1966,7 +2039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
@@ -1999,33 +2072,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B15" s="1">
         <f t="shared" ref="B15:H15" si="1">SUM(B2:B14)</f>
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="C15" s="1">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="D15" s="1">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>27.5</v>
       </c>
       <c r="E15" s="1">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>30.5</v>
       </c>
       <c r="F15" s="1">
         <f t="shared" si="1"/>
-        <v>65.5</v>
+        <v>75</v>
       </c>
       <c r="G15" s="1">
         <f t="shared" si="1"/>
-        <v>2.5</v>
+        <v>3.5</v>
       </c>
       <c r="H15" s="1">
         <f t="shared" si="1"/>
@@ -2033,10 +2106,10 @@
       </c>
       <c r="I15" s="1">
         <f>SUM(I2:I14)</f>
-        <v>106.5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+        <v>178</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
updated personal cost summary
</commit_message>
<xml_diff>
--- a/Report/Costings summary.xlsx
+++ b/Report/Costings summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CSC3600\Report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan2\Documents\GitHub\CSC3600\Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{5E4DC56D-9765-4B01-871B-1B1DEA424785}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B005A59B-0683-4419-A1A0-406BAB2ED5D6}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9390" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9390" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Greg" sheetId="2" r:id="rId1"/>
@@ -19,10 +19,15 @@
     <sheet name="Isaac" sheetId="8" r:id="rId4"/>
     <sheet name="Total Hrs" sheetId="10" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="179017" concurrentCalc="0"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -858,8 +863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -906,108 +911,168 @@
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>0.5</v>
+      </c>
       <c r="I2">
         <f>SUM(B2:H2)</f>
-        <v>0</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
       <c r="I3">
         <f t="shared" ref="I3:I13" si="0">SUM(B3:H3)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="D4">
+        <v>1.5</v>
+      </c>
       <c r="I4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
       <c r="I5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
       <c r="I6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="B7">
+        <v>0.5</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
       <c r="I7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="E8">
+        <v>11</v>
+      </c>
       <c r="I8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="E9">
+        <v>5</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
       <c r="I9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="E10">
+        <v>3</v>
+      </c>
+      <c r="F10">
+        <v>2.5</v>
+      </c>
       <c r="I10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="F11">
+        <v>8</v>
+      </c>
       <c r="I11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="F12">
+        <v>4.5</v>
+      </c>
+      <c r="G12">
+        <v>0.5</v>
+      </c>
       <c r="I12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="E13">
+        <v>2.5</v>
+      </c>
+      <c r="F13">
+        <v>3</v>
+      </c>
+      <c r="G13">
+        <v>2.5</v>
+      </c>
       <c r="I13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1021,27 +1086,27 @@
       </c>
       <c r="B15" s="1">
         <f t="shared" ref="B15:H15" si="1">SUM(B2:B14)</f>
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="C15" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="D15" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>8.5</v>
       </c>
       <c r="E15" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>22.5</v>
       </c>
       <c r="F15" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G15" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H15" s="1">
         <f t="shared" si="1"/>
@@ -1049,7 +1114,7 @@
       </c>
       <c r="I15" s="1">
         <f>SUM(I2:I14)</f>
-        <v>0</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -1065,7 +1130,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
@@ -1601,11 +1666,11 @@
       </c>
       <c r="B2">
         <f>Table1[[#This Row],[Initialising]]+Table13[[#This Row],[Initialising]]+Table134[[#This Row],[Initialising]]+Table1345[[#This Row],[Initialising]]</f>
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C2">
         <f>Table1[[#This Row],[Discover and understand the details of the problem]]+Table13[[#This Row],[Discover and understand the details of the problem]]+Table134[[#This Row],[Discover and understand the details of the problem]]+Table1345[[#This Row],[Discover and understand the details of the problem]]</f>
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="D2">
         <f>Table1[[#This Row],[Create the project plan.]]+Table13[[#This Row],[Create the project plan.]]+Table134[[#This Row],[Create the project plan.]]+Table1345[[#This Row],[Create the project plan.]]</f>
@@ -1629,7 +1694,7 @@
       </c>
       <c r="I2">
         <f>SUM(B2:H2)</f>
-        <v>19.5</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1638,11 +1703,11 @@
       </c>
       <c r="B3">
         <f>Table1[[#This Row],[Initialising]]+Table13[[#This Row],[Initialising]]+Table134[[#This Row],[Initialising]]+Table1345[[#This Row],[Initialising]]</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C3">
         <f>Table1[[#This Row],[Discover and understand the details of the problem]]+Table13[[#This Row],[Discover and understand the details of the problem]]+Table134[[#This Row],[Discover and understand the details of the problem]]+Table1345[[#This Row],[Discover and understand the details of the problem]]</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D3">
         <f>Table1[[#This Row],[Create the project plan.]]+Table13[[#This Row],[Create the project plan.]]+Table134[[#This Row],[Create the project plan.]]+Table1345[[#This Row],[Create the project plan.]]</f>
@@ -1666,7 +1731,7 @@
       </c>
       <c r="I3">
         <f t="shared" ref="I3:I13" si="0">SUM(B3:H3)</f>
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1683,7 +1748,7 @@
       </c>
       <c r="D4">
         <f>Table1[[#This Row],[Create the project plan.]]+Table13[[#This Row],[Create the project plan.]]+Table134[[#This Row],[Create the project plan.]]+Table1345[[#This Row],[Create the project plan.]]</f>
-        <v>12.5</v>
+        <v>14</v>
       </c>
       <c r="E4">
         <f>Table1[[#This Row],[Design Components]]+Table13[[#This Row],[Design Components]]+Table134[[#This Row],[Design Components]]+Table1345[[#This Row],[Design Components]]</f>
@@ -1703,7 +1768,7 @@
       </c>
       <c r="I4">
         <f t="shared" si="0"/>
-        <v>16.5</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1720,7 +1785,7 @@
       </c>
       <c r="D5">
         <f>Table1[[#This Row],[Create the project plan.]]+Table13[[#This Row],[Create the project plan.]]+Table134[[#This Row],[Create the project plan.]]+Table1345[[#This Row],[Create the project plan.]]</f>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E5">
         <f>Table1[[#This Row],[Design Components]]+Table13[[#This Row],[Design Components]]+Table134[[#This Row],[Design Components]]+Table1345[[#This Row],[Design Components]]</f>
@@ -1740,7 +1805,7 @@
       </c>
       <c r="I5">
         <f t="shared" si="0"/>
-        <v>18.5</v>
+        <v>22.5</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1757,7 +1822,7 @@
       </c>
       <c r="D6">
         <f>Table1[[#This Row],[Create the project plan.]]+Table13[[#This Row],[Create the project plan.]]+Table134[[#This Row],[Create the project plan.]]+Table1345[[#This Row],[Create the project plan.]]</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E6">
         <f>Table1[[#This Row],[Design Components]]+Table13[[#This Row],[Design Components]]+Table134[[#This Row],[Design Components]]+Table1345[[#This Row],[Design Components]]</f>
@@ -1777,7 +1842,7 @@
       </c>
       <c r="I6">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1786,7 +1851,7 @@
       </c>
       <c r="B7">
         <f>Table1[[#This Row],[Initialising]]+Table13[[#This Row],[Initialising]]+Table134[[#This Row],[Initialising]]+Table1345[[#This Row],[Initialising]]</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C7">
         <f>Table1[[#This Row],[Discover and understand the details of the problem]]+Table13[[#This Row],[Discover and understand the details of the problem]]+Table134[[#This Row],[Discover and understand the details of the problem]]+Table1345[[#This Row],[Discover and understand the details of the problem]]</f>
@@ -1798,7 +1863,7 @@
       </c>
       <c r="E7">
         <f>Table1[[#This Row],[Design Components]]+Table13[[#This Row],[Design Components]]+Table134[[#This Row],[Design Components]]+Table1345[[#This Row],[Design Components]]</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F7">
         <f>Table1[[#This Row],[Implement and Test]]+Table13[[#This Row],[Implement and Test]]+Table134[[#This Row],[Implement and Test]]+Table1345[[#This Row],[Implement and Test]]</f>
@@ -1814,7 +1879,7 @@
       </c>
       <c r="I7">
         <f t="shared" si="0"/>
-        <v>12.5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1835,7 +1900,7 @@
       </c>
       <c r="E8">
         <f>Table1[[#This Row],[Design Components]]+Table13[[#This Row],[Design Components]]+Table134[[#This Row],[Design Components]]+Table1345[[#This Row],[Design Components]]</f>
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="F8">
         <f>Table1[[#This Row],[Implement and Test]]+Table13[[#This Row],[Implement and Test]]+Table134[[#This Row],[Implement and Test]]+Table1345[[#This Row],[Implement and Test]]</f>
@@ -1851,7 +1916,7 @@
       </c>
       <c r="I8">
         <f t="shared" si="0"/>
-        <v>23</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -1872,11 +1937,11 @@
       </c>
       <c r="E9">
         <f>Table1[[#This Row],[Design Components]]+Table13[[#This Row],[Design Components]]+Table134[[#This Row],[Design Components]]+Table1345[[#This Row],[Design Components]]</f>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="F9">
         <f>Table1[[#This Row],[Implement and Test]]+Table13[[#This Row],[Implement and Test]]+Table134[[#This Row],[Implement and Test]]+Table1345[[#This Row],[Implement and Test]]</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G9">
         <f>Table1[[#This Row],[Monitoring and Controlling]]+Table13[[#This Row],[Monitoring and Controlling]]+Table134[[#This Row],[Monitoring and Controlling]]+Table1345[[#This Row],[Monitoring and Controlling]]</f>
@@ -1888,7 +1953,7 @@
       </c>
       <c r="I9">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -1909,11 +1974,11 @@
       </c>
       <c r="E10">
         <f>Table1[[#This Row],[Design Components]]+Table13[[#This Row],[Design Components]]+Table134[[#This Row],[Design Components]]+Table1345[[#This Row],[Design Components]]</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F10">
         <f>Table1[[#This Row],[Implement and Test]]+Table13[[#This Row],[Implement and Test]]+Table134[[#This Row],[Implement and Test]]+Table1345[[#This Row],[Implement and Test]]</f>
-        <v>8</v>
+        <v>10.5</v>
       </c>
       <c r="G10">
         <f>Table1[[#This Row],[Monitoring and Controlling]]+Table13[[#This Row],[Monitoring and Controlling]]+Table134[[#This Row],[Monitoring and Controlling]]+Table1345[[#This Row],[Monitoring and Controlling]]</f>
@@ -1925,7 +1990,7 @@
       </c>
       <c r="I10">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>20.5</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -1950,7 +2015,7 @@
       </c>
       <c r="F11">
         <f>Table1[[#This Row],[Implement and Test]]+Table13[[#This Row],[Implement and Test]]+Table134[[#This Row],[Implement and Test]]+Table1345[[#This Row],[Implement and Test]]</f>
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="G11">
         <f>Table1[[#This Row],[Monitoring and Controlling]]+Table13[[#This Row],[Monitoring and Controlling]]+Table134[[#This Row],[Monitoring and Controlling]]+Table1345[[#This Row],[Monitoring and Controlling]]</f>
@@ -1962,7 +2027,7 @@
       </c>
       <c r="I11">
         <f t="shared" si="0"/>
-        <v>14.5</v>
+        <v>22.5</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1987,11 +2052,11 @@
       </c>
       <c r="F12">
         <f>Table1[[#This Row],[Implement and Test]]+Table13[[#This Row],[Implement and Test]]+Table134[[#This Row],[Implement and Test]]+Table1345[[#This Row],[Implement and Test]]</f>
-        <v>8.5</v>
+        <v>13</v>
       </c>
       <c r="G12">
         <f>Table1[[#This Row],[Monitoring and Controlling]]+Table13[[#This Row],[Monitoring and Controlling]]+Table134[[#This Row],[Monitoring and Controlling]]+Table1345[[#This Row],[Monitoring and Controlling]]</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H12">
         <f>Table1[[#This Row],[Deploy]]+Table13[[#This Row],[Deploy]]+Table134[[#This Row],[Deploy]]+Table1345[[#This Row],[Deploy]]</f>
@@ -1999,7 +2064,7 @@
       </c>
       <c r="I12">
         <f t="shared" si="0"/>
-        <v>12.5</v>
+        <v>17.5</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -2020,15 +2085,15 @@
       </c>
       <c r="E13">
         <f>Table1[[#This Row],[Design Components]]+Table13[[#This Row],[Design Components]]+Table134[[#This Row],[Design Components]]+Table1345[[#This Row],[Design Components]]</f>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="F13">
         <f>Table1[[#This Row],[Implement and Test]]+Table13[[#This Row],[Implement and Test]]+Table134[[#This Row],[Implement and Test]]+Table1345[[#This Row],[Implement and Test]]</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G13">
         <f>Table1[[#This Row],[Monitoring and Controlling]]+Table13[[#This Row],[Monitoring and Controlling]]+Table134[[#This Row],[Monitoring and Controlling]]+Table1345[[#This Row],[Monitoring and Controlling]]</f>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="H13">
         <f>Table1[[#This Row],[Deploy]]+Table13[[#This Row],[Deploy]]+Table134[[#This Row],[Deploy]]+Table1345[[#This Row],[Deploy]]</f>
@@ -2036,7 +2101,7 @@
       </c>
       <c r="I13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2078,27 +2143,27 @@
       </c>
       <c r="B15" s="1">
         <f t="shared" ref="B15:H15" si="1">SUM(B2:B14)</f>
-        <v>19</v>
+        <v>23.5</v>
       </c>
       <c r="C15" s="1">
         <f t="shared" si="1"/>
-        <v>22</v>
+        <v>24.5</v>
       </c>
       <c r="D15" s="1">
         <f t="shared" si="1"/>
-        <v>27.5</v>
+        <v>36</v>
       </c>
       <c r="E15" s="1">
         <f t="shared" si="1"/>
-        <v>30.5</v>
+        <v>53</v>
       </c>
       <c r="F15" s="1">
         <f t="shared" si="1"/>
-        <v>75</v>
+        <v>95</v>
       </c>
       <c r="G15" s="1">
         <f t="shared" si="1"/>
-        <v>3.5</v>
+        <v>6.5</v>
       </c>
       <c r="H15" s="1">
         <f t="shared" si="1"/>
@@ -2106,7 +2171,7 @@
       </c>
       <c r="I15" s="1">
         <f>SUM(I2:I14)</f>
-        <v>178</v>
+        <v>239</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
added Costings to report
</commit_message>
<xml_diff>
--- a/Report/Costings summary.xlsx
+++ b/Report/Costings summary.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zac\Documents\GitHub\CSC3600\Report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jocelyn\Documents\GitHub\CSC3600\Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53C76BA2-F9DD-4029-B131-8AD4173BF69D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9390" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9396" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Greg" sheetId="2" r:id="rId1"/>
@@ -18,8 +17,10 @@
     <sheet name="Andrew" sheetId="6" r:id="rId3"/>
     <sheet name="Isaac" sheetId="8" r:id="rId4"/>
     <sheet name="Total Hrs" sheetId="10" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="11" r:id="rId6"/>
+    <sheet name="Sheet2" sheetId="12" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="41">
   <si>
     <t>Initialising</t>
   </si>
@@ -99,12 +100,158 @@
   <si>
     <t>Column1</t>
   </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <r>
+      <t>Hours</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(4)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Cost (Business Analyst Rate</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(1)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Cost (Programmer Rate</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(2)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Cost (Project Manager Rate</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(3)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>Total Phase Cost</t>
+  </si>
+  <si>
+    <t>Totals</t>
+  </si>
+  <si>
+    <t>Notes:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1.   Business Analyst Hourly Rate-$48.65 (PayScale 2018).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   2.   Programmer Hourly Rate-$35(PayScale 2018).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   3.   Project Manager Hourly Rate-$80.93(PayScale 2018).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   4.   Phase hours sourced from WBS, refer Table 1.</t>
+  </si>
+  <si>
+    <t>Week Number</t>
+  </si>
+  <si>
+    <t>Build all the program components, integrate and test.</t>
+  </si>
+  <si>
+    <t>PM Hours</t>
+  </si>
+  <si>
+    <t>BA/ Programmer Hours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   4.   Phase hours sourced from Task Log Summary, refer Appendix XX.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -128,8 +275,32 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <vertAlign val="superscript"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -141,8 +312,20 @@
         <fgColor rgb="FFA5A5A5"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF94B6D2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE9F0F6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -165,15 +348,246 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF94B6D2"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF94B6D2"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF94B6D2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF94B6D2"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF94B6D2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF94B6D2"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF94B6D2"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF94B6D2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFBED3E4"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFBED3E4"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFBED3E4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFBED3E4"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFBED3E4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFBED3E4"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFBED3E4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFBED3E4"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFBED3E4"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFBED3E4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFBED3E4"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FFBED3E4"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFBED3E4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFBED3E4"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFBED3E4"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFBED3E4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFBED3E4"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FFBED3E4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FFBED3E4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFBED3E4"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFBED3E4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="8" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="8" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
@@ -218,91 +632,1169 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="3.3333333333333333E-2"/>
+          <c:y val="0.17273148148148151"/>
+          <c:w val="0.93888888888888888"/>
+          <c:h val="0.71523950131233593"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Actual</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="38100" cap="flat" cmpd="dbl" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$L$2:$L$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Initialising</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Discover and understand the details of the problem</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Create the project plan.</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Design Components</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Build all the program components, integrate and test.</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Monitoring and Controlling</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Deploy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$C$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>26.75</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>31.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>103.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>17.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Planned</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="38100" cap="flat" cmpd="dbl" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$L$2:$L$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Initialising</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Discover and understand the details of the problem</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Create the project plan.</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Design Components</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Build all the program components, integrate and test.</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Monitoring and Controlling</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Deploy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$M$2:$M$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>37</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="231922368"/>
+        <c:axId val="231925504"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="231922368"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="32000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="3175" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+            <a:tailEnd type="none" w="med" len="lg"/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="231925504"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="0"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="231925504"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="32000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="3175" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+            <a:tailEnd type="none" w="med" len="lg"/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="231922368"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="237">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="3175" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+        <a:tailEnd type="none" w="med" len="lg"/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="38100" cap="flat" cmpd="dbl" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:alpha val="32000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+            <a:alpha val="32000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="3175" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+        <a:tailEnd type="none" w="med" len="lg"/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1800" b="1" kern="1200" cap="all" spc="150" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="rnd"/>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="3175" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+        <a:tailEnd type="none" w="med" len="lg"/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>518160</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>388620</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:I15" totalsRowShown="0">
-  <autoFilter ref="A1:I15" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:I15" totalsRowShown="0">
+  <autoFilter ref="A1:I15"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Column1" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Initialising"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Discover and understand the details of the problem"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Create the project plan."/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Design Components"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Implement and Test"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Monitoring and Controlling"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Deploy"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Weekly Total"/>
+    <tableColumn id="1" name="Column1" dataDxfId="4"/>
+    <tableColumn id="2" name="Initialising"/>
+    <tableColumn id="3" name="Discover and understand the details of the problem"/>
+    <tableColumn id="4" name="Create the project plan."/>
+    <tableColumn id="5" name="Design Components"/>
+    <tableColumn id="6" name="Implement and Test"/>
+    <tableColumn id="7" name="Monitoring and Controlling"/>
+    <tableColumn id="8" name="Deploy"/>
+    <tableColumn id="9" name="Weekly Total"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table13" displayName="Table13" ref="A1:I15" totalsRowShown="0">
-  <autoFilter ref="A1:I15" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A1:I15" totalsRowShown="0">
+  <autoFilter ref="A1:I15"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Column1" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Initialising"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Discover and understand the details of the problem"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Create the project plan."/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Design Components"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Implement and Test"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Monitoring and Controlling"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Deploy"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Weekly Total"/>
+    <tableColumn id="1" name="Column1" dataDxfId="3"/>
+    <tableColumn id="2" name="Initialising"/>
+    <tableColumn id="3" name="Discover and understand the details of the problem"/>
+    <tableColumn id="4" name="Create the project plan."/>
+    <tableColumn id="5" name="Design Components"/>
+    <tableColumn id="6" name="Implement and Test"/>
+    <tableColumn id="7" name="Monitoring and Controlling"/>
+    <tableColumn id="8" name="Deploy"/>
+    <tableColumn id="9" name="Weekly Total"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table134" displayName="Table134" ref="A1:I15" totalsRowShown="0">
-  <autoFilter ref="A1:I15" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table134" displayName="Table134" ref="A1:I15" totalsRowShown="0">
+  <autoFilter ref="A1:I15"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Column1" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Initialising"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Discover and understand the details of the problem"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Create the project plan."/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Design Components"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Implement and Test"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Monitoring and Controlling"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Deploy"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="Weekly Total"/>
+    <tableColumn id="1" name="Column1" dataDxfId="2"/>
+    <tableColumn id="2" name="Initialising"/>
+    <tableColumn id="3" name="Discover and understand the details of the problem"/>
+    <tableColumn id="4" name="Create the project plan."/>
+    <tableColumn id="5" name="Design Components"/>
+    <tableColumn id="6" name="Implement and Test"/>
+    <tableColumn id="7" name="Monitoring and Controlling"/>
+    <tableColumn id="8" name="Deploy"/>
+    <tableColumn id="9" name="Weekly Total"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table1345" displayName="Table1345" ref="A1:I15" totalsRowShown="0">
-  <autoFilter ref="A1:I15" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table1345" displayName="Table1345" ref="A1:I15" totalsRowShown="0">
+  <autoFilter ref="A1:I15"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Column1" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Initialising"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Discover and understand the details of the problem"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Create the project plan."/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Design Components"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Implement and Test"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="Monitoring and Controlling"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="Deploy"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0300-000009000000}" name="Weekly Total"/>
+    <tableColumn id="1" name="Column1" dataDxfId="1"/>
+    <tableColumn id="2" name="Initialising"/>
+    <tableColumn id="3" name="Discover and understand the details of the problem"/>
+    <tableColumn id="4" name="Create the project plan."/>
+    <tableColumn id="5" name="Design Components"/>
+    <tableColumn id="6" name="Implement and Test"/>
+    <tableColumn id="7" name="Monitoring and Controlling"/>
+    <tableColumn id="8" name="Deploy"/>
+    <tableColumn id="9" name="Weekly Total"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table13456" displayName="Table13456" ref="A1:I15" totalsRowShown="0">
-  <autoFilter ref="A1:I15" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table13456" displayName="Table13456" ref="A1:I15" totalsRowShown="0">
+  <autoFilter ref="A1:I15"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Column1" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Initialising"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Discover and understand the details of the problem"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Create the project plan."/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="Design Components"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0400-000006000000}" name="Implement and Test"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0400-000007000000}" name="Monitoring and Controlling"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0400-000008000000}" name="Deploy"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0400-000009000000}" name="Weekly Total"/>
+    <tableColumn id="1" name="Week Number" dataDxfId="0"/>
+    <tableColumn id="2" name="Initialising"/>
+    <tableColumn id="3" name="Discover and understand the details of the problem"/>
+    <tableColumn id="4" name="Create the project plan."/>
+    <tableColumn id="5" name="Design Components"/>
+    <tableColumn id="6" name="Implement and Test"/>
+    <tableColumn id="7" name="Monitoring and Controlling"/>
+    <tableColumn id="8" name="Deploy"/>
+    <tableColumn id="9" name="Weekly Total"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -570,26 +2062,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.44140625" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="50" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="21.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -618,25 +2110,25 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B2">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I2">
         <f>SUM(B2:H2)</f>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -654,7 +2146,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -672,7 +2164,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
@@ -684,7 +2176,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
@@ -696,7 +2188,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -714,7 +2206,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -732,7 +2224,7 @@
         <v>10.5</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -747,7 +2239,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
@@ -765,7 +2257,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
@@ -780,7 +2272,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
@@ -795,27 +2287,30 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="H13">
+        <v>2</v>
+      </c>
       <c r="I13">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B15" s="1">
         <f t="shared" ref="B15:H15" si="1">SUM(B2:B14)</f>
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C15" s="1">
         <f t="shared" si="1"/>
@@ -823,7 +2318,7 @@
       </c>
       <c r="D15" s="1">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E15" s="1">
         <f t="shared" si="1"/>
@@ -839,14 +2334,14 @@
       </c>
       <c r="H15" s="1">
         <f t="shared" si="1"/>
-        <v>0.5</v>
+        <v>2.5</v>
       </c>
       <c r="I15" s="1">
         <f>SUM(I2:I14)</f>
-        <v>106.5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+        <v>103.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -856,25 +2351,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" customWidth="1"/>
-    <col min="3" max="3" width="45.85546875" customWidth="1"/>
-    <col min="4" max="4" width="22.7109375" customWidth="1"/>
-    <col min="5" max="6" width="19.7109375" customWidth="1"/>
-    <col min="7" max="7" width="25.7109375" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" customWidth="1"/>
+    <col min="1" max="1" width="11.44140625" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" customWidth="1"/>
+    <col min="3" max="3" width="45.88671875" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" customWidth="1"/>
+    <col min="5" max="6" width="19.6640625" customWidth="1"/>
+    <col min="7" max="7" width="25.6640625" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -903,7 +2398,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -918,7 +2413,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -933,7 +2428,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -945,7 +2440,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
@@ -957,7 +2452,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
@@ -969,7 +2464,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -984,7 +2479,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -996,7 +2491,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -1011,7 +2506,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
@@ -1026,7 +2521,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
@@ -1038,7 +2533,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
@@ -1053,7 +2548,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
@@ -1071,12 +2566,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>21</v>
       </c>
@@ -1113,7 +2608,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -1123,25 +2618,25 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" customWidth="1"/>
-    <col min="3" max="3" width="45.85546875" customWidth="1"/>
-    <col min="4" max="4" width="22.7109375" customWidth="1"/>
-    <col min="5" max="6" width="19.7109375" customWidth="1"/>
-    <col min="7" max="7" width="25.7109375" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" customWidth="1"/>
+    <col min="1" max="1" width="11.44140625" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" customWidth="1"/>
+    <col min="3" max="3" width="45.88671875" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" customWidth="1"/>
+    <col min="5" max="6" width="19.6640625" customWidth="1"/>
+    <col min="7" max="7" width="25.6640625" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -1170,7 +2665,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1185,7 +2680,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -1203,7 +2698,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -1215,7 +2710,7 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
@@ -1230,7 +2725,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
@@ -1242,7 +2737,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -1257,7 +2752,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -1278,7 +2773,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -1296,7 +2791,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
@@ -1311,7 +2806,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
@@ -1326,7 +2821,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
@@ -1341,7 +2836,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
@@ -1350,12 +2845,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>21</v>
       </c>
@@ -1392,7 +2887,7 @@
         <v>71.5</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -1402,26 +2897,26 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:I16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.44140625" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="50" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="21.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -1450,7 +2945,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1465,7 +2960,7 @@
         <v>2.25</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -1480,7 +2975,7 @@
         <v>1.75</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -1498,7 +2993,7 @@
         <v>3.25</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
@@ -1516,7 +3011,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
@@ -1534,7 +3029,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -1552,7 +3047,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -1570,7 +3065,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -1591,7 +3086,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
@@ -1612,7 +3107,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
@@ -1633,7 +3128,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
@@ -1654,7 +3149,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
@@ -1675,12 +3170,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>21</v>
       </c>
@@ -1717,7 +3212,88 @@
         <v>57.25</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B22">
+        <v>6.25</v>
+      </c>
+      <c r="C22">
+        <v>7</v>
+      </c>
+      <c r="D22">
+        <v>7.5</v>
+      </c>
+      <c r="E22">
+        <v>17</v>
+      </c>
+      <c r="F22">
+        <v>8.5</v>
+      </c>
+      <c r="G22">
+        <v>11</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B24">
+        <v>6.25</v>
+      </c>
+      <c r="C24">
+        <v>7</v>
+      </c>
+      <c r="D24">
+        <v>7.5</v>
+      </c>
+      <c r="E24">
+        <v>17</v>
+      </c>
+      <c r="F24">
+        <v>8.5</v>
+      </c>
+      <c r="G24">
+        <v>11</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B26">
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B27">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B28">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B29">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B30">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B31">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B32">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -1727,27 +3303,27 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:I16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" customWidth="1"/>
-    <col min="3" max="3" width="45.85546875" customWidth="1"/>
-    <col min="4" max="4" width="22.7109375" customWidth="1"/>
-    <col min="5" max="6" width="19.7109375" customWidth="1"/>
-    <col min="7" max="7" width="25.7109375" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" customWidth="1"/>
+    <col min="1" max="1" width="11.44140625" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" customWidth="1"/>
+    <col min="3" max="3" width="45.88671875" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" customWidth="1"/>
+    <col min="5" max="6" width="19.6640625" customWidth="1"/>
+    <col min="7" max="7" width="25.6640625" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1774,13 +3350,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B2">
         <f>Table1[[#This Row],[Initialising]]+Table13[[#This Row],[Initialising]]+Table134[[#This Row],[Initialising]]+Table1345[[#This Row],[Initialising]]</f>
-        <v>15.25</v>
+        <v>12.25</v>
       </c>
       <c r="C2">
         <f>Table1[[#This Row],[Discover and understand the details of the problem]]+Table13[[#This Row],[Discover and understand the details of the problem]]+Table134[[#This Row],[Discover and understand the details of the problem]]+Table1345[[#This Row],[Discover and understand the details of the problem]]</f>
@@ -1788,7 +3364,7 @@
       </c>
       <c r="D2">
         <f>Table1[[#This Row],[Create the project plan.]]+Table13[[#This Row],[Create the project plan.]]+Table134[[#This Row],[Create the project plan.]]+Table1345[[#This Row],[Create the project plan.]]</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E2">
         <f>Table1[[#This Row],[Design Components]]+Table13[[#This Row],[Design Components]]+Table134[[#This Row],[Design Components]]+Table1345[[#This Row],[Design Components]]</f>
@@ -1808,10 +3384,10 @@
       </c>
       <c r="I2">
         <f>SUM(B2:H2)</f>
-        <v>25.25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>20.25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -1848,7 +3424,7 @@
         <v>22.75</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -1885,7 +3461,7 @@
         <v>21.25</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
@@ -1922,7 +3498,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
@@ -1959,7 +3535,7 @@
         <v>20.5</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -1996,7 +3572,7 @@
         <v>17.5</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -2033,7 +3609,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -2070,7 +3646,7 @@
         <v>25.5</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
@@ -2107,7 +3683,7 @@
         <v>29.5</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
@@ -2144,7 +3720,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
@@ -2181,7 +3757,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
@@ -2211,14 +3787,14 @@
       </c>
       <c r="H13">
         <f>Table1[[#This Row],[Deploy]]+Table13[[#This Row],[Deploy]]+Table134[[#This Row],[Deploy]]+Table1345[[#This Row],[Deploy]]</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I13">
         <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
@@ -2251,13 +3827,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B15" s="1">
         <f t="shared" ref="B15:H15" si="1">SUM(B2:B14)</f>
-        <v>29.75</v>
+        <v>26.75</v>
       </c>
       <c r="C15" s="1">
         <f t="shared" si="1"/>
@@ -2265,7 +3841,7 @@
       </c>
       <c r="D15" s="1">
         <f t="shared" si="1"/>
-        <v>43.5</v>
+        <v>41.5</v>
       </c>
       <c r="E15" s="1">
         <f t="shared" si="1"/>
@@ -2281,18 +3857,763 @@
       </c>
       <c r="H15" s="1">
         <f t="shared" si="1"/>
-        <v>0.5</v>
+        <v>2.5</v>
       </c>
       <c r="I15" s="1">
         <f>SUM(I2:I14)</f>
-        <v>296.25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+        <v>293.25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B17">
+        <v>15</v>
+      </c>
+      <c r="C17">
+        <v>20</v>
+      </c>
+      <c r="D17">
+        <v>32</v>
+      </c>
+      <c r="E17">
+        <v>12</v>
+      </c>
+      <c r="F17" s="15">
+        <v>201</v>
+      </c>
+      <c r="G17">
+        <v>60</v>
+      </c>
+      <c r="H17">
+        <v>37</v>
+      </c>
+      <c r="I17">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="15"/>
+      <c r="B21" s="15"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3.77734375" customWidth="1"/>
+    <col min="2" max="2" width="22.44140625" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" customWidth="1"/>
+    <col min="6" max="6" width="14.77734375" customWidth="1"/>
+    <col min="7" max="7" width="17.5546875" customWidth="1"/>
+    <col min="9" max="9" width="13.77734375" customWidth="1"/>
+    <col min="12" max="12" width="32.77734375" customWidth="1"/>
+    <col min="14" max="14" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="6">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="7">
+        <f>'Total Hrs'!B15</f>
+        <v>26.75</v>
+      </c>
+      <c r="D2" s="10">
+        <f>I2*D16</f>
+        <v>997.32499999999993</v>
+      </c>
+      <c r="E2" s="10">
+        <v>0</v>
+      </c>
+      <c r="F2" s="10">
+        <f>H2*F$16</f>
+        <v>505.81250000000006</v>
+      </c>
+      <c r="G2" s="10">
+        <v>3403.2</v>
+      </c>
+      <c r="H2">
+        <f>Isaac!B15</f>
+        <v>6.25</v>
+      </c>
+      <c r="I2">
+        <f>C2-H2</f>
+        <v>20.5</v>
+      </c>
+      <c r="K2" s="6">
+        <v>1</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="M2" s="7">
+        <v>15</v>
+      </c>
+      <c r="N2" s="10">
+        <v>2189.25</v>
+      </c>
+      <c r="O2" s="10">
+        <v>0</v>
+      </c>
+      <c r="P2" s="10">
+        <v>1213.95</v>
+      </c>
+      <c r="Q2" s="10">
+        <v>3403.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="11">
+        <v>2</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="12">
+        <f>'Total Hrs'!C15</f>
+        <v>31.5</v>
+      </c>
+      <c r="D3" s="14">
+        <f>I3*D16</f>
+        <v>1191.925</v>
+      </c>
+      <c r="E3" s="14">
+        <v>0</v>
+      </c>
+      <c r="F3" s="14">
+        <f t="shared" ref="F3:F8" si="0">H3*F$16</f>
+        <v>566.51</v>
+      </c>
+      <c r="G3" s="14">
+        <v>4537.6000000000004</v>
+      </c>
+      <c r="H3">
+        <f>Isaac!C15</f>
+        <v>7</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I8" si="1">C3-H3</f>
+        <v>24.5</v>
+      </c>
+      <c r="K3" s="11">
+        <v>2</v>
+      </c>
+      <c r="L3" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="M3" s="12">
+        <v>20</v>
+      </c>
+      <c r="N3" s="14">
+        <v>2919</v>
+      </c>
+      <c r="O3" s="14">
+        <v>0</v>
+      </c>
+      <c r="P3" s="14">
+        <v>1618.6</v>
+      </c>
+      <c r="Q3" s="14">
+        <v>4537.6000000000004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="6">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="7">
+        <f>'Total Hrs'!D15</f>
+        <v>41.5</v>
+      </c>
+      <c r="D4" s="10">
+        <f>I4*D16</f>
+        <v>1654.1</v>
+      </c>
+      <c r="E4" s="10">
+        <v>0</v>
+      </c>
+      <c r="F4" s="10">
+        <f t="shared" si="0"/>
+        <v>606.97500000000002</v>
+      </c>
+      <c r="G4" s="10">
+        <v>7260.16</v>
+      </c>
+      <c r="H4">
+        <f>Isaac!D15</f>
+        <v>7.5</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="K4" s="6">
+        <v>3</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="M4" s="7">
+        <v>32</v>
+      </c>
+      <c r="N4" s="10">
+        <v>4670.3999999999996</v>
+      </c>
+      <c r="O4" s="10">
+        <v>0</v>
+      </c>
+      <c r="P4" s="10">
+        <v>2589.7600000000002</v>
+      </c>
+      <c r="Q4" s="10">
+        <v>7260.16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="11">
+        <v>4</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="12">
+        <v>70</v>
+      </c>
+      <c r="D5" s="14">
+        <v>0</v>
+      </c>
+      <c r="E5" s="14">
+        <f>I5*E16</f>
+        <v>1855</v>
+      </c>
+      <c r="F5" s="14">
+        <f t="shared" si="0"/>
+        <v>1375.8100000000002</v>
+      </c>
+      <c r="G5" s="14">
+        <v>1680</v>
+      </c>
+      <c r="H5">
+        <f>Isaac!E15</f>
+        <v>17</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="1"/>
+        <v>53</v>
+      </c>
+      <c r="K5" s="11">
+        <v>4</v>
+      </c>
+      <c r="L5" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="M5" s="12">
+        <v>12</v>
+      </c>
+      <c r="N5" s="14">
+        <v>0</v>
+      </c>
+      <c r="O5" s="14">
+        <v>1680</v>
+      </c>
+      <c r="P5" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="14">
+        <v>1680</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="7">
+        <f>'Total Hrs'!F15</f>
+        <v>103.5</v>
+      </c>
+      <c r="D6" s="10">
+        <v>0</v>
+      </c>
+      <c r="E6" s="10">
+        <f>I6*E16</f>
+        <v>3325</v>
+      </c>
+      <c r="F6" s="10">
+        <f t="shared" si="0"/>
+        <v>687.90500000000009</v>
+      </c>
+      <c r="G6" s="10">
+        <v>25200</v>
+      </c>
+      <c r="H6">
+        <f>Isaac!F15</f>
+        <v>8.5</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="1"/>
+        <v>95</v>
+      </c>
+      <c r="K6" s="6">
+        <v>5</v>
+      </c>
+      <c r="L6" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="M6" s="7">
+        <v>240</v>
+      </c>
+      <c r="N6" s="10">
+        <v>0</v>
+      </c>
+      <c r="O6" s="10">
+        <v>25200</v>
+      </c>
+      <c r="P6" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="10">
+        <v>25200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="11">
+        <v>6</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="12">
+        <f>'Total Hrs'!G15</f>
+        <v>17.5</v>
+      </c>
+      <c r="D7" s="14">
+        <f>I7*D16</f>
+        <v>316.22499999999997</v>
+      </c>
+      <c r="E7" s="14">
+        <v>0</v>
+      </c>
+      <c r="F7" s="14">
+        <f t="shared" si="0"/>
+        <v>890.23</v>
+      </c>
+      <c r="G7" s="14">
+        <v>4764.4799999999996</v>
+      </c>
+      <c r="H7">
+        <f>Isaac!G15</f>
+        <v>11</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="1"/>
+        <v>6.5</v>
+      </c>
+      <c r="K7" s="11">
+        <v>6</v>
+      </c>
+      <c r="L7" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="M7" s="12">
+        <v>21</v>
+      </c>
+      <c r="N7" s="14">
+        <v>3064.95</v>
+      </c>
+      <c r="O7" s="14">
+        <v>0</v>
+      </c>
+      <c r="P7" s="14">
+        <v>1699.53</v>
+      </c>
+      <c r="Q7" s="14">
+        <v>4764.4799999999996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="6">
+        <v>7</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="7">
+        <f>'Total Hrs'!H15</f>
+        <v>2.5</v>
+      </c>
+      <c r="D8" s="10">
+        <f>I8*D16</f>
+        <v>121.625</v>
+      </c>
+      <c r="E8" s="10">
+        <v>0</v>
+      </c>
+      <c r="F8" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G8" s="10">
+        <v>8394.56</v>
+      </c>
+      <c r="H8">
+        <f>Isaac!H15</f>
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="1"/>
+        <v>2.5</v>
+      </c>
+      <c r="K8" s="6">
+        <v>7</v>
+      </c>
+      <c r="L8" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="M8" s="7">
+        <v>37</v>
+      </c>
+      <c r="N8" s="10">
+        <v>5400.15</v>
+      </c>
+      <c r="O8" s="10">
+        <v>0</v>
+      </c>
+      <c r="P8" s="10">
+        <v>2994.41</v>
+      </c>
+      <c r="Q8" s="10">
+        <v>8394.56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="20"/>
+      <c r="C9" s="13">
+        <f>SUM(C2:C8)</f>
+        <v>293.25</v>
+      </c>
+      <c r="D9" s="16">
+        <f>SUM(D2:D8)</f>
+        <v>4281.2</v>
+      </c>
+      <c r="E9" s="16">
+        <f>SUM(E2:E8)</f>
+        <v>5180</v>
+      </c>
+      <c r="F9" s="16">
+        <f>SUM(F2:F8)</f>
+        <v>4633.2425000000003</v>
+      </c>
+      <c r="G9" s="16">
+        <f>SUM(D9:F9)</f>
+        <v>14094.442500000001</v>
+      </c>
+      <c r="K9" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="L9" s="20"/>
+      <c r="M9" s="13">
+        <v>377</v>
+      </c>
+      <c r="N9" s="16">
+        <v>18243.75</v>
+      </c>
+      <c r="O9" s="16">
+        <v>38556</v>
+      </c>
+      <c r="P9" s="16">
+        <v>10116.25</v>
+      </c>
+      <c r="Q9" s="16">
+        <v>66916</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="23"/>
+      <c r="H10">
+        <v>3400</v>
+      </c>
+      <c r="I10" s="9">
+        <f>G9+H10</f>
+        <v>17494.442500000001</v>
+      </c>
+      <c r="K10" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="L10" s="22"/>
+      <c r="M10" s="22"/>
+      <c r="N10" s="22"/>
+      <c r="O10" s="22"/>
+      <c r="P10" s="22"/>
+      <c r="Q10" s="23"/>
+    </row>
+    <row r="11" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="26"/>
+      <c r="I11" s="9">
+        <f>O22-I10</f>
+        <v>2634.557499999999</v>
+      </c>
+      <c r="K11" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="L11" s="25"/>
+      <c r="M11" s="25"/>
+      <c r="N11" s="25"/>
+      <c r="O11" s="25"/>
+      <c r="P11" s="25"/>
+      <c r="Q11" s="26"/>
+    </row>
+    <row r="12" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="25"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="26"/>
+      <c r="K12" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="L12" s="25"/>
+      <c r="M12" s="25"/>
+      <c r="N12" s="25"/>
+      <c r="O12" s="25"/>
+      <c r="P12" s="25"/>
+      <c r="Q12" s="26"/>
+    </row>
+    <row r="13" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="25"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="26"/>
+      <c r="K13" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="L13" s="25"/>
+      <c r="M13" s="25"/>
+      <c r="N13" s="25"/>
+      <c r="O13" s="25"/>
+      <c r="P13" s="25"/>
+      <c r="Q13" s="26"/>
+    </row>
+    <row r="14" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="28"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="29"/>
+      <c r="K14" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="L14" s="28"/>
+      <c r="M14" s="28"/>
+      <c r="N14" s="28"/>
+      <c r="O14" s="28"/>
+      <c r="P14" s="28"/>
+      <c r="Q14" s="29"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="D16">
+        <v>48.65</v>
+      </c>
+      <c r="E16">
+        <v>35</v>
+      </c>
+      <c r="F16">
+        <v>80.930000000000007</v>
+      </c>
+      <c r="M16">
+        <f>SUM(M2:M8)</f>
+        <v>377</v>
+      </c>
+    </row>
+    <row r="17" spans="7:15" x14ac:dyDescent="0.3">
+      <c r="M17">
+        <f>M9-M16</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="7:15" x14ac:dyDescent="0.3">
+      <c r="N19" s="9">
+        <f>3400+G9</f>
+        <v>17494.442500000001</v>
+      </c>
+    </row>
+    <row r="20" spans="7:15" x14ac:dyDescent="0.3">
+      <c r="G20" s="9"/>
+      <c r="O20" s="9">
+        <f>Q9/4</f>
+        <v>16729</v>
+      </c>
+    </row>
+    <row r="21" spans="7:15" x14ac:dyDescent="0.3">
+      <c r="O21" s="18">
+        <v>3400</v>
+      </c>
+    </row>
+    <row r="22" spans="7:15" x14ac:dyDescent="0.3">
+      <c r="O22" s="9">
+        <f>SUM(O20:O21)</f>
+        <v>20129</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="K14:Q14"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:G10"/>
+    <mergeCell ref="A11:G11"/>
+    <mergeCell ref="A12:G12"/>
+    <mergeCell ref="A13:G13"/>
+    <mergeCell ref="A14:G14"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="K10:Q10"/>
+    <mergeCell ref="K11:Q11"/>
+    <mergeCell ref="K12:Q12"/>
+    <mergeCell ref="K13:Q13"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="K2:M2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="11:13" x14ac:dyDescent="0.3">
+      <c r="K2">
+        <f>103/240</f>
+        <v>0.42916666666666664</v>
+      </c>
+      <c r="L2">
+        <f>70/12*100</f>
+        <v>583.33333333333326</v>
+      </c>
+      <c r="M2">
+        <f>6*12</f>
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated my final costing summary
</commit_message>
<xml_diff>
--- a/Report/Costings summary.xlsx
+++ b/Report/Costings summary.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jocelyn\Documents\GitHub\CSC3600\Report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Documents\GitHub\CSC3600\Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD292E91-130C-4E3C-AAB0-49AF13D82B55}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9396" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9390" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Greg" sheetId="2" r:id="rId1"/>
@@ -20,7 +21,7 @@
     <sheet name="Sheet1" sheetId="11" r:id="rId6"/>
     <sheet name="Sheet2" sheetId="12" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -247,9 +248,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -531,8 +532,8 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="8" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -544,17 +545,26 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="8" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="4" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -577,15 +587,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -633,7 +634,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -719,7 +720,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -785,18 +785,23 @@
                   <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>103.5</c:v>
+                  <c:v>111.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>17.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.5</c:v>
+                  <c:v>5.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-ACD9-4971-BA0D-4B8446FB8B5C}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -855,7 +860,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -933,6 +937,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-ACD9-4971-BA0D-4B8446FB8B5C}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -987,7 +996,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -1692,7 +1701,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1711,90 +1726,90 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:I15" totalsRowShown="0">
-  <autoFilter ref="A1:I15"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:I15" totalsRowShown="0">
+  <autoFilter ref="A1:I15" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="Column1" dataDxfId="4"/>
-    <tableColumn id="2" name="Initialising"/>
-    <tableColumn id="3" name="Discover and understand the details of the problem"/>
-    <tableColumn id="4" name="Create the project plan."/>
-    <tableColumn id="5" name="Design Components"/>
-    <tableColumn id="6" name="Implement and Test"/>
-    <tableColumn id="7" name="Monitoring and Controlling"/>
-    <tableColumn id="8" name="Deploy"/>
-    <tableColumn id="9" name="Weekly Total"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Column1" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Initialising"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Discover and understand the details of the problem"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Create the project plan."/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Design Components"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Implement and Test"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Monitoring and Controlling"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Deploy"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Weekly Total"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A1:I15" totalsRowShown="0">
-  <autoFilter ref="A1:I15"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table13" displayName="Table13" ref="A1:I15" totalsRowShown="0">
+  <autoFilter ref="A1:I15" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="Column1" dataDxfId="3"/>
-    <tableColumn id="2" name="Initialising"/>
-    <tableColumn id="3" name="Discover and understand the details of the problem"/>
-    <tableColumn id="4" name="Create the project plan."/>
-    <tableColumn id="5" name="Design Components"/>
-    <tableColumn id="6" name="Implement and Test"/>
-    <tableColumn id="7" name="Monitoring and Controlling"/>
-    <tableColumn id="8" name="Deploy"/>
-    <tableColumn id="9" name="Weekly Total"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Column1" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Initialising"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Discover and understand the details of the problem"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Create the project plan."/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Design Components"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Implement and Test"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Monitoring and Controlling"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Deploy"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Weekly Total"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table134" displayName="Table134" ref="A1:I15" totalsRowShown="0">
-  <autoFilter ref="A1:I15"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table134" displayName="Table134" ref="A1:I15" totalsRowShown="0">
+  <autoFilter ref="A1:I15" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="Column1" dataDxfId="2"/>
-    <tableColumn id="2" name="Initialising"/>
-    <tableColumn id="3" name="Discover and understand the details of the problem"/>
-    <tableColumn id="4" name="Create the project plan."/>
-    <tableColumn id="5" name="Design Components"/>
-    <tableColumn id="6" name="Implement and Test"/>
-    <tableColumn id="7" name="Monitoring and Controlling"/>
-    <tableColumn id="8" name="Deploy"/>
-    <tableColumn id="9" name="Weekly Total"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Column1" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Initialising"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Discover and understand the details of the problem"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Create the project plan."/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Design Components"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Implement and Test"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Monitoring and Controlling"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Deploy"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="Weekly Total"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table1345" displayName="Table1345" ref="A1:I15" totalsRowShown="0">
-  <autoFilter ref="A1:I15"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table1345" displayName="Table1345" ref="A1:I15" totalsRowShown="0">
+  <autoFilter ref="A1:I15" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="Column1" dataDxfId="1"/>
-    <tableColumn id="2" name="Initialising"/>
-    <tableColumn id="3" name="Discover and understand the details of the problem"/>
-    <tableColumn id="4" name="Create the project plan."/>
-    <tableColumn id="5" name="Design Components"/>
-    <tableColumn id="6" name="Implement and Test"/>
-    <tableColumn id="7" name="Monitoring and Controlling"/>
-    <tableColumn id="8" name="Deploy"/>
-    <tableColumn id="9" name="Weekly Total"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Column1" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Initialising"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Discover and understand the details of the problem"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Create the project plan."/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Design Components"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Implement and Test"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="Monitoring and Controlling"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="Deploy"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0300-000009000000}" name="Weekly Total"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table13456" displayName="Table13456" ref="A1:I15" totalsRowShown="0">
-  <autoFilter ref="A1:I15"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table13456" displayName="Table13456" ref="A1:I15" totalsRowShown="0">
+  <autoFilter ref="A1:I15" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="Week Number" dataDxfId="0"/>
-    <tableColumn id="2" name="Initialising"/>
-    <tableColumn id="3" name="Discover and understand the details of the problem"/>
-    <tableColumn id="4" name="Create the project plan."/>
-    <tableColumn id="5" name="Design Components"/>
-    <tableColumn id="6" name="Implement and Test"/>
-    <tableColumn id="7" name="Monitoring and Controlling"/>
-    <tableColumn id="8" name="Deploy"/>
-    <tableColumn id="9" name="Weekly Total"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Week Number" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Initialising"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Discover and understand the details of the problem"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Create the project plan."/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="Design Components"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0400-000006000000}" name="Implement and Test"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0400-000007000000}" name="Monitoring and Controlling"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0400-000008000000}" name="Deploy"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0400-000009000000}" name="Weekly Total"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2062,26 +2077,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView topLeftCell="C10" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" customWidth="1"/>
-    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="50" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -2110,7 +2125,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -2128,7 +2143,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -2146,7 +2161,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -2164,7 +2179,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
@@ -2176,7 +2191,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
@@ -2188,7 +2203,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -2206,7 +2221,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -2224,7 +2239,7 @@
         <v>10.5</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -2239,7 +2254,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
@@ -2257,7 +2272,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
@@ -2272,7 +2287,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
@@ -2287,24 +2302,27 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H13">
-        <v>2</v>
+      <c r="F13">
+        <v>8</v>
       </c>
       <c r="I13">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>21</v>
       </c>
@@ -2326,7 +2344,7 @@
       </c>
       <c r="F15" s="1">
         <f t="shared" si="1"/>
-        <v>65.5</v>
+        <v>73.5</v>
       </c>
       <c r="G15" s="1">
         <f t="shared" si="1"/>
@@ -2334,14 +2352,14 @@
       </c>
       <c r="H15" s="1">
         <f t="shared" si="1"/>
-        <v>2.5</v>
+        <v>5.5</v>
       </c>
       <c r="I15" s="1">
         <f>SUM(I2:I14)</f>
-        <v>103.5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+        <v>109.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -2351,25 +2369,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" customWidth="1"/>
-    <col min="3" max="3" width="45.88671875" customWidth="1"/>
-    <col min="4" max="4" width="22.6640625" customWidth="1"/>
-    <col min="5" max="6" width="19.6640625" customWidth="1"/>
-    <col min="7" max="7" width="25.6640625" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
+    <col min="3" max="3" width="45.85546875" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" customWidth="1"/>
+    <col min="5" max="6" width="19.7109375" customWidth="1"/>
+    <col min="7" max="7" width="25.7109375" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -2398,7 +2416,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -2413,7 +2431,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -2428,7 +2446,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -2440,7 +2458,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
@@ -2452,7 +2470,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
@@ -2464,7 +2482,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -2479,7 +2497,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -2491,7 +2509,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -2506,7 +2524,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
@@ -2521,7 +2539,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
@@ -2533,7 +2551,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
@@ -2548,7 +2566,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
@@ -2566,12 +2584,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>21</v>
       </c>
@@ -2608,7 +2626,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -2618,25 +2636,25 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" customWidth="1"/>
-    <col min="3" max="3" width="45.88671875" customWidth="1"/>
-    <col min="4" max="4" width="22.6640625" customWidth="1"/>
-    <col min="5" max="6" width="19.6640625" customWidth="1"/>
-    <col min="7" max="7" width="25.6640625" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
+    <col min="3" max="3" width="45.85546875" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" customWidth="1"/>
+    <col min="5" max="6" width="19.7109375" customWidth="1"/>
+    <col min="7" max="7" width="25.7109375" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -2665,7 +2683,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -2680,7 +2698,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -2698,7 +2716,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -2710,7 +2728,7 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
@@ -2725,7 +2743,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
@@ -2737,7 +2755,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -2752,7 +2770,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -2773,7 +2791,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -2791,7 +2809,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
@@ -2806,7 +2824,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
@@ -2821,7 +2839,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
@@ -2836,7 +2854,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
@@ -2845,12 +2863,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>21</v>
       </c>
@@ -2887,7 +2905,7 @@
         <v>71.5</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -2897,26 +2915,26 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" customWidth="1"/>
-    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="50" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -2945,7 +2963,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -2960,7 +2978,7 @@
         <v>2.25</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -2975,7 +2993,7 @@
         <v>1.75</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -2993,7 +3011,7 @@
         <v>3.25</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
@@ -3011,7 +3029,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
@@ -3029,7 +3047,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -3047,7 +3065,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -3065,7 +3083,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -3086,7 +3104,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
@@ -3107,7 +3125,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
@@ -3128,7 +3146,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
@@ -3149,7 +3167,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
@@ -3170,12 +3188,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>21</v>
       </c>
@@ -3212,8 +3230,8 @@
         <v>57.25</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>6.25</v>
       </c>
@@ -3236,7 +3254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>6.25</v>
       </c>
@@ -3259,37 +3277,37 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>6.25</v>
       </c>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>7.5</v>
       </c>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>8.5</v>
       </c>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31">
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B32">
         <v>0</v>
       </c>
@@ -3303,25 +3321,25 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" customWidth="1"/>
-    <col min="3" max="3" width="45.88671875" customWidth="1"/>
-    <col min="4" max="4" width="22.6640625" customWidth="1"/>
-    <col min="5" max="6" width="19.6640625" customWidth="1"/>
-    <col min="7" max="7" width="25.6640625" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
+    <col min="3" max="3" width="45.85546875" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" customWidth="1"/>
+    <col min="5" max="6" width="19.7109375" customWidth="1"/>
+    <col min="7" max="7" width="25.7109375" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>36</v>
       </c>
@@ -3350,7 +3368,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -3387,7 +3405,7 @@
         <v>20.25</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -3424,7 +3442,7 @@
         <v>22.75</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -3461,7 +3479,7 @@
         <v>21.25</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
@@ -3498,7 +3516,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
@@ -3535,7 +3553,7 @@
         <v>20.5</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -3572,7 +3590,7 @@
         <v>17.5</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -3609,7 +3627,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -3646,7 +3664,7 @@
         <v>25.5</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
@@ -3683,7 +3701,7 @@
         <v>29.5</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
@@ -3720,7 +3738,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
@@ -3757,7 +3775,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
@@ -3779,7 +3797,7 @@
       </c>
       <c r="F13">
         <f>Table1[[#This Row],[Implement and Test]]+Table13[[#This Row],[Implement and Test]]+Table134[[#This Row],[Implement and Test]]+Table1345[[#This Row],[Implement and Test]]</f>
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="G13">
         <f>Table1[[#This Row],[Monitoring and Controlling]]+Table13[[#This Row],[Monitoring and Controlling]]+Table134[[#This Row],[Monitoring and Controlling]]+Table1345[[#This Row],[Monitoring and Controlling]]</f>
@@ -3787,14 +3805,14 @@
       </c>
       <c r="H13">
         <f>Table1[[#This Row],[Deploy]]+Table13[[#This Row],[Deploy]]+Table134[[#This Row],[Deploy]]+Table1345[[#This Row],[Deploy]]</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I13">
         <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
@@ -3824,10 +3842,10 @@
       </c>
       <c r="H14">
         <f>Table1[[#This Row],[Deploy]]+Table13[[#This Row],[Deploy]]+Table134[[#This Row],[Deploy]]+Table1345[[#This Row],[Deploy]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>21</v>
       </c>
@@ -3849,7 +3867,7 @@
       </c>
       <c r="F15" s="1">
         <f t="shared" si="1"/>
-        <v>103.5</v>
+        <v>111.5</v>
       </c>
       <c r="G15" s="1">
         <f t="shared" si="1"/>
@@ -3857,15 +3875,15 @@
       </c>
       <c r="H15" s="1">
         <f t="shared" si="1"/>
-        <v>2.5</v>
+        <v>5.5</v>
       </c>
       <c r="I15" s="1">
         <f>SUM(I2:I14)</f>
-        <v>293.25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+        <v>299.25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>15</v>
       </c>
@@ -3891,7 +3909,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="15"/>
       <c r="B21" s="15"/>
     </row>
@@ -3905,30 +3923,30 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:Q22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.77734375" customWidth="1"/>
-    <col min="2" max="2" width="22.44140625" customWidth="1"/>
-    <col min="4" max="4" width="18.6640625" customWidth="1"/>
-    <col min="5" max="5" width="13.5546875" customWidth="1"/>
-    <col min="6" max="6" width="14.77734375" customWidth="1"/>
-    <col min="7" max="7" width="17.5546875" customWidth="1"/>
-    <col min="9" max="9" width="13.77734375" customWidth="1"/>
-    <col min="12" max="12" width="32.77734375" customWidth="1"/>
-    <col min="14" max="14" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" customWidth="1"/>
+    <col min="7" max="7" width="17.5703125" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" customWidth="1"/>
+    <col min="12" max="12" width="32.7109375" customWidth="1"/>
+    <col min="14" max="14" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
@@ -3978,7 +3996,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -4033,7 +4051,7 @@
         <v>3403.2</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="11">
         <v>2</v>
       </c>
@@ -4088,7 +4106,7 @@
         <v>4537.6000000000004</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -4143,7 +4161,7 @@
         <v>7260.16</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="11">
         <v>4</v>
       </c>
@@ -4197,7 +4215,7 @@
         <v>1680</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <v>5</v>
       </c>
@@ -4206,14 +4224,14 @@
       </c>
       <c r="C6" s="7">
         <f>'Total Hrs'!F15</f>
-        <v>103.5</v>
+        <v>111.5</v>
       </c>
       <c r="D6" s="10">
         <v>0</v>
       </c>
       <c r="E6" s="10">
         <f>I6*E16</f>
-        <v>3325</v>
+        <v>3605</v>
       </c>
       <c r="F6" s="10">
         <f t="shared" si="0"/>
@@ -4228,7 +4246,7 @@
       </c>
       <c r="I6">
         <f t="shared" si="1"/>
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="K6" s="6">
         <v>5</v>
@@ -4252,7 +4270,7 @@
         <v>25200</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="11">
         <v>6</v>
       </c>
@@ -4307,7 +4325,7 @@
         <v>4764.4799999999996</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <v>7</v>
       </c>
@@ -4316,11 +4334,11 @@
       </c>
       <c r="C8" s="7">
         <f>'Total Hrs'!H15</f>
-        <v>2.5</v>
+        <v>5.5</v>
       </c>
       <c r="D8" s="10">
         <f>I8*D16</f>
-        <v>121.625</v>
+        <v>267.57499999999999</v>
       </c>
       <c r="E8" s="10">
         <v>0</v>
@@ -4338,7 +4356,7 @@
       </c>
       <c r="I8">
         <f t="shared" si="1"/>
-        <v>2.5</v>
+        <v>5.5</v>
       </c>
       <c r="K8" s="6">
         <v>7</v>
@@ -4362,22 +4380,22 @@
         <v>8394.56</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="19" t="s">
+    <row r="9" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="20"/>
+      <c r="B9" s="23"/>
       <c r="C9" s="13">
         <f>SUM(C2:C8)</f>
-        <v>293.25</v>
+        <v>304.25</v>
       </c>
       <c r="D9" s="16">
         <f>SUM(D2:D8)</f>
-        <v>4281.2</v>
+        <v>4427.1499999999996</v>
       </c>
       <c r="E9" s="16">
         <f>SUM(E2:E8)</f>
-        <v>5180</v>
+        <v>5460</v>
       </c>
       <c r="F9" s="16">
         <f>SUM(F2:F8)</f>
@@ -4385,12 +4403,12 @@
       </c>
       <c r="G9" s="16">
         <f>SUM(D9:F9)</f>
-        <v>14094.442500000001</v>
-      </c>
-      <c r="K9" s="19" t="s">
+        <v>14520.3925</v>
+      </c>
+      <c r="K9" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="L9" s="20"/>
+      <c r="L9" s="23"/>
       <c r="M9" s="13">
         <v>377</v>
       </c>
@@ -4407,124 +4425,124 @@
         <v>66916</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="21" t="s">
+    <row r="10" spans="1:17" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="22"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="23"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="26"/>
       <c r="H10">
         <v>3400</v>
       </c>
       <c r="I10" s="9">
         <f>G9+H10</f>
-        <v>17494.442500000001</v>
-      </c>
-      <c r="K10" s="21" t="s">
+        <v>17920.392500000002</v>
+      </c>
+      <c r="K10" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="L10" s="22"/>
-      <c r="M10" s="22"/>
-      <c r="N10" s="22"/>
-      <c r="O10" s="22"/>
-      <c r="P10" s="22"/>
-      <c r="Q10" s="23"/>
-    </row>
-    <row r="11" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="24" t="s">
+      <c r="L10" s="25"/>
+      <c r="M10" s="25"/>
+      <c r="N10" s="25"/>
+      <c r="O10" s="25"/>
+      <c r="P10" s="25"/>
+      <c r="Q10" s="26"/>
+    </row>
+    <row r="11" spans="1:17" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="25"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="26"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="29"/>
       <c r="I11" s="9">
         <f>O22-I10</f>
-        <v>2634.557499999999</v>
-      </c>
-      <c r="K11" s="24" t="s">
+        <v>2208.6074999999983</v>
+      </c>
+      <c r="K11" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="L11" s="25"/>
-      <c r="M11" s="25"/>
-      <c r="N11" s="25"/>
-      <c r="O11" s="25"/>
-      <c r="P11" s="25"/>
-      <c r="Q11" s="26"/>
-    </row>
-    <row r="12" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="24" t="s">
+      <c r="L11" s="28"/>
+      <c r="M11" s="28"/>
+      <c r="N11" s="28"/>
+      <c r="O11" s="28"/>
+      <c r="P11" s="28"/>
+      <c r="Q11" s="29"/>
+    </row>
+    <row r="12" spans="1:17" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="25"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="26"/>
-      <c r="K12" s="24" t="s">
+      <c r="B12" s="28"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="29"/>
+      <c r="K12" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="L12" s="25"/>
-      <c r="M12" s="25"/>
-      <c r="N12" s="25"/>
-      <c r="O12" s="25"/>
-      <c r="P12" s="25"/>
-      <c r="Q12" s="26"/>
-    </row>
-    <row r="13" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="24" t="s">
+      <c r="L12" s="28"/>
+      <c r="M12" s="28"/>
+      <c r="N12" s="28"/>
+      <c r="O12" s="28"/>
+      <c r="P12" s="28"/>
+      <c r="Q12" s="29"/>
+    </row>
+    <row r="13" spans="1:17" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="25"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="26"/>
-      <c r="K13" s="24" t="s">
+      <c r="B13" s="28"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="29"/>
+      <c r="K13" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="L13" s="25"/>
-      <c r="M13" s="25"/>
-      <c r="N13" s="25"/>
-      <c r="O13" s="25"/>
-      <c r="P13" s="25"/>
-      <c r="Q13" s="26"/>
-    </row>
-    <row r="14" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="27" t="s">
+      <c r="L13" s="28"/>
+      <c r="M13" s="28"/>
+      <c r="N13" s="28"/>
+      <c r="O13" s="28"/>
+      <c r="P13" s="28"/>
+      <c r="Q13" s="29"/>
+    </row>
+    <row r="14" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="28"/>
-      <c r="C14" s="28"/>
-      <c r="D14" s="28"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="29"/>
-      <c r="K14" s="27" t="s">
+      <c r="B14" s="20"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="21"/>
+      <c r="K14" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="L14" s="28"/>
-      <c r="M14" s="28"/>
-      <c r="N14" s="28"/>
-      <c r="O14" s="28"/>
-      <c r="P14" s="28"/>
-      <c r="Q14" s="29"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="L14" s="20"/>
+      <c r="M14" s="20"/>
+      <c r="N14" s="20"/>
+      <c r="O14" s="20"/>
+      <c r="P14" s="20"/>
+      <c r="Q14" s="21"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D15" s="9"/>
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D16">
         <v>48.65</v>
       </c>
@@ -4539,31 +4557,31 @@
         <v>377</v>
       </c>
     </row>
-    <row r="17" spans="7:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="7:15" x14ac:dyDescent="0.25">
       <c r="M17">
         <f>M9-M16</f>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="7:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="7:15" x14ac:dyDescent="0.25">
       <c r="N19" s="9">
         <f>3400+G9</f>
-        <v>17494.442500000001</v>
-      </c>
-    </row>
-    <row r="20" spans="7:15" x14ac:dyDescent="0.3">
+        <v>17920.392500000002</v>
+      </c>
+    </row>
+    <row r="20" spans="7:15" x14ac:dyDescent="0.25">
       <c r="G20" s="9"/>
       <c r="O20" s="9">
         <f>Q9/4</f>
         <v>16729</v>
       </c>
     </row>
-    <row r="21" spans="7:15" x14ac:dyDescent="0.3">
+    <row r="21" spans="7:15" x14ac:dyDescent="0.25">
       <c r="O21" s="18">
         <v>3400</v>
       </c>
     </row>
-    <row r="22" spans="7:15" x14ac:dyDescent="0.3">
+    <row r="22" spans="7:15" x14ac:dyDescent="0.25">
       <c r="O22" s="9">
         <f>SUM(O20:O21)</f>
         <v>20129</v>
@@ -4589,16 +4607,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="K2:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="11:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="11:13" x14ac:dyDescent="0.25">
       <c r="K2">
         <f>103/240</f>
         <v>0.42916666666666664</v>

</xml_diff>

<commit_message>
Updatd costs and processes
</commit_message>
<xml_diff>
--- a/Report/Costings summary.xlsx
+++ b/Report/Costings summary.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Documents\GitHub\CSC3600\Report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jocelyn\Documents\GitHub\CSC3600\Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD292E91-130C-4E3C-AAB0-49AF13D82B55}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9390" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9396" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Greg" sheetId="2" r:id="rId1"/>
@@ -21,7 +20,7 @@
     <sheet name="Sheet1" sheetId="11" r:id="rId6"/>
     <sheet name="Sheet2" sheetId="12" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="42">
   <si>
     <t>Initialising</t>
   </si>
@@ -244,15 +243,18 @@
   <si>
     <t xml:space="preserve">   4.   Phase hours sourced from Task Log Summary, refer Appendix XX.</t>
   </si>
+  <si>
+    <t>Week 14</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -300,6 +302,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -326,7 +336,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -505,12 +515,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF94B6D2"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF94B6D2"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF94B6D2"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF94B6D2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -532,8 +557,8 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="8" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -545,11 +570,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -587,6 +612,11 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="8" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="8" fontId="3" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -634,7 +664,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -718,8 +748,9 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -773,7 +804,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>26.75</c:v>
+                  <c:v>29.25</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>31.5</c:v>
@@ -785,19 +816,19 @@
                   <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>111.5</c:v>
+                  <c:v>114.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>17.5</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.5</c:v>
+                  <c:v>24.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-ACD9-4971-BA0D-4B8446FB8B5C}"/>
             </c:ext>
@@ -858,8 +889,9 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -937,7 +969,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-ACD9-4971-BA0D-4B8446FB8B5C}"/>
             </c:ext>
@@ -952,11 +984,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="231922368"/>
-        <c:axId val="231925504"/>
+        <c:axId val="479364200"/>
+        <c:axId val="479363024"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="231922368"/>
+        <c:axId val="479364200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1015,7 +1047,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="231925504"/>
+        <c:crossAx val="479363024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -1023,7 +1055,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="231925504"/>
+        <c:axId val="479363024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1082,7 +1114,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="231922368"/>
+        <c:crossAx val="479364200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1689,22 +1721,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>518160</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>160020</xdr:rowOff>
+      <xdr:colOff>480060</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>388620</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
+      <xdr:colOff>350520</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0600-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1726,90 +1758,90 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:I15" totalsRowShown="0">
-  <autoFilter ref="A1:I15" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:I16" totalsRowShown="0">
+  <autoFilter ref="A1:I16"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Column1" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Initialising"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Discover and understand the details of the problem"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Create the project plan."/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Design Components"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Implement and Test"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Monitoring and Controlling"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Deploy"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Weekly Total"/>
+    <tableColumn id="1" name="Column1" dataDxfId="0"/>
+    <tableColumn id="2" name="Initialising"/>
+    <tableColumn id="3" name="Discover and understand the details of the problem"/>
+    <tableColumn id="4" name="Create the project plan."/>
+    <tableColumn id="5" name="Design Components"/>
+    <tableColumn id="6" name="Implement and Test"/>
+    <tableColumn id="7" name="Monitoring and Controlling"/>
+    <tableColumn id="8" name="Deploy"/>
+    <tableColumn id="9" name="Weekly Total"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table13" displayName="Table13" ref="A1:I15" totalsRowShown="0">
-  <autoFilter ref="A1:I15" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A1:I16" totalsRowShown="0">
+  <autoFilter ref="A1:I16"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Column1" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Initialising"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Discover and understand the details of the problem"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Create the project plan."/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Design Components"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Implement and Test"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Monitoring and Controlling"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Deploy"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Weekly Total"/>
+    <tableColumn id="1" name="Column1" dataDxfId="4"/>
+    <tableColumn id="2" name="Initialising"/>
+    <tableColumn id="3" name="Discover and understand the details of the problem"/>
+    <tableColumn id="4" name="Create the project plan."/>
+    <tableColumn id="5" name="Design Components"/>
+    <tableColumn id="6" name="Implement and Test"/>
+    <tableColumn id="7" name="Monitoring and Controlling"/>
+    <tableColumn id="8" name="Deploy"/>
+    <tableColumn id="9" name="Weekly Total"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table134" displayName="Table134" ref="A1:I15" totalsRowShown="0">
-  <autoFilter ref="A1:I15" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table134" displayName="Table134" ref="A1:I16" totalsRowShown="0">
+  <autoFilter ref="A1:I16"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Column1" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Initialising"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Discover and understand the details of the problem"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Create the project plan."/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Design Components"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Implement and Test"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Monitoring and Controlling"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Deploy"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="Weekly Total"/>
+    <tableColumn id="1" name="Column1" dataDxfId="3"/>
+    <tableColumn id="2" name="Initialising"/>
+    <tableColumn id="3" name="Discover and understand the details of the problem"/>
+    <tableColumn id="4" name="Create the project plan."/>
+    <tableColumn id="5" name="Design Components"/>
+    <tableColumn id="6" name="Implement and Test"/>
+    <tableColumn id="7" name="Monitoring and Controlling"/>
+    <tableColumn id="8" name="Deploy"/>
+    <tableColumn id="9" name="Weekly Total"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table1345" displayName="Table1345" ref="A1:I15" totalsRowShown="0">
-  <autoFilter ref="A1:I15" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table1345" displayName="Table1345" ref="A1:I16" totalsRowShown="0">
+  <autoFilter ref="A1:I16"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Column1" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Initialising"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Discover and understand the details of the problem"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Create the project plan."/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Design Components"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Implement and Test"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="Monitoring and Controlling"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="Deploy"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0300-000009000000}" name="Weekly Total"/>
+    <tableColumn id="1" name="Column1" dataDxfId="2"/>
+    <tableColumn id="2" name="Initialising"/>
+    <tableColumn id="3" name="Discover and understand the details of the problem"/>
+    <tableColumn id="4" name="Create the project plan."/>
+    <tableColumn id="5" name="Design Components"/>
+    <tableColumn id="6" name="Implement and Test"/>
+    <tableColumn id="7" name="Monitoring and Controlling"/>
+    <tableColumn id="8" name="Deploy"/>
+    <tableColumn id="9" name="Weekly Total"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table13456" displayName="Table13456" ref="A1:I15" totalsRowShown="0">
-  <autoFilter ref="A1:I15" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table13456" displayName="Table13456" ref="A1:I16" totalsRowShown="0">
+  <autoFilter ref="A1:I16"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Week Number" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Initialising"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Discover and understand the details of the problem"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Create the project plan."/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="Design Components"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0400-000006000000}" name="Implement and Test"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0400-000007000000}" name="Monitoring and Controlling"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0400-000008000000}" name="Deploy"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0400-000009000000}" name="Weekly Total"/>
+    <tableColumn id="1" name="Week Number" dataDxfId="1"/>
+    <tableColumn id="2" name="Initialising"/>
+    <tableColumn id="3" name="Discover and understand the details of the problem"/>
+    <tableColumn id="4" name="Create the project plan."/>
+    <tableColumn id="5" name="Design Components"/>
+    <tableColumn id="6" name="Implement and Test"/>
+    <tableColumn id="7" name="Monitoring and Controlling"/>
+    <tableColumn id="8" name="Deploy"/>
+    <tableColumn id="9" name="Weekly Total"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2077,26 +2109,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView topLeftCell="C10" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.44140625" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="50" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="21.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -2125,121 +2158,186 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B2">
-        <v>5</v>
-      </c>
-      <c r="C2">
+        <v>2.5</v>
+      </c>
+      <c r="K2" s="30">
+        <v>43297</v>
+      </c>
+      <c r="L2" s="30">
+        <v>43303</v>
+      </c>
+      <c r="M2">
         <v>1</v>
       </c>
-      <c r="D2">
-        <v>3</v>
-      </c>
-      <c r="I2">
-        <f>SUM(B2:H2)</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
         <v>3</v>
       </c>
-      <c r="C3">
-        <v>3</v>
-      </c>
-      <c r="D3">
-        <v>4</v>
-      </c>
       <c r="I3">
-        <f t="shared" ref="I3:I13" si="0">SUM(B3:H3)</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <f>SUM(B3:H3)</f>
+        <v>9</v>
+      </c>
+      <c r="K3" s="30">
+        <f>K2+7</f>
+        <v>43304</v>
+      </c>
+      <c r="L3" s="30">
+        <f>L2+7</f>
+        <v>43310</v>
+      </c>
+      <c r="M3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
       <c r="D4">
+        <v>4</v>
+      </c>
+      <c r="I4">
+        <f t="shared" ref="I4:I14" si="0">SUM(B4:H4)</f>
+        <v>10</v>
+      </c>
+      <c r="K4" s="30">
+        <f t="shared" ref="K4:K15" si="1">K3+7</f>
+        <v>43311</v>
+      </c>
+      <c r="L4" s="30">
+        <f t="shared" ref="L4:L15" si="2">L3+7</f>
+        <v>43317</v>
+      </c>
+      <c r="M4">
         <v>3</v>
       </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>3</v>
-      </c>
-      <c r="I4">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
       <c r="F5">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="I5">
         <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="K5" s="30">
+        <f t="shared" si="1"/>
+        <v>43318</v>
+      </c>
+      <c r="L5" s="30">
+        <f t="shared" si="2"/>
+        <v>43324</v>
+      </c>
+      <c r="M5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F6">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="I6">
         <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="K6" s="30">
+        <f t="shared" si="1"/>
+        <v>43325</v>
+      </c>
+      <c r="L6" s="30">
+        <f t="shared" si="2"/>
+        <v>43331</v>
+      </c>
+      <c r="M6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C7">
-        <v>3</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
       <c r="F7">
+        <v>10</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="K7" s="30">
+        <f t="shared" si="1"/>
+        <v>43332</v>
+      </c>
+      <c r="L7" s="30">
+        <f t="shared" si="2"/>
+        <v>43338</v>
+      </c>
+      <c r="M7">
         <v>6</v>
       </c>
-      <c r="I7">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C8">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
       </c>
       <c r="F8">
-        <v>7.5</v>
-      </c>
-      <c r="G8">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="I8">
         <f t="shared" si="0"/>
-        <v>10.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="K8" s="30">
+        <f t="shared" si="1"/>
+        <v>43339</v>
+      </c>
+      <c r="L8" s="30">
+        <f t="shared" si="2"/>
+        <v>43345</v>
+      </c>
+      <c r="M8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -2247,14 +2345,28 @@
         <v>2</v>
       </c>
       <c r="F9">
-        <v>5</v>
+        <v>7.5</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
       </c>
       <c r="I9">
         <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>10.5</v>
+      </c>
+      <c r="K9" s="30">
+        <f t="shared" si="1"/>
+        <v>43346</v>
+      </c>
+      <c r="L9" s="30">
+        <f t="shared" si="2"/>
+        <v>43352</v>
+      </c>
+      <c r="M9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
@@ -2262,47 +2374,86 @@
         <v>2</v>
       </c>
       <c r="F10">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G10">
         <v>1</v>
       </c>
       <c r="I10">
         <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="J10">
+        <v>8</v>
+      </c>
+      <c r="K10" s="30">
+        <f t="shared" si="1"/>
+        <v>43353</v>
+      </c>
+      <c r="L10" s="30">
+        <f t="shared" si="2"/>
+        <v>43359</v>
+      </c>
+      <c r="M10">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
       <c r="F11">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G11">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="I11">
         <f t="shared" si="0"/>
-        <v>8.5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="K11" s="30">
+        <f t="shared" si="1"/>
+        <v>43360</v>
+      </c>
+      <c r="L11" s="30">
+        <f t="shared" si="2"/>
+        <v>43366</v>
+      </c>
+      <c r="M11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
       <c r="F12">
-        <v>8</v>
+        <v>7.5</v>
       </c>
       <c r="H12">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="I12">
         <f t="shared" si="0"/>
         <v>8.5</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K12" s="30">
+        <f t="shared" si="1"/>
+        <v>43367</v>
+      </c>
+      <c r="L12" s="30">
+        <f t="shared" si="2"/>
+        <v>43373</v>
+      </c>
+      <c r="M12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
@@ -2310,56 +2461,94 @@
         <v>8</v>
       </c>
       <c r="I13">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <f>SUM(B14:H14)</f>
+        <v>5</v>
+      </c>
+      <c r="K13" s="30">
+        <f t="shared" si="1"/>
+        <v>43374</v>
+      </c>
+      <c r="L13" s="30">
+        <f t="shared" si="2"/>
+        <v>43380</v>
+      </c>
+      <c r="M13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
       <c r="H14">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
+      <c r="K14" s="30">
+        <f t="shared" si="1"/>
+        <v>43381</v>
+      </c>
+      <c r="L14" s="30">
+        <f t="shared" si="2"/>
+        <v>43387</v>
+      </c>
+      <c r="M14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H15">
+        <v>3</v>
+      </c>
+      <c r="K15" s="30">
+        <f t="shared" si="1"/>
+        <v>43388</v>
+      </c>
+      <c r="L15" s="30">
+        <f t="shared" si="2"/>
+        <v>43394</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="1">
-        <f t="shared" ref="B15:H15" si="1">SUM(B2:B14)</f>
-        <v>8</v>
-      </c>
-      <c r="C15" s="1">
-        <f t="shared" si="1"/>
+      <c r="B16" s="1">
+        <f>SUM(B2:B15)</f>
+        <v>10.5</v>
+      </c>
+      <c r="C16" s="1">
+        <f>SUM(C3:C15)</f>
         <v>13</v>
       </c>
-      <c r="D15" s="1">
-        <f t="shared" si="1"/>
+      <c r="D16" s="1">
+        <f>SUM(D3:D15)</f>
         <v>10</v>
       </c>
-      <c r="E15" s="1">
-        <f t="shared" si="1"/>
+      <c r="E16" s="1">
+        <f>SUM(E3:E15)</f>
         <v>2</v>
       </c>
-      <c r="F15" s="1">
-        <f t="shared" si="1"/>
-        <v>73.5</v>
-      </c>
-      <c r="G15" s="1">
-        <f t="shared" si="1"/>
-        <v>2.5</v>
-      </c>
-      <c r="H15" s="1">
-        <f t="shared" si="1"/>
-        <v>5.5</v>
-      </c>
-      <c r="I15" s="1">
-        <f>SUM(I2:I14)</f>
-        <v>109.5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="F16" s="1">
+        <f>SUM(F3:F14)</f>
+        <v>65</v>
+      </c>
+      <c r="G16" s="1">
+        <f>SUM(G3:G14)</f>
+        <v>3</v>
+      </c>
+      <c r="H16" s="1">
+        <f>SUM(H3:H14)</f>
+        <v>6</v>
+      </c>
+      <c r="I16" s="1">
+        <f>SUM(I3:I14)</f>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="17" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -2369,25 +2558,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" customWidth="1"/>
-    <col min="3" max="3" width="45.85546875" customWidth="1"/>
-    <col min="4" max="4" width="22.7109375" customWidth="1"/>
-    <col min="5" max="6" width="19.7109375" customWidth="1"/>
-    <col min="7" max="7" width="25.7109375" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" customWidth="1"/>
+    <col min="1" max="1" width="11.44140625" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" customWidth="1"/>
+    <col min="3" max="3" width="45.88671875" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" customWidth="1"/>
+    <col min="5" max="6" width="19.6640625" customWidth="1"/>
+    <col min="7" max="7" width="25.6640625" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -2416,7 +2605,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -2431,7 +2620,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -2442,11 +2631,11 @@
         <v>2</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I13" si="0">SUM(B3:H3)</f>
+        <f t="shared" ref="I3:I15" si="0">SUM(B3:H3)</f>
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -2458,7 +2647,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
@@ -2470,7 +2659,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
@@ -2482,7 +2671,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -2497,7 +2686,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -2509,7 +2698,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -2524,7 +2713,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
@@ -2539,7 +2728,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
@@ -2551,7 +2740,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
@@ -2566,7 +2755,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
@@ -2584,49 +2773,74 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
+      <c r="F14">
+        <v>3</v>
+      </c>
+      <c r="G14">
+        <v>2.5</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="0"/>
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15">
+        <v>4.5</v>
+      </c>
+      <c r="G15">
+        <v>2.5</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="1">
-        <f t="shared" ref="B15:H15" si="1">SUM(B2:B14)</f>
+      <c r="B16" s="1">
+        <f>SUM(B2:B15)</f>
         <v>4.5</v>
       </c>
-      <c r="C15" s="1">
-        <f t="shared" si="1"/>
+      <c r="C16" s="1">
+        <f t="shared" ref="C16:I16" si="1">SUM(C2:C15)</f>
         <v>2.5</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D16" s="1">
         <f t="shared" si="1"/>
         <v>8.5</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E16" s="1">
         <f t="shared" si="1"/>
         <v>22.5</v>
       </c>
-      <c r="F15" s="1">
+      <c r="F16" s="1">
         <f t="shared" si="1"/>
-        <v>20</v>
-      </c>
-      <c r="G15" s="1">
+        <v>27.5</v>
+      </c>
+      <c r="G16" s="1">
         <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="H15" s="1">
+        <v>8</v>
+      </c>
+      <c r="H16" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I15" s="1">
-        <f>SUM(I2:I14)</f>
-        <v>61</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="I16" s="1">
+        <f>SUM(I2:I15)</f>
+        <v>73.5</v>
+      </c>
+    </row>
+    <row r="17" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -2636,25 +2850,25 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:I16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" customWidth="1"/>
-    <col min="3" max="3" width="45.85546875" customWidth="1"/>
-    <col min="4" max="4" width="22.7109375" customWidth="1"/>
-    <col min="5" max="6" width="19.7109375" customWidth="1"/>
-    <col min="7" max="7" width="25.7109375" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" customWidth="1"/>
+    <col min="1" max="1" width="11.44140625" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" customWidth="1"/>
+    <col min="3" max="3" width="45.88671875" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" customWidth="1"/>
+    <col min="5" max="6" width="19.6640625" customWidth="1"/>
+    <col min="7" max="7" width="25.6640625" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -2683,7 +2897,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -2698,7 +2912,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -2712,11 +2926,11 @@
         <v>2</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I13" si="0">SUM(B3:H3)</f>
+        <f t="shared" ref="I3:I15" si="0">SUM(B3:H3)</f>
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -2728,7 +2942,7 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
@@ -2743,7 +2957,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
@@ -2755,7 +2969,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -2770,7 +2984,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -2791,7 +3005,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -2809,7 +3023,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
@@ -2824,7 +3038,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
@@ -2839,7 +3053,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
@@ -2854,58 +3068,80 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="F13">
+        <v>4</v>
+      </c>
       <c r="I13">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
+      <c r="H14">
+        <v>2.5</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H15">
+        <v>1.5</v>
+      </c>
+      <c r="I15">
+        <f>SUM(B15:H15)</f>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="1">
-        <f t="shared" ref="B15:H15" si="1">SUM(B2:B14)</f>
+      <c r="B16" s="1">
+        <f>SUM(B2:B15)</f>
         <v>8</v>
       </c>
-      <c r="C15" s="1">
-        <f t="shared" si="1"/>
+      <c r="C16" s="1">
+        <f t="shared" ref="C16:I16" si="1">SUM(C2:C15)</f>
         <v>9</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D16" s="1">
         <f t="shared" si="1"/>
         <v>15.5</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E16" s="1">
         <f t="shared" si="1"/>
         <v>28.5</v>
       </c>
-      <c r="F15" s="1">
+      <c r="F16" s="1">
         <f t="shared" si="1"/>
-        <v>9.5</v>
-      </c>
-      <c r="G15" s="1">
+        <v>13.5</v>
+      </c>
+      <c r="G16" s="1">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="H15" s="1">
+      <c r="H16" s="1">
+        <f>SUM(H2:H15)</f>
+        <v>4</v>
+      </c>
+      <c r="I16" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I15" s="1">
-        <f>SUM(I2:I14)</f>
-        <v>71.5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+        <v>79.5</v>
+      </c>
+    </row>
+    <row r="17" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -2915,26 +3151,26 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:I32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.44140625" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="50" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="21.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -2963,7 +3199,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -2978,7 +3214,7 @@
         <v>2.25</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -2989,11 +3225,11 @@
         <v>0.25</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I13" si="0">SUM(B3:H3)</f>
+        <f>SUM(B3:H3)</f>
         <v>1.75</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -3007,11 +3243,11 @@
         <v>0.25</v>
       </c>
       <c r="I4">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="I4:I15" si="0">SUM(B4:H4)</f>
         <v>3.25</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
@@ -3029,7 +3265,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
@@ -3047,7 +3283,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -3065,7 +3301,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -3083,7 +3319,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -3104,7 +3340,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
@@ -3125,7 +3361,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
@@ -3146,7 +3382,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
@@ -3167,7 +3403,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
@@ -3188,127 +3424,152 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
+      <c r="G14">
+        <v>0.5</v>
+      </c>
+      <c r="H14">
+        <v>5</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="0"/>
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G15">
+        <v>1.5</v>
+      </c>
+      <c r="H15">
+        <v>6.25</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="0"/>
+        <v>7.75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="1">
-        <f t="shared" ref="B15:H15" si="1">SUM(B2:B14)</f>
+      <c r="B16" s="1">
+        <f>SUM(B2:B15)</f>
         <v>6.25</v>
       </c>
-      <c r="C15" s="1">
-        <f t="shared" si="1"/>
+      <c r="C16" s="1">
+        <f t="shared" ref="C16:I16" si="1">SUM(C2:C15)</f>
         <v>7</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D16" s="1">
         <f t="shared" si="1"/>
         <v>7.5</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E16" s="1">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="F15" s="1">
+      <c r="F16" s="1">
         <f t="shared" si="1"/>
         <v>8.5</v>
       </c>
-      <c r="G15" s="1">
+      <c r="G16" s="1">
         <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="H16" s="1">
+        <f t="shared" si="1"/>
+        <v>11.25</v>
+      </c>
+      <c r="I16" s="1">
+        <f t="shared" si="1"/>
+        <v>70.5</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B23">
+        <v>6.25</v>
+      </c>
+      <c r="C23">
+        <v>7</v>
+      </c>
+      <c r="D23">
+        <v>7.5</v>
+      </c>
+      <c r="E23">
+        <v>17</v>
+      </c>
+      <c r="F23">
+        <v>8.5</v>
+      </c>
+      <c r="G23">
         <v>11</v>
       </c>
-      <c r="H15" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I15" s="1">
-        <f>SUM(I2:I14)</f>
-        <v>57.25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22">
+      <c r="H23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B25">
         <v>6.25</v>
       </c>
-      <c r="C22">
+      <c r="C25">
         <v>7</v>
       </c>
-      <c r="D22">
+      <c r="D25">
         <v>7.5</v>
       </c>
-      <c r="E22">
+      <c r="E25">
         <v>17</v>
       </c>
-      <c r="F22">
+      <c r="F25">
         <v>8.5</v>
       </c>
-      <c r="G22">
+      <c r="G25">
         <v>11</v>
       </c>
-      <c r="H22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24">
+      <c r="H25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B27">
         <v>6.25</v>
       </c>
-      <c r="C24">
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B28">
         <v>7</v>
       </c>
-      <c r="D24">
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B29">
         <v>7.5</v>
       </c>
-      <c r="E24">
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B30">
         <v>17</v>
       </c>
-      <c r="F24">
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B31">
         <v>8.5</v>
       </c>
-      <c r="G24">
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B32">
         <v>11</v>
       </c>
-      <c r="H24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B26">
-        <v>6.25</v>
-      </c>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B27">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B28">
-        <v>7.5</v>
-      </c>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B29">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B30">
-        <v>8.5</v>
-      </c>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B31">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B32">
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B33">
         <v>0</v>
       </c>
     </row>
@@ -3321,25 +3582,25 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:I21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" customWidth="1"/>
-    <col min="3" max="3" width="45.85546875" customWidth="1"/>
-    <col min="4" max="4" width="22.7109375" customWidth="1"/>
-    <col min="5" max="6" width="19.7109375" customWidth="1"/>
-    <col min="7" max="7" width="25.7109375" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" customWidth="1"/>
+    <col min="1" max="1" width="11.44140625" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" customWidth="1"/>
+    <col min="3" max="3" width="16.109375" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" customWidth="1"/>
+    <col min="5" max="6" width="19.6640625" customWidth="1"/>
+    <col min="7" max="7" width="25.6640625" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>36</v>
       </c>
@@ -3368,21 +3629,21 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B2">
         <f>Table1[[#This Row],[Initialising]]+Table13[[#This Row],[Initialising]]+Table134[[#This Row],[Initialising]]+Table1345[[#This Row],[Initialising]]</f>
-        <v>12.25</v>
+        <v>9.75</v>
       </c>
       <c r="C2">
         <f>Table1[[#This Row],[Discover and understand the details of the problem]]+Table13[[#This Row],[Discover and understand the details of the problem]]+Table134[[#This Row],[Discover and understand the details of the problem]]+Table1345[[#This Row],[Discover and understand the details of the problem]]</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D2">
         <f>Table1[[#This Row],[Create the project plan.]]+Table13[[#This Row],[Create the project plan.]]+Table134[[#This Row],[Create the project plan.]]+Table1345[[#This Row],[Create the project plan.]]</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E2">
         <f>Table1[[#This Row],[Design Components]]+Table13[[#This Row],[Design Components]]+Table134[[#This Row],[Design Components]]+Table1345[[#This Row],[Design Components]]</f>
@@ -3402,24 +3663,24 @@
       </c>
       <c r="I2">
         <f>SUM(B2:H2)</f>
-        <v>20.25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>13.75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B3">
         <f>Table1[[#This Row],[Initialising]]+Table13[[#This Row],[Initialising]]+Table134[[#This Row],[Initialising]]+Table1345[[#This Row],[Initialising]]</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C3">
         <f>Table1[[#This Row],[Discover and understand the details of the problem]]+Table13[[#This Row],[Discover and understand the details of the problem]]+Table134[[#This Row],[Discover and understand the details of the problem]]+Table1345[[#This Row],[Discover and understand the details of the problem]]</f>
-        <v>7.5</v>
+        <v>5.5</v>
       </c>
       <c r="D3">
         <f>Table1[[#This Row],[Create the project plan.]]+Table13[[#This Row],[Create the project plan.]]+Table134[[#This Row],[Create the project plan.]]+Table1345[[#This Row],[Create the project plan.]]</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E3">
         <f>Table1[[#This Row],[Design Components]]+Table13[[#This Row],[Design Components]]+Table134[[#This Row],[Design Components]]+Table1345[[#This Row],[Design Components]]</f>
@@ -3438,33 +3699,33 @@
         <v>0</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I13" si="0">SUM(B3:H3)</f>
-        <v>22.75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <f t="shared" ref="I3:I14" si="0">SUM(B3:H3)</f>
+        <v>21.75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B4">
         <f>Table1[[#This Row],[Initialising]]+Table13[[#This Row],[Initialising]]+Table134[[#This Row],[Initialising]]+Table1345[[#This Row],[Initialising]]</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C4">
         <f>Table1[[#This Row],[Discover and understand the details of the problem]]+Table13[[#This Row],[Discover and understand the details of the problem]]+Table134[[#This Row],[Discover and understand the details of the problem]]+Table1345[[#This Row],[Discover and understand the details of the problem]]</f>
-        <v>1.5</v>
+        <v>4.5</v>
       </c>
       <c r="D4">
         <f>Table1[[#This Row],[Create the project plan.]]+Table13[[#This Row],[Create the project plan.]]+Table134[[#This Row],[Create the project plan.]]+Table1345[[#This Row],[Create the project plan.]]</f>
-        <v>15.5</v>
+        <v>16.5</v>
       </c>
       <c r="E4">
         <f>Table1[[#This Row],[Design Components]]+Table13[[#This Row],[Design Components]]+Table134[[#This Row],[Design Components]]+Table1345[[#This Row],[Design Components]]</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4">
         <f>Table1[[#This Row],[Implement and Test]]+Table13[[#This Row],[Implement and Test]]+Table134[[#This Row],[Implement and Test]]+Table1345[[#This Row],[Implement and Test]]</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G4">
         <f>Table1[[#This Row],[Monitoring and Controlling]]+Table13[[#This Row],[Monitoring and Controlling]]+Table134[[#This Row],[Monitoring and Controlling]]+Table1345[[#This Row],[Monitoring and Controlling]]</f>
@@ -3476,10 +3737,10 @@
       </c>
       <c r="I4">
         <f t="shared" si="0"/>
-        <v>21.25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>24.25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
@@ -3493,15 +3754,15 @@
       </c>
       <c r="D5">
         <f>Table1[[#This Row],[Create the project plan.]]+Table13[[#This Row],[Create the project plan.]]+Table134[[#This Row],[Create the project plan.]]+Table1345[[#This Row],[Create the project plan.]]</f>
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E5">
         <f>Table1[[#This Row],[Design Components]]+Table13[[#This Row],[Design Components]]+Table134[[#This Row],[Design Components]]+Table1345[[#This Row],[Design Components]]</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5">
         <f>Table1[[#This Row],[Implement and Test]]+Table13[[#This Row],[Implement and Test]]+Table134[[#This Row],[Implement and Test]]+Table1345[[#This Row],[Implement and Test]]</f>
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="G5">
         <f>Table1[[#This Row],[Monitoring and Controlling]]+Table13[[#This Row],[Monitoring and Controlling]]+Table134[[#This Row],[Monitoring and Controlling]]+Table1345[[#This Row],[Monitoring and Controlling]]</f>
@@ -3513,10 +3774,10 @@
       </c>
       <c r="I5">
         <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
@@ -3538,7 +3799,7 @@
       </c>
       <c r="F6">
         <f>Table1[[#This Row],[Implement and Test]]+Table13[[#This Row],[Implement and Test]]+Table134[[#This Row],[Implement and Test]]+Table1345[[#This Row],[Implement and Test]]</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G6">
         <f>Table1[[#This Row],[Monitoring and Controlling]]+Table13[[#This Row],[Monitoring and Controlling]]+Table134[[#This Row],[Monitoring and Controlling]]+Table1345[[#This Row],[Monitoring and Controlling]]</f>
@@ -3550,10 +3811,10 @@
       </c>
       <c r="I6">
         <f t="shared" si="0"/>
-        <v>20.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>22.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -3563,7 +3824,7 @@
       </c>
       <c r="C7">
         <f>Table1[[#This Row],[Discover and understand the details of the problem]]+Table13[[#This Row],[Discover and understand the details of the problem]]+Table134[[#This Row],[Discover and understand the details of the problem]]+Table1345[[#This Row],[Discover and understand the details of the problem]]</f>
-        <v>5.25</v>
+        <v>2.25</v>
       </c>
       <c r="D7">
         <f>Table1[[#This Row],[Create the project plan.]]+Table13[[#This Row],[Create the project plan.]]+Table134[[#This Row],[Create the project plan.]]+Table1345[[#This Row],[Create the project plan.]]</f>
@@ -3571,11 +3832,11 @@
       </c>
       <c r="E7">
         <f>Table1[[#This Row],[Design Components]]+Table13[[#This Row],[Design Components]]+Table134[[#This Row],[Design Components]]+Table1345[[#This Row],[Design Components]]</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F7">
         <f>Table1[[#This Row],[Implement and Test]]+Table13[[#This Row],[Implement and Test]]+Table134[[#This Row],[Implement and Test]]+Table1345[[#This Row],[Implement and Test]]</f>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G7">
         <f>Table1[[#This Row],[Monitoring and Controlling]]+Table13[[#This Row],[Monitoring and Controlling]]+Table134[[#This Row],[Monitoring and Controlling]]+Table1345[[#This Row],[Monitoring and Controlling]]</f>
@@ -3590,7 +3851,7 @@
         <v>17.5</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -3600,7 +3861,7 @@
       </c>
       <c r="C8">
         <f>Table1[[#This Row],[Discover and understand the details of the problem]]+Table13[[#This Row],[Discover and understand the details of the problem]]+Table134[[#This Row],[Discover and understand the details of the problem]]+Table1345[[#This Row],[Discover and understand the details of the problem]]</f>
-        <v>3.75</v>
+        <v>4.75</v>
       </c>
       <c r="D8">
         <f>Table1[[#This Row],[Create the project plan.]]+Table13[[#This Row],[Create the project plan.]]+Table134[[#This Row],[Create the project plan.]]+Table1345[[#This Row],[Create the project plan.]]</f>
@@ -3608,15 +3869,15 @@
       </c>
       <c r="E8">
         <f>Table1[[#This Row],[Design Components]]+Table13[[#This Row],[Design Components]]+Table134[[#This Row],[Design Components]]+Table1345[[#This Row],[Design Components]]</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F8">
         <f>Table1[[#This Row],[Implement and Test]]+Table13[[#This Row],[Implement and Test]]+Table134[[#This Row],[Implement and Test]]+Table1345[[#This Row],[Implement and Test]]</f>
-        <v>10.5</v>
+        <v>9</v>
       </c>
       <c r="G8">
         <f>Table1[[#This Row],[Monitoring and Controlling]]+Table13[[#This Row],[Monitoring and Controlling]]+Table134[[#This Row],[Monitoring and Controlling]]+Table1345[[#This Row],[Monitoring and Controlling]]</f>
-        <v>2.75</v>
+        <v>1.75</v>
       </c>
       <c r="H8">
         <f>Table1[[#This Row],[Deploy]]+Table13[[#This Row],[Deploy]]+Table134[[#This Row],[Deploy]]+Table1345[[#This Row],[Deploy]]</f>
@@ -3624,10 +3885,10 @@
       </c>
       <c r="I8">
         <f t="shared" si="0"/>
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>36.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -3649,11 +3910,11 @@
       </c>
       <c r="F9">
         <f>Table1[[#This Row],[Implement and Test]]+Table13[[#This Row],[Implement and Test]]+Table134[[#This Row],[Implement and Test]]+Table1345[[#This Row],[Implement and Test]]</f>
-        <v>8.5</v>
+        <v>11</v>
       </c>
       <c r="G9">
         <f>Table1[[#This Row],[Monitoring and Controlling]]+Table13[[#This Row],[Monitoring and Controlling]]+Table134[[#This Row],[Monitoring and Controlling]]+Table1345[[#This Row],[Monitoring and Controlling]]</f>
-        <v>0.75</v>
+        <v>1.75</v>
       </c>
       <c r="H9">
         <f>Table1[[#This Row],[Deploy]]+Table13[[#This Row],[Deploy]]+Table134[[#This Row],[Deploy]]+Table1345[[#This Row],[Deploy]]</f>
@@ -3661,10 +3922,10 @@
       </c>
       <c r="I9">
         <f t="shared" si="0"/>
-        <v>25.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
@@ -3686,7 +3947,7 @@
       </c>
       <c r="F10">
         <f>Table1[[#This Row],[Implement and Test]]+Table13[[#This Row],[Implement and Test]]+Table134[[#This Row],[Implement and Test]]+Table1345[[#This Row],[Implement and Test]]</f>
-        <v>12.5</v>
+        <v>11.5</v>
       </c>
       <c r="G10">
         <f>Table1[[#This Row],[Monitoring and Controlling]]+Table13[[#This Row],[Monitoring and Controlling]]+Table134[[#This Row],[Monitoring and Controlling]]+Table1345[[#This Row],[Monitoring and Controlling]]</f>
@@ -3698,10 +3959,10 @@
       </c>
       <c r="I10">
         <f t="shared" si="0"/>
-        <v>29.5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <v>28.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
@@ -3711,7 +3972,7 @@
       </c>
       <c r="C11">
         <f>Table1[[#This Row],[Discover and understand the details of the problem]]+Table13[[#This Row],[Discover and understand the details of the problem]]+Table134[[#This Row],[Discover and understand the details of the problem]]+Table1345[[#This Row],[Discover and understand the details of the problem]]</f>
-        <v>0.25</v>
+        <v>2.25</v>
       </c>
       <c r="D11">
         <f>Table1[[#This Row],[Create the project plan.]]+Table13[[#This Row],[Create the project plan.]]+Table134[[#This Row],[Create the project plan.]]+Table1345[[#This Row],[Create the project plan.]]</f>
@@ -3723,11 +3984,11 @@
       </c>
       <c r="F11">
         <f>Table1[[#This Row],[Implement and Test]]+Table13[[#This Row],[Implement and Test]]+Table134[[#This Row],[Implement and Test]]+Table1345[[#This Row],[Implement and Test]]</f>
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G11">
         <f>Table1[[#This Row],[Monitoring and Controlling]]+Table13[[#This Row],[Monitoring and Controlling]]+Table134[[#This Row],[Monitoring and Controlling]]+Table1345[[#This Row],[Monitoring and Controlling]]</f>
-        <v>0.75</v>
+        <v>1.25</v>
       </c>
       <c r="H11">
         <f>Table1[[#This Row],[Deploy]]+Table13[[#This Row],[Deploy]]+Table134[[#This Row],[Deploy]]+Table1345[[#This Row],[Deploy]]</f>
@@ -3735,10 +3996,10 @@
       </c>
       <c r="I11">
         <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+        <v>28.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
@@ -3760,7 +4021,7 @@
       </c>
       <c r="F12">
         <f>Table1[[#This Row],[Implement and Test]]+Table13[[#This Row],[Implement and Test]]+Table134[[#This Row],[Implement and Test]]+Table1345[[#This Row],[Implement and Test]]</f>
-        <v>15</v>
+        <v>14.5</v>
       </c>
       <c r="G12">
         <f>Table1[[#This Row],[Monitoring and Controlling]]+Table13[[#This Row],[Monitoring and Controlling]]+Table134[[#This Row],[Monitoring and Controlling]]+Table1345[[#This Row],[Monitoring and Controlling]]</f>
@@ -3768,14 +4029,14 @@
       </c>
       <c r="H12">
         <f>Table1[[#This Row],[Deploy]]+Table13[[#This Row],[Deploy]]+Table134[[#This Row],[Deploy]]+Table1345[[#This Row],[Deploy]]</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="I12">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
@@ -3797,7 +4058,7 @@
       </c>
       <c r="F13">
         <f>Table1[[#This Row],[Implement and Test]]+Table13[[#This Row],[Implement and Test]]+Table134[[#This Row],[Implement and Test]]+Table1345[[#This Row],[Implement and Test]]</f>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G13">
         <f>Table1[[#This Row],[Monitoring and Controlling]]+Table13[[#This Row],[Monitoring and Controlling]]+Table134[[#This Row],[Monitoring and Controlling]]+Table1345[[#This Row],[Monitoring and Controlling]]</f>
@@ -3809,10 +4070,10 @@
       </c>
       <c r="I13">
         <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
@@ -3834,84 +4095,125 @@
       </c>
       <c r="F14">
         <f>Table1[[#This Row],[Implement and Test]]+Table13[[#This Row],[Implement and Test]]+Table134[[#This Row],[Implement and Test]]+Table1345[[#This Row],[Implement and Test]]</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G14">
         <f>Table1[[#This Row],[Monitoring and Controlling]]+Table13[[#This Row],[Monitoring and Controlling]]+Table134[[#This Row],[Monitoring and Controlling]]+Table1345[[#This Row],[Monitoring and Controlling]]</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H14">
         <f>Table1[[#This Row],[Deploy]]+Table13[[#This Row],[Deploy]]+Table134[[#This Row],[Deploy]]+Table1345[[#This Row],[Deploy]]</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
+        <v>12.5</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="0"/>
+        <v>18.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15">
+        <f>Table1[[#This Row],[Initialising]]+Table13[[#This Row],[Initialising]]+Table134[[#This Row],[Initialising]]+Table1345[[#This Row],[Initialising]]</f>
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <f>Table1[[#This Row],[Discover and understand the details of the problem]]+Table13[[#This Row],[Discover and understand the details of the problem]]+Table134[[#This Row],[Discover and understand the details of the problem]]+Table1345[[#This Row],[Discover and understand the details of the problem]]</f>
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <f>Table1[[#This Row],[Create the project plan.]]+Table13[[#This Row],[Create the project plan.]]+Table134[[#This Row],[Create the project plan.]]+Table1345[[#This Row],[Create the project plan.]]</f>
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <f>Table1[[#This Row],[Design Components]]+Table13[[#This Row],[Design Components]]+Table134[[#This Row],[Design Components]]+Table1345[[#This Row],[Design Components]]</f>
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <f>Table1[[#This Row],[Implement and Test]]+Table13[[#This Row],[Implement and Test]]+Table134[[#This Row],[Implement and Test]]+Table1345[[#This Row],[Implement and Test]]</f>
+        <v>4.5</v>
+      </c>
+      <c r="G15">
+        <f>Table1[[#This Row],[Monitoring and Controlling]]+Table13[[#This Row],[Monitoring and Controlling]]+Table134[[#This Row],[Monitoring and Controlling]]+Table1345[[#This Row],[Monitoring and Controlling]]</f>
+        <v>4</v>
+      </c>
+      <c r="H15">
+        <f>Table1[[#This Row],[Deploy]]+Table13[[#This Row],[Deploy]]+Table134[[#This Row],[Deploy]]+Table1345[[#This Row],[Deploy]]</f>
+        <v>10.75</v>
+      </c>
+      <c r="I15">
+        <f t="shared" ref="I15" si="1">SUM(B15:H15)</f>
+        <v>19.25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="1">
-        <f t="shared" ref="B15:H15" si="1">SUM(B2:B14)</f>
-        <v>26.75</v>
-      </c>
-      <c r="C15" s="1">
-        <f t="shared" si="1"/>
+      <c r="B16" s="1">
+        <f>SUM(B2:B15)</f>
+        <v>29.25</v>
+      </c>
+      <c r="C16" s="1">
+        <f t="shared" ref="C16:I16" si="2">SUM(C2:C15)</f>
         <v>31.5</v>
       </c>
-      <c r="D15" s="1">
-        <f t="shared" si="1"/>
+      <c r="D16" s="1">
+        <f t="shared" si="2"/>
         <v>41.5</v>
       </c>
-      <c r="E15" s="1">
-        <f t="shared" si="1"/>
+      <c r="E16" s="1">
+        <f t="shared" si="2"/>
         <v>70</v>
       </c>
-      <c r="F15" s="1">
-        <f t="shared" si="1"/>
-        <v>111.5</v>
-      </c>
-      <c r="G15" s="1">
-        <f t="shared" si="1"/>
-        <v>17.5</v>
-      </c>
-      <c r="H15" s="1">
-        <f t="shared" si="1"/>
-        <v>5.5</v>
-      </c>
-      <c r="I15" s="1">
-        <f>SUM(I2:I14)</f>
-        <v>299.25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B17">
+      <c r="F16" s="1">
+        <f t="shared" si="2"/>
+        <v>114.5</v>
+      </c>
+      <c r="G16" s="1">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="H16" s="1">
+        <f t="shared" si="2"/>
+        <v>24.25</v>
+      </c>
+      <c r="I16" s="1">
+        <f>SUM(I2:I15)</f>
+        <v>336</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B18">
         <v>15</v>
       </c>
-      <c r="C17">
+      <c r="C18">
         <v>20</v>
       </c>
-      <c r="D17">
+      <c r="D18">
         <v>32</v>
       </c>
-      <c r="E17">
+      <c r="E18">
         <v>12</v>
       </c>
-      <c r="F17" s="15">
+      <c r="F18" s="15">
         <v>201</v>
       </c>
-      <c r="G17">
+      <c r="G18">
         <v>60</v>
       </c>
-      <c r="H17">
+      <c r="H18">
         <v>37</v>
       </c>
-      <c r="I17">
+      <c r="I18">
         <v>377</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="15"/>
-      <c r="B21" s="15"/>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="15"/>
+      <c r="B22" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3923,30 +4225,30 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:Q22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" customWidth="1"/>
-    <col min="7" max="7" width="17.5703125" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" customWidth="1"/>
-    <col min="12" max="12" width="32.7109375" customWidth="1"/>
-    <col min="14" max="14" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.6640625" customWidth="1"/>
+    <col min="2" max="2" width="22.44140625" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" customWidth="1"/>
+    <col min="7" max="7" width="17.5546875" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" customWidth="1"/>
+    <col min="12" max="12" width="32.6640625" customWidth="1"/>
+    <col min="14" max="14" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
@@ -3996,7 +4298,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -4004,12 +4306,12 @@
         <v>0</v>
       </c>
       <c r="C2" s="7">
-        <f>'Total Hrs'!B15</f>
-        <v>26.75</v>
+        <f>'Total Hrs'!B16</f>
+        <v>29.25</v>
       </c>
       <c r="D2" s="10">
         <f>I2*D16</f>
-        <v>997.32499999999993</v>
+        <v>1118.95</v>
       </c>
       <c r="E2" s="10">
         <v>0</v>
@@ -4022,12 +4324,12 @@
         <v>3403.2</v>
       </c>
       <c r="H2">
-        <f>Isaac!B15</f>
+        <f>Isaac!B16</f>
         <v>6.25</v>
       </c>
       <c r="I2">
         <f>C2-H2</f>
-        <v>20.5</v>
+        <v>23</v>
       </c>
       <c r="K2" s="6">
         <v>1</v>
@@ -4051,7 +4353,7 @@
         <v>3403.2</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="11">
         <v>2</v>
       </c>
@@ -4059,7 +4361,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="12">
-        <f>'Total Hrs'!C15</f>
+        <f>'Total Hrs'!C16</f>
         <v>31.5</v>
       </c>
       <c r="D3" s="14">
@@ -4077,7 +4379,7 @@
         <v>4537.6000000000004</v>
       </c>
       <c r="H3">
-        <f>Isaac!C15</f>
+        <f>Isaac!C16</f>
         <v>7</v>
       </c>
       <c r="I3">
@@ -4106,7 +4408,7 @@
         <v>4537.6000000000004</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -4114,7 +4416,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="7">
-        <f>'Total Hrs'!D15</f>
+        <f>'Total Hrs'!D16</f>
         <v>41.5</v>
       </c>
       <c r="D4" s="10">
@@ -4132,7 +4434,7 @@
         <v>7260.16</v>
       </c>
       <c r="H4">
-        <f>Isaac!D15</f>
+        <f>Isaac!D16</f>
         <v>7.5</v>
       </c>
       <c r="I4">
@@ -4161,7 +4463,7 @@
         <v>7260.16</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="11">
         <v>4</v>
       </c>
@@ -4186,7 +4488,7 @@
         <v>1680</v>
       </c>
       <c r="H5">
-        <f>Isaac!E15</f>
+        <f>Isaac!E16</f>
         <v>17</v>
       </c>
       <c r="I5">
@@ -4215,7 +4517,7 @@
         <v>1680</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="6">
         <v>5</v>
       </c>
@@ -4223,15 +4525,15 @@
         <v>37</v>
       </c>
       <c r="C6" s="7">
-        <f>'Total Hrs'!F15</f>
-        <v>111.5</v>
+        <f>'Total Hrs'!F16</f>
+        <v>114.5</v>
       </c>
       <c r="D6" s="10">
         <v>0</v>
       </c>
       <c r="E6" s="10">
         <f>I6*E16</f>
-        <v>3605</v>
+        <v>3710</v>
       </c>
       <c r="F6" s="10">
         <f t="shared" si="0"/>
@@ -4241,12 +4543,12 @@
         <v>25200</v>
       </c>
       <c r="H6">
-        <f>Isaac!F15</f>
+        <f>Isaac!F16</f>
         <v>8.5</v>
       </c>
       <c r="I6">
         <f t="shared" si="1"/>
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="K6" s="6">
         <v>5</v>
@@ -4270,7 +4572,7 @@
         <v>25200</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="11">
         <v>6</v>
       </c>
@@ -4278,30 +4580,30 @@
         <v>4</v>
       </c>
       <c r="C7" s="12">
-        <f>'Total Hrs'!G15</f>
-        <v>17.5</v>
+        <f>'Total Hrs'!G16</f>
+        <v>25</v>
       </c>
       <c r="D7" s="14">
         <f>I7*D16</f>
-        <v>316.22499999999997</v>
+        <v>583.79999999999995</v>
       </c>
       <c r="E7" s="14">
         <v>0</v>
       </c>
       <c r="F7" s="14">
         <f t="shared" si="0"/>
-        <v>890.23</v>
+        <v>1052.0900000000001</v>
       </c>
       <c r="G7" s="14">
         <v>4764.4799999999996</v>
       </c>
       <c r="H7">
-        <f>Isaac!G15</f>
-        <v>11</v>
+        <f>Isaac!G16</f>
+        <v>13</v>
       </c>
       <c r="I7">
         <f t="shared" si="1"/>
-        <v>6.5</v>
+        <v>12</v>
       </c>
       <c r="K7" s="11">
         <v>6</v>
@@ -4325,7 +4627,7 @@
         <v>4764.4799999999996</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="6">
         <v>7</v>
       </c>
@@ -4333,30 +4635,30 @@
         <v>5</v>
       </c>
       <c r="C8" s="7">
-        <f>'Total Hrs'!H15</f>
-        <v>5.5</v>
+        <f>'Total Hrs'!H16</f>
+        <v>24.25</v>
       </c>
       <c r="D8" s="10">
         <f>I8*D16</f>
-        <v>267.57499999999999</v>
+        <v>632.44999999999993</v>
       </c>
       <c r="E8" s="10">
         <v>0</v>
       </c>
       <c r="F8" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>910.46250000000009</v>
       </c>
       <c r="G8" s="10">
         <v>8394.56</v>
       </c>
       <c r="H8">
-        <f>Isaac!H15</f>
-        <v>0</v>
+        <f>Isaac!H16</f>
+        <v>11.25</v>
       </c>
       <c r="I8">
         <f t="shared" si="1"/>
-        <v>5.5</v>
+        <v>13</v>
       </c>
       <c r="K8" s="6">
         <v>7</v>
@@ -4380,30 +4682,30 @@
         <v>8394.56</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="22" t="s">
         <v>30</v>
       </c>
       <c r="B9" s="23"/>
       <c r="C9" s="13">
         <f>SUM(C2:C8)</f>
-        <v>304.25</v>
+        <v>336</v>
       </c>
       <c r="D9" s="16">
         <f>SUM(D2:D8)</f>
-        <v>4427.1499999999996</v>
+        <v>5181.2249999999995</v>
       </c>
       <c r="E9" s="16">
         <f>SUM(E2:E8)</f>
-        <v>5460</v>
+        <v>5565</v>
       </c>
       <c r="F9" s="16">
         <f>SUM(F2:F8)</f>
-        <v>4633.2425000000003</v>
+        <v>5705.5650000000005</v>
       </c>
       <c r="G9" s="16">
         <f>SUM(D9:F9)</f>
-        <v>14520.3925</v>
+        <v>16451.79</v>
       </c>
       <c r="K9" s="22" t="s">
         <v>30</v>
@@ -4425,7 +4727,7 @@
         <v>66916</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="24" t="s">
         <v>31</v>
       </c>
@@ -4440,7 +4742,7 @@
       </c>
       <c r="I10" s="9">
         <f>G9+H10</f>
-        <v>17920.392500000002</v>
+        <v>19851.79</v>
       </c>
       <c r="K10" s="24" t="s">
         <v>31</v>
@@ -4452,7 +4754,7 @@
       <c r="P10" s="25"/>
       <c r="Q10" s="26"/>
     </row>
-    <row r="11" spans="1:17" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="27" t="s">
         <v>32</v>
       </c>
@@ -4464,7 +4766,7 @@
       <c r="G11" s="29"/>
       <c r="I11" s="9">
         <f>O22-I10</f>
-        <v>2208.6074999999983</v>
+        <v>277.20999999999913</v>
       </c>
       <c r="K11" s="27" t="s">
         <v>32</v>
@@ -4476,7 +4778,7 @@
       <c r="P11" s="28"/>
       <c r="Q11" s="29"/>
     </row>
-    <row r="12" spans="1:17" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="27" t="s">
         <v>33</v>
       </c>
@@ -4496,7 +4798,7 @@
       <c r="P12" s="28"/>
       <c r="Q12" s="29"/>
     </row>
-    <row r="13" spans="1:17" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="27" t="s">
         <v>34</v>
       </c>
@@ -4516,7 +4818,7 @@
       <c r="P13" s="28"/>
       <c r="Q13" s="29"/>
     </row>
-    <row r="14" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="19" t="s">
         <v>40</v>
       </c>
@@ -4536,13 +4838,13 @@
       <c r="P14" s="20"/>
       <c r="Q14" s="21"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="D15" s="9"/>
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="D16">
         <v>48.65</v>
       </c>
@@ -4557,34 +4859,58 @@
         <v>377</v>
       </c>
     </row>
-    <row r="17" spans="7:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:15" x14ac:dyDescent="0.3">
       <c r="M17">
         <f>M9-M16</f>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="7:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:15" x14ac:dyDescent="0.3">
       <c r="N19" s="9">
         <f>3400+G9</f>
-        <v>17920.392500000002</v>
-      </c>
-    </row>
-    <row r="20" spans="7:15" x14ac:dyDescent="0.25">
+        <v>19851.79</v>
+      </c>
+    </row>
+    <row r="20" spans="4:15" x14ac:dyDescent="0.3">
       <c r="G20" s="9"/>
       <c r="O20" s="9">
         <f>Q9/4</f>
         <v>16729</v>
       </c>
     </row>
-    <row r="21" spans="7:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D21" s="31">
+        <v>16451.79</v>
+      </c>
       <c r="O21" s="18">
         <v>3400</v>
       </c>
     </row>
-    <row r="22" spans="7:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D22" s="9">
+        <v>3400</v>
+      </c>
       <c r="O22" s="9">
         <f>SUM(O20:O21)</f>
         <v>20129</v>
+      </c>
+    </row>
+    <row r="23" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D23" s="9">
+        <f>D21+D22</f>
+        <v>19851.79</v>
+      </c>
+    </row>
+    <row r="25" spans="4:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="26" spans="4:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D26" s="32">
+        <v>20129</v>
+      </c>
+    </row>
+    <row r="27" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D27" s="9">
+        <f>D26-D23</f>
+        <v>277.20999999999913</v>
       </c>
     </row>
   </sheetData>
@@ -4607,16 +4933,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="K2:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="11:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="11:13" x14ac:dyDescent="0.3">
       <c r="K2">
         <f>103/240</f>
         <v>0.42916666666666664</v>

</xml_diff>

<commit_message>
Small update to costings
</commit_message>
<xml_diff>
--- a/Report/Costings summary.xlsx
+++ b/Report/Costings summary.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jocelyn\Documents\GitHub\CSC3600\Report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Documents\GitHub\CSC3600\Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92C32216-CE54-4F47-A76B-7F9806BFBA41}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9396" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9390" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Greg" sheetId="2" r:id="rId1"/>
@@ -21,7 +22,7 @@
     <sheet name="Sheet1" sheetId="11" r:id="rId7"/>
     <sheet name="Sheet2" sheetId="12" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="64">
   <si>
     <t>Initialising</t>
   </si>
@@ -317,10 +318,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="164" formatCode="0.0%"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
+    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -764,7 +766,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -786,8 +788,8 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="8" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -799,11 +801,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="8" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -811,9 +813,61 @@
     </xf>
     <xf numFmtId="4" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="8" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="8" fontId="3" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="4" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="6" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="6" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="3" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -848,58 +902,8 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="4" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="6" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="6" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="3" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="3" fillId="3" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="3" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
@@ -945,7 +949,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1029,7 +1033,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
@@ -1084,31 +1088,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>29.25</c:v>
+                  <c:v>30.25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>31.5</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>41.5</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>107</c:v>
+                  <c:v>107.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>25</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>31.75</c:v>
+                  <c:v>29.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-ACD9-4971-BA0D-4B8446FB8B5C}"/>
             </c:ext>
@@ -1169,7 +1173,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
@@ -1248,7 +1252,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-ACD9-4971-BA0D-4B8446FB8B5C}"/>
             </c:ext>
@@ -2015,7 +2019,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2037,90 +2041,90 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:I16" totalsRowShown="0">
-  <autoFilter ref="A1:I16"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:I16" totalsRowShown="0">
+  <autoFilter ref="A1:I16" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="Column1" dataDxfId="4"/>
-    <tableColumn id="2" name="Initialising"/>
-    <tableColumn id="3" name="Discover and understand the details of the problem"/>
-    <tableColumn id="4" name="Create the project plan."/>
-    <tableColumn id="5" name="Design Components"/>
-    <tableColumn id="6" name="Implement and Test"/>
-    <tableColumn id="7" name="Monitoring and Controlling"/>
-    <tableColumn id="8" name="Deploy"/>
-    <tableColumn id="9" name="Weekly Total"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Column1" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Initialising"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Discover and understand the details of the problem"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Create the project plan."/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Design Components"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Implement and Test"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Monitoring and Controlling"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Deploy"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Weekly Total"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A1:I16" totalsRowShown="0">
-  <autoFilter ref="A1:I16"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table13" displayName="Table13" ref="A1:I16" totalsRowShown="0">
+  <autoFilter ref="A1:I16" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="Column1" dataDxfId="3"/>
-    <tableColumn id="2" name="Initialising"/>
-    <tableColumn id="3" name="Discover and understand the details of the problem"/>
-    <tableColumn id="4" name="Create the project plan."/>
-    <tableColumn id="5" name="Design Components"/>
-    <tableColumn id="6" name="Implement and Test"/>
-    <tableColumn id="7" name="Monitoring and Controlling"/>
-    <tableColumn id="8" name="Deploy"/>
-    <tableColumn id="9" name="Weekly Total"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Column1" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Initialising"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Discover and understand the details of the problem"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Create the project plan."/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Design Components"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Implement and Test"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Monitoring and Controlling"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Deploy"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Weekly Total"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table134" displayName="Table134" ref="A1:I16" totalsRowShown="0">
-  <autoFilter ref="A1:I16"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table134" displayName="Table134" ref="A1:I16" totalsRowShown="0">
+  <autoFilter ref="A1:I16" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="Column1" dataDxfId="2"/>
-    <tableColumn id="2" name="Initialising"/>
-    <tableColumn id="3" name="Discover and understand the details of the problem"/>
-    <tableColumn id="4" name="Create the project plan."/>
-    <tableColumn id="5" name="Design Components"/>
-    <tableColumn id="6" name="Implement and Test"/>
-    <tableColumn id="7" name="Monitoring and Controlling"/>
-    <tableColumn id="8" name="Deploy"/>
-    <tableColumn id="9" name="Weekly Total"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Column1" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Initialising"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Discover and understand the details of the problem"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Create the project plan."/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Design Components"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Implement and Test"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Monitoring and Controlling"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Deploy"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="Weekly Total"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table1345" displayName="Table1345" ref="A1:I16" totalsRowShown="0">
-  <autoFilter ref="A1:I16"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table1345" displayName="Table1345" ref="A1:I16" totalsRowShown="0">
+  <autoFilter ref="A1:I16" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="Column1" dataDxfId="1"/>
-    <tableColumn id="2" name="Initialising"/>
-    <tableColumn id="3" name="Discover and understand the details of the problem"/>
-    <tableColumn id="4" name="Create the project plan."/>
-    <tableColumn id="5" name="Design Components"/>
-    <tableColumn id="6" name="Implement and Test"/>
-    <tableColumn id="7" name="Monitoring and Controlling"/>
-    <tableColumn id="8" name="Deploy"/>
-    <tableColumn id="9" name="Weekly Total"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Column1" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Initialising"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Discover and understand the details of the problem"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Create the project plan."/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Design Components"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Implement and Test"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="Monitoring and Controlling"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="Deploy"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0300-000009000000}" name="Weekly Total"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table13456" displayName="Table13456" ref="A1:I16" totalsRowShown="0">
-  <autoFilter ref="A1:I16"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table13456" displayName="Table13456" ref="A1:I16" totalsRowShown="0">
+  <autoFilter ref="A1:I16" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="Week Number" dataDxfId="0"/>
-    <tableColumn id="2" name="Initialising"/>
-    <tableColumn id="3" name="Discover and understand the details of the problem"/>
-    <tableColumn id="4" name="Create the project plan."/>
-    <tableColumn id="5" name="Design Components"/>
-    <tableColumn id="6" name="Implement and Test"/>
-    <tableColumn id="7" name="Monitoring and Controlling"/>
-    <tableColumn id="8" name="Deploy"/>
-    <tableColumn id="9" name="Weekly Total"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Week Number" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Initialising"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Discover and understand the details of the problem"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Create the project plan."/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="Design Components"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0400-000006000000}" name="Implement and Test"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0400-000007000000}" name="Monitoring and Controlling"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0400-000008000000}" name="Deploy"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0400-000009000000}" name="Weekly Total"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2388,27 +2392,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:I16"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" customWidth="1"/>
-    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="50" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -2437,7 +2441,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -2454,7 +2458,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -2483,7 +2487,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -2512,7 +2516,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
@@ -2541,7 +2545,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
@@ -2564,7 +2568,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -2587,7 +2591,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -2616,7 +2620,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -2645,7 +2649,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
@@ -2677,7 +2681,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
@@ -2706,7 +2710,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
@@ -2732,7 +2736,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
@@ -2755,7 +2759,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
@@ -2774,7 +2778,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>41</v>
       </c>
@@ -2790,7 +2794,7 @@
         <v>43394</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>21</v>
       </c>
@@ -2827,7 +2831,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="17" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -2837,25 +2841,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" customWidth="1"/>
-    <col min="3" max="3" width="45.88671875" customWidth="1"/>
-    <col min="4" max="4" width="22.6640625" customWidth="1"/>
-    <col min="5" max="6" width="19.6640625" customWidth="1"/>
-    <col min="7" max="7" width="25.6640625" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
+    <col min="3" max="3" width="45.85546875" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" customWidth="1"/>
+    <col min="5" max="6" width="19.7109375" customWidth="1"/>
+    <col min="7" max="7" width="25.7109375" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -2884,73 +2888,88 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <v>0.5</v>
       </c>
+      <c r="G2">
+        <v>0.25</v>
+      </c>
       <c r="I2">
         <f>SUM(B2:H2)</f>
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
+      <c r="G3">
+        <v>0.25</v>
+      </c>
       <c r="I3">
-        <f t="shared" ref="I3:I15" si="0">SUM(B3:H3)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+        <f t="shared" ref="I3:I13" si="0">SUM(B3:H3)</f>
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D4">
+      <c r="C4">
         <v>1.5</v>
+      </c>
+      <c r="G4">
+        <v>0.25</v>
       </c>
       <c r="I4">
         <f t="shared" si="0"/>
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D5">
         <v>4</v>
       </c>
+      <c r="G5">
+        <v>0.25</v>
+      </c>
       <c r="I5">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+        <v>4.25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D6">
         <v>3</v>
       </c>
+      <c r="G6">
+        <v>0.25</v>
+      </c>
       <c r="I6">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+        <v>3.25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -2960,39 +2979,48 @@
       <c r="E7">
         <v>1</v>
       </c>
+      <c r="G7">
+        <v>0.25</v>
+      </c>
       <c r="I7">
         <f t="shared" si="0"/>
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E8">
         <v>11</v>
       </c>
+      <c r="G8">
+        <v>0.25</v>
+      </c>
       <c r="I8">
         <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+        <v>11.25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E9">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F9">
         <v>2</v>
       </c>
+      <c r="G9">
+        <v>0.25</v>
+      </c>
       <c r="I9">
         <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+        <v>8.25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
@@ -3000,26 +3028,32 @@
         <v>3</v>
       </c>
       <c r="F10">
-        <v>2.5</v>
+        <v>3</v>
+      </c>
+      <c r="G10">
+        <v>0.25</v>
       </c>
       <c r="I10">
         <f t="shared" si="0"/>
-        <v>5.5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F11">
         <v>8</v>
       </c>
+      <c r="G11">
+        <v>0.25</v>
+      </c>
       <c r="I11">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+        <v>8.25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
@@ -3027,14 +3061,14 @@
         <v>4.5</v>
       </c>
       <c r="G12">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="I12">
         <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+        <v>4.75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
@@ -3045,81 +3079,81 @@
         <v>3</v>
       </c>
       <c r="G13">
-        <v>2.5</v>
+        <v>2.75</v>
       </c>
       <c r="I13">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+        <v>8.25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
       <c r="G14">
-        <v>2.5</v>
+        <v>2.75</v>
       </c>
       <c r="H14">
         <v>3</v>
       </c>
       <c r="I14">
         <f>SUM(B14:H14)</f>
-        <v>5.5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>41</v>
       </c>
       <c r="G15">
-        <v>2.5</v>
+        <v>2.75</v>
       </c>
       <c r="H15">
-        <v>4.5</v>
+        <v>2</v>
       </c>
       <c r="I15">
         <f>SUM(B15:H15)</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>4.75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B16" s="1">
         <f>SUM(B2:B15)</f>
-        <v>4.5</v>
+        <v>5.5</v>
       </c>
       <c r="C16" s="1">
-        <f t="shared" ref="C16:H16" si="1">SUM(C2:C15)</f>
-        <v>2.5</v>
+        <f t="shared" ref="C16:G16" si="1">SUM(C2:C15)</f>
+        <v>4</v>
       </c>
       <c r="D16" s="1">
         <f t="shared" si="1"/>
-        <v>8.5</v>
+        <v>7</v>
       </c>
       <c r="E16" s="1">
         <f t="shared" si="1"/>
-        <v>22.5</v>
+        <v>23.5</v>
       </c>
       <c r="F16" s="1">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>20.5</v>
       </c>
       <c r="G16" s="1">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="H16" s="1">
         <f>SUM(H2:H15)</f>
-        <v>7.5</v>
+        <v>5</v>
       </c>
       <c r="I16" s="1">
         <f>SUM(I2:I15)</f>
-        <v>73.5</v>
-      </c>
-    </row>
-    <row r="17" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+        <v>76.5</v>
+      </c>
+    </row>
+    <row r="17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -3129,25 +3163,25 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:I16"/>
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" customWidth="1"/>
-    <col min="3" max="3" width="45.88671875" customWidth="1"/>
-    <col min="4" max="4" width="22.6640625" customWidth="1"/>
-    <col min="5" max="6" width="19.6640625" customWidth="1"/>
-    <col min="7" max="7" width="25.6640625" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
+    <col min="3" max="3" width="45.85546875" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" customWidth="1"/>
+    <col min="5" max="6" width="19.7109375" customWidth="1"/>
+    <col min="7" max="7" width="25.7109375" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -3176,7 +3210,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -3191,7 +3225,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -3209,7 +3243,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -3221,7 +3255,7 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
@@ -3236,7 +3270,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
@@ -3248,7 +3282,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -3263,7 +3297,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -3284,7 +3318,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -3302,7 +3336,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
@@ -3317,7 +3351,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
@@ -3332,7 +3366,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
@@ -3347,7 +3381,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
@@ -3359,7 +3393,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
@@ -3371,7 +3405,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>41</v>
       </c>
@@ -3383,7 +3417,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>21</v>
       </c>
@@ -3420,7 +3454,7 @@
         <v>79.5</v>
       </c>
     </row>
-    <row r="17" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -3430,26 +3464,26 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" customWidth="1"/>
-    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="50" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -3478,7 +3512,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -3493,7 +3527,7 @@
         <v>2.25</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -3508,7 +3542,7 @@
         <v>1.75</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -3526,7 +3560,7 @@
         <v>3.25</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
@@ -3544,7 +3578,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
@@ -3562,7 +3596,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -3580,7 +3614,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -3598,7 +3632,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -3619,7 +3653,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
@@ -3640,7 +3674,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
@@ -3661,7 +3695,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
@@ -3682,7 +3716,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
@@ -3703,7 +3737,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
@@ -3718,7 +3752,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>41</v>
       </c>
@@ -3733,7 +3767,7 @@
         <v>7.75</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>21</v>
       </c>
@@ -3770,8 +3804,8 @@
         <v>70.5</v>
       </c>
     </row>
-    <row r="17" spans="2:8" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>6.25</v>
       </c>
@@ -3794,7 +3828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>6.25</v>
       </c>
@@ -3817,37 +3851,37 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>6.25</v>
       </c>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>7.5</v>
       </c>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31">
         <v>8.5</v>
       </c>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B32">
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33">
         <v>0</v>
       </c>
@@ -3861,49 +3895,49 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:Q32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12:Q12"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="8" max="8" width="13.44140625" customWidth="1"/>
-    <col min="9" max="9" width="17.6640625" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" customWidth="1"/>
+    <col min="9" max="9" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A1" s="33" t="s">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="34" t="s">
+      <c r="B1" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="D1" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="34" t="s">
+      <c r="E1" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="34" t="s">
+      <c r="F1" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="34" t="s">
+      <c r="G1" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="34" t="s">
+      <c r="H1" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="35" t="s">
+      <c r="I1" s="24" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>43</v>
       </c>
@@ -3940,44 +3974,44 @@
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>44</v>
       </c>
       <c r="B3">
         <f>Ryan!B16</f>
-        <v>4.5</v>
+        <v>5.5</v>
       </c>
       <c r="C3">
         <f>Ryan!C16</f>
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="D3">
         <f>Ryan!D16</f>
-        <v>8.5</v>
+        <v>7</v>
       </c>
       <c r="E3">
         <f>Ryan!E16</f>
-        <v>22.5</v>
+        <v>23.5</v>
       </c>
       <c r="F3">
         <f>Ryan!F16</f>
-        <v>20</v>
+        <v>20.5</v>
       </c>
       <c r="G3">
         <f>Ryan!G16</f>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="H3">
         <f>Ryan!H16</f>
-        <v>7.5</v>
+        <v>5</v>
       </c>
       <c r="I3">
         <f>Ryan!I16</f>
-        <v>73.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+        <v>76.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>45</v>
       </c>
@@ -4014,7 +4048,7 @@
         <v>79.5</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>46</v>
       </c>
@@ -4051,405 +4085,734 @@
         <v>70.5</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>21</v>
       </c>
       <c r="B6">
         <f>SUM(B2:B5)</f>
-        <v>29.25</v>
+        <v>30.25</v>
       </c>
       <c r="C6">
         <f t="shared" ref="C6:I6" si="0">SUM(C2:C5)</f>
-        <v>31.5</v>
+        <v>33</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>41.5</v>
+        <v>40</v>
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F6">
         <f t="shared" si="0"/>
-        <v>107</v>
+        <v>107.5</v>
       </c>
       <c r="G6">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H6">
         <f t="shared" si="0"/>
-        <v>28.75</v>
+        <v>26.25</v>
       </c>
       <c r="I6">
         <f t="shared" si="0"/>
-        <v>322.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="M7" s="37" t="s">
+        <v>325.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="M7" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="N7" s="39" t="s">
+      <c r="N7" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="O7" s="39" t="s">
+      <c r="O7" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="P7" s="48" t="s">
+      <c r="P7" s="40" t="s">
         <v>53</v>
       </c>
-      <c r="Q7" s="41" t="s">
+      <c r="Q7" s="30" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="33" t="s">
+    <row r="8" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="B8" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8" s="34" t="s">
+      <c r="B8" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="34" t="s">
+      <c r="D8" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="34" t="s">
+      <c r="E8" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="F8" s="34" t="s">
+      <c r="F8" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="34" t="s">
+      <c r="G8" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="H8" s="34" t="s">
+      <c r="H8" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="I8" s="35" t="s">
+      <c r="I8" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="M8" s="38" t="s">
+      <c r="M8" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="N8" s="40" t="s">
+      <c r="N8" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="O8" s="40" t="s">
+      <c r="O8" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="P8" s="49"/>
-      <c r="Q8" s="42" t="s">
+      <c r="P8" s="41"/>
+      <c r="Q8" s="31" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>43</v>
       </c>
-      <c r="B9" s="36">
+      <c r="B9" s="25">
         <f>B2/B$6</f>
-        <v>0.35897435897435898</v>
-      </c>
-      <c r="C9" s="36">
-        <f t="shared" ref="C9:I9" si="1">C2/C$6</f>
-        <v>0.41269841269841268</v>
-      </c>
-      <c r="D9" s="36">
+        <v>0.34710743801652894</v>
+      </c>
+      <c r="C9" s="25">
+        <f t="shared" ref="C9:H9" si="1">C2/C$6</f>
+        <v>0.39393939393939392</v>
+      </c>
+      <c r="D9" s="25">
         <f t="shared" si="1"/>
-        <v>0.24096385542168675</v>
-      </c>
-      <c r="E9" s="36">
+        <v>0.25</v>
+      </c>
+      <c r="E9" s="25">
         <f t="shared" si="1"/>
-        <v>2.8571428571428571E-2</v>
-      </c>
-      <c r="F9" s="36">
+        <v>2.8169014084507043E-2</v>
+      </c>
+      <c r="F9" s="25">
         <f t="shared" si="1"/>
-        <v>0.60747663551401865</v>
-      </c>
-      <c r="G9" s="36">
+        <v>0.60465116279069764</v>
+      </c>
+      <c r="G9" s="25">
         <f t="shared" si="1"/>
-        <v>0.12</v>
-      </c>
-      <c r="H9" s="36">
+        <v>0.10714285714285714</v>
+      </c>
+      <c r="H9" s="25">
         <f t="shared" si="1"/>
-        <v>0.20869565217391303</v>
-      </c>
-      <c r="I9" s="36">
-        <f t="shared" si="1"/>
-        <v>0.30697674418604654</v>
-      </c>
-      <c r="M9" s="43"/>
-      <c r="N9" s="50">
+        <v>0.22857142857142856</v>
+      </c>
+      <c r="I9" s="25">
+        <v>0.25</v>
+      </c>
+      <c r="J9" s="25">
+        <v>0.25</v>
+      </c>
+      <c r="K9" s="25">
+        <f>SUM(B9:J9)/9</f>
+        <v>0.27328681050504594</v>
+      </c>
+      <c r="M9" s="32"/>
+      <c r="N9" s="37">
         <v>0.154</v>
       </c>
-      <c r="O9" s="51">
+      <c r="O9" s="38">
         <v>0.214</v>
       </c>
-      <c r="P9" s="51">
+      <c r="P9" s="38">
         <v>0.27400000000000002</v>
       </c>
-      <c r="Q9" s="52">
+      <c r="Q9" s="39">
         <v>0.35899999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="36">
-        <f t="shared" ref="B10:I10" si="2">B3/B$6</f>
-        <v>0.15384615384615385</v>
-      </c>
-      <c r="C10" s="36">
+      <c r="B10" s="25">
+        <f t="shared" ref="B10:H10" si="2">B3/B$6</f>
+        <v>0.18181818181818182</v>
+      </c>
+      <c r="C10" s="25">
         <f t="shared" si="2"/>
-        <v>7.9365079365079361E-2</v>
-      </c>
-      <c r="D10" s="36">
+        <v>0.12121212121212122</v>
+      </c>
+      <c r="D10" s="25">
         <f t="shared" si="2"/>
-        <v>0.20481927710843373</v>
-      </c>
-      <c r="E10" s="36">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="E10" s="25">
         <f t="shared" si="2"/>
-        <v>0.32142857142857145</v>
-      </c>
-      <c r="F10" s="36">
+        <v>0.33098591549295775</v>
+      </c>
+      <c r="F10" s="25">
         <f t="shared" si="2"/>
-        <v>0.18691588785046728</v>
-      </c>
-      <c r="G10" s="36">
+        <v>0.19069767441860466</v>
+      </c>
+      <c r="G10" s="25">
         <f t="shared" si="2"/>
-        <v>0.32</v>
-      </c>
-      <c r="H10" s="36">
+        <v>0.39285714285714285</v>
+      </c>
+      <c r="H10" s="25">
         <f t="shared" si="2"/>
-        <v>0.2608695652173913</v>
-      </c>
-      <c r="I10" s="36">
-        <f t="shared" si="2"/>
-        <v>0.22790697674418606</v>
-      </c>
-      <c r="M10" s="43" t="s">
+        <v>0.19047619047619047</v>
+      </c>
+      <c r="I10" s="25">
+        <v>0.25</v>
+      </c>
+      <c r="J10" s="25">
+        <v>0.25</v>
+      </c>
+      <c r="K10" s="25">
+        <f t="shared" ref="K10:K12" si="3">SUM(B10:J10)/9</f>
+        <v>0.2314496918083554</v>
+      </c>
+      <c r="M10" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="N10" s="44">
+      <c r="N10" s="33">
         <v>7.9000000000000001E-2</v>
       </c>
-      <c r="O10" s="44">
+      <c r="O10" s="33">
         <v>0.222</v>
       </c>
-      <c r="P10" s="44">
+      <c r="P10" s="33">
         <v>0.28599999999999998</v>
       </c>
-      <c r="Q10" s="44">
+      <c r="Q10" s="33">
         <v>0.41299999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>45</v>
       </c>
-      <c r="B11" s="36">
-        <f t="shared" ref="B11:I11" si="3">B4/B$6</f>
-        <v>0.27350427350427353</v>
-      </c>
-      <c r="C11" s="36">
+      <c r="B11" s="25">
+        <f t="shared" ref="B11:H11" si="4">B4/B$6</f>
+        <v>0.26446280991735538</v>
+      </c>
+      <c r="C11" s="25">
+        <f t="shared" si="4"/>
+        <v>0.27272727272727271</v>
+      </c>
+      <c r="D11" s="25">
+        <f t="shared" si="4"/>
+        <v>0.38750000000000001</v>
+      </c>
+      <c r="E11" s="25">
+        <f t="shared" si="4"/>
+        <v>0.40140845070422537</v>
+      </c>
+      <c r="F11" s="25">
+        <f t="shared" si="4"/>
+        <v>0.12558139534883722</v>
+      </c>
+      <c r="G11" s="25">
+        <f t="shared" si="4"/>
+        <v>3.5714285714285712E-2</v>
+      </c>
+      <c r="H11" s="25">
+        <f t="shared" si="4"/>
+        <v>0.15238095238095239</v>
+      </c>
+      <c r="I11" s="25">
+        <v>0.25</v>
+      </c>
+      <c r="J11" s="25">
+        <v>0.25</v>
+      </c>
+      <c r="K11" s="25">
         <f t="shared" si="3"/>
-        <v>0.2857142857142857</v>
-      </c>
-      <c r="D11" s="36">
-        <f t="shared" si="3"/>
-        <v>0.37349397590361444</v>
-      </c>
-      <c r="E11" s="36">
-        <f t="shared" si="3"/>
-        <v>0.40714285714285714</v>
-      </c>
-      <c r="F11" s="36">
-        <f t="shared" si="3"/>
-        <v>0.12616822429906541</v>
-      </c>
-      <c r="G11" s="36">
-        <f t="shared" si="3"/>
-        <v>0.04</v>
-      </c>
-      <c r="H11" s="36">
-        <f t="shared" si="3"/>
-        <v>0.1391304347826087</v>
-      </c>
-      <c r="I11" s="36">
-        <f t="shared" si="3"/>
-        <v>0.24651162790697675</v>
-      </c>
-      <c r="M11" s="43" t="s">
+        <v>0.23775279631032545</v>
+      </c>
+      <c r="M11" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="N11" s="45">
+      <c r="N11" s="34">
         <v>0.25</v>
       </c>
-      <c r="O11" s="45">
+      <c r="O11" s="34">
         <v>0.25</v>
       </c>
-      <c r="P11" s="45">
+      <c r="P11" s="34">
         <v>0.25</v>
       </c>
-      <c r="Q11" s="45">
+      <c r="Q11" s="34">
         <v>0.25</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="36">
-        <f t="shared" ref="B12:I12" si="4">B5/B$6</f>
-        <v>0.21367521367521367</v>
-      </c>
-      <c r="C12" s="36">
-        <f t="shared" si="4"/>
-        <v>0.22222222222222221</v>
-      </c>
-      <c r="D12" s="36">
-        <f t="shared" si="4"/>
-        <v>0.18072289156626506</v>
-      </c>
-      <c r="E12" s="36">
-        <f t="shared" si="4"/>
-        <v>0.24285714285714285</v>
-      </c>
-      <c r="F12" s="36">
-        <f t="shared" si="4"/>
-        <v>7.9439252336448593E-2</v>
-      </c>
-      <c r="G12" s="36">
-        <f t="shared" si="4"/>
+      <c r="B12" s="25">
+        <f t="shared" ref="B12:H12" si="5">B5/B$6</f>
+        <v>0.20661157024793389</v>
+      </c>
+      <c r="C12" s="25">
+        <f t="shared" si="5"/>
+        <v>0.21212121212121213</v>
+      </c>
+      <c r="D12" s="25">
+        <f t="shared" si="5"/>
+        <v>0.1875</v>
+      </c>
+      <c r="E12" s="25">
+        <f t="shared" si="5"/>
+        <v>0.23943661971830985</v>
+      </c>
+      <c r="F12" s="25">
+        <f t="shared" si="5"/>
+        <v>7.9069767441860464E-2</v>
+      </c>
+      <c r="G12" s="25">
+        <f t="shared" si="5"/>
+        <v>0.4642857142857143</v>
+      </c>
+      <c r="H12" s="25">
+        <f t="shared" si="5"/>
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="I12" s="25">
+        <v>0.25</v>
+      </c>
+      <c r="J12" s="25">
+        <v>0.25</v>
+      </c>
+      <c r="K12" s="25">
+        <f t="shared" si="3"/>
+        <v>0.25751070137627319</v>
+      </c>
+      <c r="M12" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="N12" s="34">
+        <v>0.25</v>
+      </c>
+      <c r="O12" s="34">
+        <v>0.25</v>
+      </c>
+      <c r="P12" s="34">
+        <v>0.25</v>
+      </c>
+      <c r="Q12" s="34">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M13" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="N13" s="36">
+        <v>0.32100000000000001</v>
+      </c>
+      <c r="O13" s="36">
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="P13" s="36">
+        <v>0.40699999999999997</v>
+      </c>
+      <c r="Q13" s="36">
+        <v>2.9000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M14" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="N14" s="35"/>
+      <c r="O14" s="35"/>
+      <c r="P14" s="35"/>
+      <c r="Q14" s="35"/>
+    </row>
+    <row r="15" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="25">
+        <v>0.34710743801652894</v>
+      </c>
+      <c r="C15" s="25">
+        <v>0.39393939393939392</v>
+      </c>
+      <c r="D15" s="25">
+        <v>0.25</v>
+      </c>
+      <c r="E15" s="25">
+        <v>2.8169014084507043E-2</v>
+      </c>
+      <c r="F15" s="25">
+        <v>0.60465116279069764</v>
+      </c>
+      <c r="G15" s="25">
+        <v>0.10714285714285714</v>
+      </c>
+      <c r="H15" s="25">
+        <v>0.22857142857142856</v>
+      </c>
+      <c r="I15" s="25">
+        <v>0.25</v>
+      </c>
+      <c r="J15" s="25">
+        <v>0.25</v>
+      </c>
+      <c r="K15">
+        <v>0.27328681050504594</v>
+      </c>
+      <c r="M15" s="32" t="s">
+        <v>61</v>
+      </c>
+      <c r="N15" s="36">
+        <v>0.187</v>
+      </c>
+      <c r="O15" s="36">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="P15" s="36">
+        <v>0.126</v>
+      </c>
+      <c r="Q15" s="36">
+        <v>0.60699999999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="25">
+        <v>0.18181818181818182</v>
+      </c>
+      <c r="C16" s="25">
+        <v>0.12121212121212122</v>
+      </c>
+      <c r="D16" s="25">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="E16" s="25">
+        <v>0.33098591549295775</v>
+      </c>
+      <c r="F16" s="25">
+        <v>0.19069767441860466</v>
+      </c>
+      <c r="G16" s="25">
+        <v>0.39285714285714285</v>
+      </c>
+      <c r="H16" s="25">
+        <v>0.19047619047619047</v>
+      </c>
+      <c r="I16" s="25">
+        <v>0.25</v>
+      </c>
+      <c r="J16" s="25">
+        <v>0.25</v>
+      </c>
+      <c r="K16">
+        <v>0.2314496918083554</v>
+      </c>
+      <c r="M16" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="N16" s="33">
+        <v>0.26100000000000001</v>
+      </c>
+      <c r="O16" s="33">
+        <v>0.39100000000000001</v>
+      </c>
+      <c r="P16" s="33">
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="Q16" s="33">
+        <v>0.20899999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="25">
+        <v>0.26446280991735538</v>
+      </c>
+      <c r="C17" s="25">
+        <v>0.27272727272727271</v>
+      </c>
+      <c r="D17" s="25">
+        <v>0.38750000000000001</v>
+      </c>
+      <c r="E17" s="25">
+        <v>0.40140845070422537</v>
+      </c>
+      <c r="F17" s="25">
+        <v>0.12558139534883722</v>
+      </c>
+      <c r="G17" s="25">
+        <v>3.5714285714285712E-2</v>
+      </c>
+      <c r="H17" s="25">
+        <v>0.15238095238095239</v>
+      </c>
+      <c r="I17" s="25">
+        <v>0.25</v>
+      </c>
+      <c r="J17" s="25">
+        <v>0.25</v>
+      </c>
+      <c r="K17">
+        <v>0.23775279631032545</v>
+      </c>
+      <c r="M17" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="N17" s="36">
+        <v>0.32</v>
+      </c>
+      <c r="O17" s="36">
         <v>0.52</v>
       </c>
-      <c r="H12" s="36">
-        <f t="shared" si="4"/>
-        <v>0.39130434782608697</v>
-      </c>
-      <c r="I12" s="36">
-        <f t="shared" si="4"/>
-        <v>0.21860465116279071</v>
-      </c>
-      <c r="M12" s="43" t="s">
-        <v>58</v>
-      </c>
-      <c r="N12" s="45">
+      <c r="P17" s="36">
+        <v>0.04</v>
+      </c>
+      <c r="Q17" s="36">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="25">
+        <v>0.20661157024793389</v>
+      </c>
+      <c r="C18" s="25">
+        <v>0.21212121212121213</v>
+      </c>
+      <c r="D18" s="25">
+        <v>0.1875</v>
+      </c>
+      <c r="E18" s="25">
+        <v>0.23943661971830985</v>
+      </c>
+      <c r="F18" s="25">
+        <v>7.9069767441860464E-2</v>
+      </c>
+      <c r="G18" s="25">
+        <v>0.4642857142857143</v>
+      </c>
+      <c r="H18" s="25">
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="I18" s="25">
         <v>0.25</v>
       </c>
-      <c r="O12" s="45">
+      <c r="J18" s="25">
         <v>0.25</v>
       </c>
-      <c r="P12" s="45">
-        <v>0.25</v>
-      </c>
-      <c r="Q12" s="45">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="M13" s="43" t="s">
-        <v>59</v>
-      </c>
-      <c r="N13" s="47">
-        <v>0.32100000000000001</v>
-      </c>
-      <c r="O13" s="47">
-        <v>0.24299999999999999</v>
-      </c>
-      <c r="P13" s="47">
-        <v>0.40699999999999997</v>
-      </c>
-      <c r="Q13" s="47">
-        <v>2.9000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="M14" s="43" t="s">
-        <v>60</v>
-      </c>
-      <c r="N14" s="46"/>
-      <c r="O14" s="46"/>
-      <c r="P14" s="46"/>
-      <c r="Q14" s="46"/>
-    </row>
-    <row r="15" spans="1:17" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="M15" s="43" t="s">
-        <v>61</v>
-      </c>
-      <c r="N15" s="47">
-        <v>0.187</v>
-      </c>
-      <c r="O15" s="47">
-        <v>7.9000000000000001E-2</v>
-      </c>
-      <c r="P15" s="47">
-        <v>0.126</v>
-      </c>
-      <c r="Q15" s="47">
-        <v>0.60699999999999998</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="M16" s="43" t="s">
-        <v>5</v>
-      </c>
-      <c r="N16" s="44">
-        <v>0.26100000000000001</v>
-      </c>
-      <c r="O16" s="44">
-        <v>0.39100000000000001</v>
-      </c>
-      <c r="P16" s="44">
-        <v>0.13900000000000001</v>
-      </c>
-      <c r="Q16" s="44">
-        <v>0.20899999999999999</v>
-      </c>
-    </row>
-    <row r="17" spans="13:17" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="M17" s="43" t="s">
-        <v>62</v>
-      </c>
-      <c r="N17" s="47">
-        <v>0.32</v>
-      </c>
-      <c r="O17" s="47">
-        <v>0.52</v>
-      </c>
-      <c r="P17" s="47">
-        <v>0.04</v>
-      </c>
-      <c r="Q17" s="47">
-        <v>0.12</v>
-      </c>
-    </row>
-    <row r="18" spans="13:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="M18" s="43" t="s">
+      <c r="K18">
+        <v>0.25751070137627319</v>
+      </c>
+      <c r="M18" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="N18" s="44">
-        <f t="shared" ref="N18:P18" si="5">SUM(N9:N17)</f>
+      <c r="N18" s="33">
+        <f t="shared" ref="N18:P18" si="6">SUM(N9:N17)</f>
         <v>1.8220000000000003</v>
       </c>
-      <c r="O18" s="44">
-        <f t="shared" si="5"/>
+      <c r="O18" s="33">
+        <f t="shared" si="6"/>
         <v>2.1689999999999996</v>
       </c>
-      <c r="P18" s="44">
-        <f t="shared" si="5"/>
+      <c r="P18" s="33">
+        <f t="shared" si="6"/>
         <v>1.772</v>
       </c>
-      <c r="Q18" s="44">
+      <c r="Q18" s="33">
         <f>SUM(Q9:Q17)</f>
         <v>2.2370000000000001</v>
       </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" t="s">
+        <v>45</v>
+      </c>
+      <c r="E21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A22" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="25">
+        <v>0.18181818181818199</v>
+      </c>
+      <c r="C22" s="25">
+        <v>0.20661157024793389</v>
+      </c>
+      <c r="D22" s="25">
+        <v>0.26446280991735538</v>
+      </c>
+      <c r="E22" s="25">
+        <v>0.34710743801652894</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A23" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" s="25">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="C23" s="25">
+        <v>0.1875</v>
+      </c>
+      <c r="D23" s="25">
+        <v>0.38750000000000001</v>
+      </c>
+      <c r="E23" s="25">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A24" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" s="25">
+        <v>0.12121212121212122</v>
+      </c>
+      <c r="C24" s="25">
+        <v>0.21212121212121213</v>
+      </c>
+      <c r="D24" s="25">
+        <v>0.27272727272727271</v>
+      </c>
+      <c r="E24" s="25">
+        <v>0.39393939393939392</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>0.25</v>
+      </c>
+      <c r="C25">
+        <v>0.25</v>
+      </c>
+      <c r="D25">
+        <v>0.25</v>
+      </c>
+      <c r="E25">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>0.25</v>
+      </c>
+      <c r="C26">
+        <v>0.25</v>
+      </c>
+      <c r="D26">
+        <v>0.25</v>
+      </c>
+      <c r="E26">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A27" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27" s="25">
+        <v>0.33098591549295775</v>
+      </c>
+      <c r="C27" s="25">
+        <v>0.23943661971830985</v>
+      </c>
+      <c r="D27" s="25">
+        <v>0.40140845070422537</v>
+      </c>
+      <c r="E27" s="25">
+        <v>2.8169014084507043E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A28" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28" s="25">
+        <v>0.19069767441860466</v>
+      </c>
+      <c r="C28" s="25">
+        <v>7.9069767441860464E-2</v>
+      </c>
+      <c r="D28" s="25">
+        <v>0.12558139534883722</v>
+      </c>
+      <c r="E28" s="25">
+        <v>0.60465116279069764</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A29" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29" s="25">
+        <v>0.39285714285714285</v>
+      </c>
+      <c r="C29" s="25">
+        <v>0.4642857142857143</v>
+      </c>
+      <c r="D29" s="25">
+        <v>3.5714285714285712E-2</v>
+      </c>
+      <c r="E29" s="25">
+        <v>0.10714285714285714</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A30" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30" s="25">
+        <v>0.19047619047619047</v>
+      </c>
+      <c r="C30" s="25">
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="D30" s="25">
+        <v>0.15238095238095239</v>
+      </c>
+      <c r="E30" s="25">
+        <v>0.22857142857142856</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B31" s="54">
+        <f>SUM(B22:B30)/9</f>
+        <v>0.23144969180835545</v>
+      </c>
+      <c r="C31" s="54">
+        <f t="shared" ref="C31:E31" si="7">SUM(C22:C30)/9</f>
+        <v>0.25751070137627319</v>
+      </c>
+      <c r="D31" s="54">
+        <f t="shared" si="7"/>
+        <v>0.23775279631032545</v>
+      </c>
+      <c r="E31" s="54">
+        <f t="shared" si="7"/>
+        <v>0.27328681050504594</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B32" s="25"/>
+      <c r="C32" s="25"/>
+      <c r="D32" s="25"/>
+      <c r="E32" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4461,25 +4824,25 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" customWidth="1"/>
-    <col min="3" max="3" width="16.109375" customWidth="1"/>
-    <col min="4" max="4" width="22.6640625" customWidth="1"/>
-    <col min="5" max="6" width="19.6640625" customWidth="1"/>
-    <col min="7" max="7" width="25.6640625" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" customWidth="1"/>
+    <col min="5" max="6" width="19.7109375" customWidth="1"/>
+    <col min="7" max="7" width="25.7109375" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>36</v>
       </c>
@@ -4508,13 +4871,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B2">
         <f>Table1[[#This Row],[Initialising]]+Table13[[#This Row],[Initialising]]+Table134[[#This Row],[Initialising]]+Table1345[[#This Row],[Initialising]]</f>
-        <v>9.75</v>
+        <v>7.75</v>
       </c>
       <c r="C2">
         <f>Table1[[#This Row],[Discover and understand the details of the problem]]+Table13[[#This Row],[Discover and understand the details of the problem]]+Table134[[#This Row],[Discover and understand the details of the problem]]+Table1345[[#This Row],[Discover and understand the details of the problem]]</f>
@@ -4534,7 +4897,7 @@
       </c>
       <c r="G2">
         <f>Table1[[#This Row],[Monitoring and Controlling]]+Table13[[#This Row],[Monitoring and Controlling]]+Table134[[#This Row],[Monitoring and Controlling]]+Table1345[[#This Row],[Monitoring and Controlling]]</f>
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="H2">
         <f>Table1[[#This Row],[Deploy]]+Table13[[#This Row],[Deploy]]+Table134[[#This Row],[Deploy]]+Table1345[[#This Row],[Deploy]]</f>
@@ -4542,16 +4905,16 @@
       </c>
       <c r="I2">
         <f>SUM(B2:H2)</f>
-        <v>13.75</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B3">
         <f>Table1[[#This Row],[Initialising]]+Table13[[#This Row],[Initialising]]+Table134[[#This Row],[Initialising]]+Table1345[[#This Row],[Initialising]]</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C3">
         <f>Table1[[#This Row],[Discover and understand the details of the problem]]+Table13[[#This Row],[Discover and understand the details of the problem]]+Table134[[#This Row],[Discover and understand the details of the problem]]+Table1345[[#This Row],[Discover and understand the details of the problem]]</f>
@@ -4571,7 +4934,7 @@
       </c>
       <c r="G3">
         <f>Table1[[#This Row],[Monitoring and Controlling]]+Table13[[#This Row],[Monitoring and Controlling]]+Table134[[#This Row],[Monitoring and Controlling]]+Table1345[[#This Row],[Monitoring and Controlling]]</f>
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="H3">
         <f>Table1[[#This Row],[Deploy]]+Table13[[#This Row],[Deploy]]+Table134[[#This Row],[Deploy]]+Table1345[[#This Row],[Deploy]]</f>
@@ -4579,10 +4942,10 @@
       </c>
       <c r="I3">
         <f t="shared" ref="I3:I14" si="0">SUM(B3:H3)</f>
-        <v>21.75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -4592,11 +4955,11 @@
       </c>
       <c r="C4">
         <f>Table1[[#This Row],[Discover and understand the details of the problem]]+Table13[[#This Row],[Discover and understand the details of the problem]]+Table134[[#This Row],[Discover and understand the details of the problem]]+Table1345[[#This Row],[Discover and understand the details of the problem]]</f>
-        <v>4.5</v>
+        <v>6</v>
       </c>
       <c r="D4">
         <f>Table1[[#This Row],[Create the project plan.]]+Table13[[#This Row],[Create the project plan.]]+Table134[[#This Row],[Create the project plan.]]+Table1345[[#This Row],[Create the project plan.]]</f>
-        <v>16.5</v>
+        <v>15</v>
       </c>
       <c r="E4">
         <f>Table1[[#This Row],[Design Components]]+Table13[[#This Row],[Design Components]]+Table134[[#This Row],[Design Components]]+Table1345[[#This Row],[Design Components]]</f>
@@ -4608,7 +4971,7 @@
       </c>
       <c r="G4">
         <f>Table1[[#This Row],[Monitoring and Controlling]]+Table13[[#This Row],[Monitoring and Controlling]]+Table134[[#This Row],[Monitoring and Controlling]]+Table1345[[#This Row],[Monitoring and Controlling]]</f>
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="H4">
         <f>Table1[[#This Row],[Deploy]]+Table13[[#This Row],[Deploy]]+Table134[[#This Row],[Deploy]]+Table1345[[#This Row],[Deploy]]</f>
@@ -4616,10 +4979,10 @@
       </c>
       <c r="I4">
         <f t="shared" si="0"/>
-        <v>24.25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
@@ -4645,7 +5008,7 @@
       </c>
       <c r="G5">
         <f>Table1[[#This Row],[Monitoring and Controlling]]+Table13[[#This Row],[Monitoring and Controlling]]+Table134[[#This Row],[Monitoring and Controlling]]+Table1345[[#This Row],[Monitoring and Controlling]]</f>
-        <v>4.25</v>
+        <v>4.5</v>
       </c>
       <c r="H5">
         <f>Table1[[#This Row],[Deploy]]+Table13[[#This Row],[Deploy]]+Table134[[#This Row],[Deploy]]+Table1345[[#This Row],[Deploy]]</f>
@@ -4653,10 +5016,10 @@
       </c>
       <c r="I5">
         <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+        <v>25.25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
@@ -4682,7 +5045,7 @@
       </c>
       <c r="G6">
         <f>Table1[[#This Row],[Monitoring and Controlling]]+Table13[[#This Row],[Monitoring and Controlling]]+Table134[[#This Row],[Monitoring and Controlling]]+Table1345[[#This Row],[Monitoring and Controlling]]</f>
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="H6">
         <f>Table1[[#This Row],[Deploy]]+Table13[[#This Row],[Deploy]]+Table134[[#This Row],[Deploy]]+Table1345[[#This Row],[Deploy]]</f>
@@ -4690,10 +5053,10 @@
       </c>
       <c r="I6">
         <f t="shared" si="0"/>
-        <v>22.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+        <v>22.75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -4719,7 +5082,7 @@
       </c>
       <c r="G7">
         <f>Table1[[#This Row],[Monitoring and Controlling]]+Table13[[#This Row],[Monitoring and Controlling]]+Table134[[#This Row],[Monitoring and Controlling]]+Table1345[[#This Row],[Monitoring and Controlling]]</f>
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="H7">
         <f>Table1[[#This Row],[Deploy]]+Table13[[#This Row],[Deploy]]+Table134[[#This Row],[Deploy]]+Table1345[[#This Row],[Deploy]]</f>
@@ -4727,10 +5090,10 @@
       </c>
       <c r="I7">
         <f t="shared" si="0"/>
-        <v>17.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+        <v>17.75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -4756,7 +5119,7 @@
       </c>
       <c r="G8">
         <f>Table1[[#This Row],[Monitoring and Controlling]]+Table13[[#This Row],[Monitoring and Controlling]]+Table134[[#This Row],[Monitoring and Controlling]]+Table1345[[#This Row],[Monitoring and Controlling]]</f>
-        <v>1.75</v>
+        <v>2</v>
       </c>
       <c r="H8">
         <f>Table1[[#This Row],[Deploy]]+Table13[[#This Row],[Deploy]]+Table134[[#This Row],[Deploy]]+Table1345[[#This Row],[Deploy]]</f>
@@ -4764,10 +5127,10 @@
       </c>
       <c r="I8">
         <f t="shared" si="0"/>
-        <v>36.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+        <v>36.75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -4785,7 +5148,7 @@
       </c>
       <c r="E9">
         <f>Table1[[#This Row],[Design Components]]+Table13[[#This Row],[Design Components]]+Table134[[#This Row],[Design Components]]+Table1345[[#This Row],[Design Components]]</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F9">
         <f>Table1[[#This Row],[Implement and Test]]+Table13[[#This Row],[Implement and Test]]+Table134[[#This Row],[Implement and Test]]+Table1345[[#This Row],[Implement and Test]]</f>
@@ -4793,7 +5156,7 @@
       </c>
       <c r="G9">
         <f>Table1[[#This Row],[Monitoring and Controlling]]+Table13[[#This Row],[Monitoring and Controlling]]+Table134[[#This Row],[Monitoring and Controlling]]+Table1345[[#This Row],[Monitoring and Controlling]]</f>
-        <v>1.75</v>
+        <v>2</v>
       </c>
       <c r="H9">
         <f>Table1[[#This Row],[Deploy]]+Table13[[#This Row],[Deploy]]+Table134[[#This Row],[Deploy]]+Table1345[[#This Row],[Deploy]]</f>
@@ -4801,10 +5164,10 @@
       </c>
       <c r="I9">
         <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+        <v>30.25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
@@ -4826,11 +5189,11 @@
       </c>
       <c r="F10">
         <f>Table1[[#This Row],[Implement and Test]]+Table13[[#This Row],[Implement and Test]]+Table134[[#This Row],[Implement and Test]]+Table1345[[#This Row],[Implement and Test]]</f>
-        <v>11.5</v>
+        <v>12</v>
       </c>
       <c r="G10">
         <f>Table1[[#This Row],[Monitoring and Controlling]]+Table13[[#This Row],[Monitoring and Controlling]]+Table134[[#This Row],[Monitoring and Controlling]]+Table1345[[#This Row],[Monitoring and Controlling]]</f>
-        <v>1.75</v>
+        <v>2</v>
       </c>
       <c r="H10">
         <f>Table1[[#This Row],[Deploy]]+Table13[[#This Row],[Deploy]]+Table134[[#This Row],[Deploy]]+Table1345[[#This Row],[Deploy]]</f>
@@ -4838,10 +5201,10 @@
       </c>
       <c r="I10">
         <f t="shared" si="0"/>
-        <v>28.5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+        <v>29.25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
@@ -4867,7 +5230,7 @@
       </c>
       <c r="G11">
         <f>Table1[[#This Row],[Monitoring and Controlling]]+Table13[[#This Row],[Monitoring and Controlling]]+Table134[[#This Row],[Monitoring and Controlling]]+Table1345[[#This Row],[Monitoring and Controlling]]</f>
-        <v>1.25</v>
+        <v>1.5</v>
       </c>
       <c r="H11">
         <f>Table1[[#This Row],[Deploy]]+Table13[[#This Row],[Deploy]]+Table134[[#This Row],[Deploy]]+Table1345[[#This Row],[Deploy]]</f>
@@ -4875,10 +5238,10 @@
       </c>
       <c r="I11">
         <f t="shared" si="0"/>
-        <v>28.5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+        <v>28.75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
@@ -4904,7 +5267,7 @@
       </c>
       <c r="G12">
         <f>Table1[[#This Row],[Monitoring and Controlling]]+Table13[[#This Row],[Monitoring and Controlling]]+Table134[[#This Row],[Monitoring and Controlling]]+Table1345[[#This Row],[Monitoring and Controlling]]</f>
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="H12">
         <f>Table1[[#This Row],[Deploy]]+Table13[[#This Row],[Deploy]]+Table134[[#This Row],[Deploy]]+Table1345[[#This Row],[Deploy]]</f>
@@ -4912,10 +5275,10 @@
       </c>
       <c r="I12">
         <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+        <v>23.75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
@@ -4941,7 +5304,7 @@
       </c>
       <c r="G13">
         <f>Table1[[#This Row],[Monitoring and Controlling]]+Table13[[#This Row],[Monitoring and Controlling]]+Table134[[#This Row],[Monitoring and Controlling]]+Table1345[[#This Row],[Monitoring and Controlling]]</f>
-        <v>5.5</v>
+        <v>5.75</v>
       </c>
       <c r="H13">
         <f>Table1[[#This Row],[Deploy]]+Table13[[#This Row],[Deploy]]+Table134[[#This Row],[Deploy]]+Table1345[[#This Row],[Deploy]]</f>
@@ -4949,10 +5312,10 @@
       </c>
       <c r="I13">
         <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+        <v>27.25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
@@ -4978,7 +5341,7 @@
       </c>
       <c r="G14">
         <f>Table1[[#This Row],[Monitoring and Controlling]]+Table13[[#This Row],[Monitoring and Controlling]]+Table134[[#This Row],[Monitoring and Controlling]]+Table1345[[#This Row],[Monitoring and Controlling]]</f>
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="H14">
         <f>Table1[[#This Row],[Deploy]]+Table13[[#This Row],[Deploy]]+Table134[[#This Row],[Deploy]]+Table1345[[#This Row],[Deploy]]</f>
@@ -4986,10 +5349,10 @@
       </c>
       <c r="I14">
         <f t="shared" si="0"/>
-        <v>18.5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>18.75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>41</v>
       </c>
@@ -5015,56 +5378,56 @@
       </c>
       <c r="G15">
         <f>Table1[[#This Row],[Monitoring and Controlling]]+Table13[[#This Row],[Monitoring and Controlling]]+Table134[[#This Row],[Monitoring and Controlling]]+Table1345[[#This Row],[Monitoring and Controlling]]</f>
-        <v>4</v>
+        <v>4.25</v>
       </c>
       <c r="H15">
         <f>Table1[[#This Row],[Deploy]]+Table13[[#This Row],[Deploy]]+Table134[[#This Row],[Deploy]]+Table1345[[#This Row],[Deploy]]</f>
-        <v>15.25</v>
+        <v>12.75</v>
       </c>
       <c r="I15">
         <f t="shared" ref="I15" si="1">SUM(B15:H15)</f>
-        <v>19.25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B16" s="1">
         <f>SUM(B2:B15)</f>
-        <v>29.25</v>
+        <v>30.25</v>
       </c>
       <c r="C16" s="1">
         <f t="shared" ref="C16:H16" si="2">SUM(C2:C15)</f>
-        <v>31.5</v>
+        <v>33</v>
       </c>
       <c r="D16" s="1">
         <f t="shared" si="2"/>
-        <v>41.5</v>
+        <v>40</v>
       </c>
       <c r="E16" s="1">
         <f t="shared" si="2"/>
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F16" s="1">
         <f t="shared" si="2"/>
-        <v>107</v>
+        <v>107.5</v>
       </c>
       <c r="G16" s="1">
         <f t="shared" si="2"/>
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H16" s="1">
         <f t="shared" si="2"/>
-        <v>31.75</v>
+        <v>29.25</v>
       </c>
       <c r="I16" s="1">
         <f>SUM(I2:I15)</f>
-        <v>336</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>15</v>
       </c>
@@ -5090,7 +5453,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="15"/>
       <c r="B22" s="15"/>
     </row>
@@ -5104,30 +5467,31 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:Q44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.6640625" customWidth="1"/>
-    <col min="2" max="2" width="22.44140625" customWidth="1"/>
-    <col min="4" max="4" width="18.6640625" customWidth="1"/>
-    <col min="5" max="5" width="13.5546875" customWidth="1"/>
-    <col min="6" max="6" width="14.6640625" customWidth="1"/>
-    <col min="7" max="7" width="17.5546875" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" customWidth="1"/>
-    <col min="12" max="12" width="32.6640625" customWidth="1"/>
-    <col min="14" max="14" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" customWidth="1"/>
+    <col min="7" max="7" width="17.5703125" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" customWidth="1"/>
+    <col min="12" max="12" width="32.7109375" customWidth="1"/>
+    <col min="14" max="14" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
@@ -5177,7 +5541,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -5186,11 +5550,11 @@
       </c>
       <c r="C2" s="7">
         <f>'Total Hrs'!B16</f>
-        <v>29.25</v>
+        <v>30.25</v>
       </c>
       <c r="D2" s="10">
         <f>I2*D16</f>
-        <v>1118.95</v>
+        <v>1167.5999999999999</v>
       </c>
       <c r="E2" s="10">
         <v>0</v>
@@ -5208,7 +5572,7 @@
       </c>
       <c r="I2">
         <f>C2-H2</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K2" s="6">
         <v>1</v>
@@ -5232,7 +5596,7 @@
         <v>3403.2</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="11">
         <v>2</v>
       </c>
@@ -5241,11 +5605,11 @@
       </c>
       <c r="C3" s="12">
         <f>'Total Hrs'!C16</f>
-        <v>31.5</v>
+        <v>33</v>
       </c>
       <c r="D3" s="14">
         <f>I3*D16</f>
-        <v>1191.925</v>
+        <v>1264.8999999999999</v>
       </c>
       <c r="E3" s="14">
         <v>0</v>
@@ -5263,7 +5627,7 @@
       </c>
       <c r="I3">
         <f t="shared" ref="I3:I8" si="1">C3-H3</f>
-        <v>24.5</v>
+        <v>26</v>
       </c>
       <c r="K3" s="11">
         <v>2</v>
@@ -5287,7 +5651,7 @@
         <v>4537.6000000000004</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -5296,11 +5660,11 @@
       </c>
       <c r="C4" s="7">
         <f>'Total Hrs'!D16</f>
-        <v>41.5</v>
+        <v>40</v>
       </c>
       <c r="D4" s="10">
         <f>I4*D16</f>
-        <v>1654.1</v>
+        <v>1581.125</v>
       </c>
       <c r="E4" s="10">
         <v>0</v>
@@ -5318,7 +5682,7 @@
       </c>
       <c r="I4">
         <f t="shared" si="1"/>
-        <v>34</v>
+        <v>32.5</v>
       </c>
       <c r="K4" s="6">
         <v>3</v>
@@ -5342,7 +5706,7 @@
         <v>7260.16</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="11">
         <v>4</v>
       </c>
@@ -5396,7 +5760,7 @@
         <v>1680</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <v>5</v>
       </c>
@@ -5405,14 +5769,14 @@
       </c>
       <c r="C6" s="7">
         <f>'Total Hrs'!F16</f>
-        <v>107</v>
+        <v>107.5</v>
       </c>
       <c r="D6" s="10">
         <v>0</v>
       </c>
       <c r="E6" s="10">
         <f>I6*E16</f>
-        <v>3447.5</v>
+        <v>3465</v>
       </c>
       <c r="F6" s="10">
         <f t="shared" si="0"/>
@@ -5427,7 +5791,7 @@
       </c>
       <c r="I6">
         <f t="shared" si="1"/>
-        <v>98.5</v>
+        <v>99</v>
       </c>
       <c r="K6" s="6">
         <v>5</v>
@@ -5451,7 +5815,7 @@
         <v>25200</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="11">
         <v>6</v>
       </c>
@@ -5460,11 +5824,11 @@
       </c>
       <c r="C7" s="12">
         <f>'Total Hrs'!G16</f>
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D7" s="14">
         <f>I7*D16</f>
-        <v>583.79999999999995</v>
+        <v>729.75</v>
       </c>
       <c r="E7" s="14">
         <v>0</v>
@@ -5482,7 +5846,7 @@
       </c>
       <c r="I7">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="K7" s="11">
         <v>6</v>
@@ -5506,7 +5870,7 @@
         <v>4764.4799999999996</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <v>7</v>
       </c>
@@ -5515,11 +5879,11 @@
       </c>
       <c r="C8" s="7">
         <f>'Total Hrs'!H16</f>
-        <v>31.75</v>
+        <v>29.25</v>
       </c>
       <c r="D8" s="10">
         <f>I8*D16</f>
-        <v>997.32499999999993</v>
+        <v>875.69999999999993</v>
       </c>
       <c r="E8" s="10">
         <v>0</v>
@@ -5537,7 +5901,7 @@
       </c>
       <c r="I8">
         <f t="shared" si="1"/>
-        <v>20.5</v>
+        <v>18</v>
       </c>
       <c r="K8" s="6">
         <v>7</v>
@@ -5561,22 +5925,22 @@
         <v>8394.56</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="25" t="s">
+    <row r="9" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="26"/>
+      <c r="B9" s="46"/>
       <c r="C9" s="13">
         <f>SUM(C2:C8)</f>
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="D9" s="16">
         <f>SUM(D2:D8)</f>
-        <v>5546.0999999999995</v>
+        <v>5619.0749999999998</v>
       </c>
       <c r="E9" s="16">
         <f>SUM(E2:E8)</f>
-        <v>5302.5</v>
+        <v>5320</v>
       </c>
       <c r="F9" s="16">
         <f>SUM(F2:F8)</f>
@@ -5584,12 +5948,12 @@
       </c>
       <c r="G9" s="16">
         <f>SUM(D9:F9)</f>
-        <v>16554.165000000001</v>
-      </c>
-      <c r="K9" s="25" t="s">
+        <v>16644.64</v>
+      </c>
+      <c r="K9" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="L9" s="26"/>
+      <c r="L9" s="46"/>
       <c r="M9" s="13">
         <v>377</v>
       </c>
@@ -5606,124 +5970,124 @@
         <v>66916</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="27" t="s">
+    <row r="10" spans="1:17" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="28"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="29"/>
+      <c r="B10" s="48"/>
+      <c r="C10" s="48"/>
+      <c r="D10" s="48"/>
+      <c r="E10" s="48"/>
+      <c r="F10" s="48"/>
+      <c r="G10" s="49"/>
       <c r="H10">
         <v>3400</v>
       </c>
       <c r="I10" s="9">
         <f>G9+H10</f>
-        <v>19954.165000000001</v>
-      </c>
-      <c r="K10" s="27" t="s">
+        <v>20044.64</v>
+      </c>
+      <c r="K10" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="L10" s="28"/>
-      <c r="M10" s="28"/>
-      <c r="N10" s="28"/>
-      <c r="O10" s="28"/>
-      <c r="P10" s="28"/>
-      <c r="Q10" s="29"/>
-    </row>
-    <row r="11" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="30" t="s">
+      <c r="L10" s="48"/>
+      <c r="M10" s="48"/>
+      <c r="N10" s="48"/>
+      <c r="O10" s="48"/>
+      <c r="P10" s="48"/>
+      <c r="Q10" s="49"/>
+    </row>
+    <row r="11" spans="1:17" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="31"/>
-      <c r="C11" s="31"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="31"/>
-      <c r="F11" s="31"/>
-      <c r="G11" s="32"/>
+      <c r="B11" s="51"/>
+      <c r="C11" s="51"/>
+      <c r="D11" s="51"/>
+      <c r="E11" s="51"/>
+      <c r="F11" s="51"/>
+      <c r="G11" s="52"/>
       <c r="I11" s="9">
         <f>O22-I10</f>
-        <v>174.83499999999913</v>
-      </c>
-      <c r="K11" s="30" t="s">
+        <v>84.360000000000582</v>
+      </c>
+      <c r="K11" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="L11" s="31"/>
-      <c r="M11" s="31"/>
-      <c r="N11" s="31"/>
-      <c r="O11" s="31"/>
-      <c r="P11" s="31"/>
-      <c r="Q11" s="32"/>
-    </row>
-    <row r="12" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="30" t="s">
+      <c r="L11" s="51"/>
+      <c r="M11" s="51"/>
+      <c r="N11" s="51"/>
+      <c r="O11" s="51"/>
+      <c r="P11" s="51"/>
+      <c r="Q11" s="52"/>
+    </row>
+    <row r="12" spans="1:17" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="50" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="31"/>
-      <c r="C12" s="31"/>
-      <c r="D12" s="31"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="31"/>
-      <c r="G12" s="32"/>
-      <c r="K12" s="30" t="s">
+      <c r="B12" s="51"/>
+      <c r="C12" s="51"/>
+      <c r="D12" s="51"/>
+      <c r="E12" s="51"/>
+      <c r="F12" s="51"/>
+      <c r="G12" s="52"/>
+      <c r="K12" s="50" t="s">
         <v>33</v>
       </c>
-      <c r="L12" s="31"/>
-      <c r="M12" s="31"/>
-      <c r="N12" s="31"/>
-      <c r="O12" s="31"/>
-      <c r="P12" s="31"/>
-      <c r="Q12" s="32"/>
-    </row>
-    <row r="13" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="30" t="s">
+      <c r="L12" s="51"/>
+      <c r="M12" s="51"/>
+      <c r="N12" s="51"/>
+      <c r="O12" s="51"/>
+      <c r="P12" s="51"/>
+      <c r="Q12" s="52"/>
+    </row>
+    <row r="13" spans="1:17" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="50" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="31"/>
-      <c r="C13" s="31"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="31"/>
-      <c r="G13" s="32"/>
-      <c r="K13" s="30" t="s">
+      <c r="B13" s="51"/>
+      <c r="C13" s="51"/>
+      <c r="D13" s="51"/>
+      <c r="E13" s="51"/>
+      <c r="F13" s="51"/>
+      <c r="G13" s="52"/>
+      <c r="K13" s="50" t="s">
         <v>34</v>
       </c>
-      <c r="L13" s="31"/>
-      <c r="M13" s="31"/>
-      <c r="N13" s="31"/>
-      <c r="O13" s="31"/>
-      <c r="P13" s="31"/>
-      <c r="Q13" s="32"/>
-    </row>
-    <row r="14" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="22" t="s">
+      <c r="L13" s="51"/>
+      <c r="M13" s="51"/>
+      <c r="N13" s="51"/>
+      <c r="O13" s="51"/>
+      <c r="P13" s="51"/>
+      <c r="Q13" s="52"/>
+    </row>
+    <row r="14" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="23"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="24"/>
-      <c r="K14" s="22" t="s">
+      <c r="B14" s="43"/>
+      <c r="C14" s="43"/>
+      <c r="D14" s="43"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="44"/>
+      <c r="K14" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="L14" s="23"/>
-      <c r="M14" s="23"/>
-      <c r="N14" s="23"/>
-      <c r="O14" s="23"/>
-      <c r="P14" s="23"/>
-      <c r="Q14" s="24"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="L14" s="43"/>
+      <c r="M14" s="43"/>
+      <c r="N14" s="43"/>
+      <c r="O14" s="43"/>
+      <c r="P14" s="43"/>
+      <c r="Q14" s="44"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D15" s="9"/>
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D16">
         <v>48.65</v>
       </c>
@@ -5738,34 +6102,34 @@
         <v>377</v>
       </c>
     </row>
-    <row r="17" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="4:15" x14ac:dyDescent="0.25">
       <c r="M17">
         <f>M9-M16</f>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="4:15" x14ac:dyDescent="0.25">
       <c r="N19" s="9">
         <f>3400+G9</f>
-        <v>19954.165000000001</v>
-      </c>
-    </row>
-    <row r="20" spans="4:15" x14ac:dyDescent="0.3">
+        <v>20044.64</v>
+      </c>
+    </row>
+    <row r="20" spans="4:15" x14ac:dyDescent="0.25">
       <c r="G20" s="9"/>
       <c r="O20" s="9">
         <f>Q9/4</f>
         <v>16729</v>
       </c>
     </row>
-    <row r="21" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="21" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D21" s="20">
-        <v>16451.79</v>
+        <v>16644.64</v>
       </c>
       <c r="O21" s="18">
         <v>3400</v>
       </c>
     </row>
-    <row r="22" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="22" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D22" s="9">
         <v>3400</v>
       </c>
@@ -5774,22 +6138,163 @@
         <v>20129</v>
       </c>
     </row>
-    <row r="23" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="23" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D23" s="9">
         <f>D21+D22</f>
-        <v>19851.79</v>
-      </c>
-    </row>
-    <row r="25" spans="4:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="26" spans="4:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>20044.64</v>
+      </c>
+    </row>
+    <row r="25" spans="4:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="4:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D26" s="21">
         <v>20129</v>
       </c>
     </row>
-    <row r="27" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="27" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D27" s="9">
         <f>D26-D23</f>
-        <v>277.20999999999913</v>
+        <v>84.360000000000582</v>
+      </c>
+    </row>
+    <row r="29" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D29" s="53">
+        <v>84.360000000000582</v>
+      </c>
+    </row>
+    <row r="37" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D37">
+        <v>30.25</v>
+      </c>
+      <c r="E37" s="53">
+        <v>1167.5999999999999</v>
+      </c>
+      <c r="F37" s="53">
+        <v>0</v>
+      </c>
+      <c r="G37" s="53">
+        <v>505.81250000000006</v>
+      </c>
+      <c r="H37" s="53">
+        <v>3403.2</v>
+      </c>
+    </row>
+    <row r="38" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D38">
+        <v>33</v>
+      </c>
+      <c r="E38" s="53">
+        <v>1264.8999999999999</v>
+      </c>
+      <c r="F38" s="53">
+        <v>0</v>
+      </c>
+      <c r="G38" s="53">
+        <v>566.51</v>
+      </c>
+      <c r="H38" s="53">
+        <v>4537.6000000000004</v>
+      </c>
+    </row>
+    <row r="39" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D39">
+        <v>40</v>
+      </c>
+      <c r="E39" s="53">
+        <v>1581.125</v>
+      </c>
+      <c r="F39" s="53">
+        <v>0</v>
+      </c>
+      <c r="G39" s="53">
+        <v>606.97500000000002</v>
+      </c>
+      <c r="H39" s="53">
+        <v>7260.16</v>
+      </c>
+    </row>
+    <row r="40" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D40">
+        <v>70</v>
+      </c>
+      <c r="E40" s="53">
+        <v>0</v>
+      </c>
+      <c r="F40" s="53">
+        <v>1855</v>
+      </c>
+      <c r="G40" s="53">
+        <v>1375.8100000000002</v>
+      </c>
+      <c r="H40" s="53">
+        <v>1680</v>
+      </c>
+    </row>
+    <row r="41" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D41">
+        <v>107.5</v>
+      </c>
+      <c r="E41" s="53">
+        <v>0</v>
+      </c>
+      <c r="F41" s="53">
+        <v>3465</v>
+      </c>
+      <c r="G41" s="53">
+        <v>687.90500000000009</v>
+      </c>
+      <c r="H41" s="53">
+        <v>25200</v>
+      </c>
+    </row>
+    <row r="42" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D42">
+        <v>28</v>
+      </c>
+      <c r="E42" s="53">
+        <v>729.75</v>
+      </c>
+      <c r="F42" s="53">
+        <v>0</v>
+      </c>
+      <c r="G42" s="53">
+        <v>1052.0900000000001</v>
+      </c>
+      <c r="H42" s="53">
+        <v>4764.4799999999996</v>
+      </c>
+    </row>
+    <row r="43" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D43">
+        <v>29.25</v>
+      </c>
+      <c r="E43" s="53">
+        <v>875.69999999999993</v>
+      </c>
+      <c r="F43" s="53">
+        <v>0</v>
+      </c>
+      <c r="G43" s="53">
+        <v>910.46250000000009</v>
+      </c>
+      <c r="H43" s="53">
+        <v>8394.56</v>
+      </c>
+    </row>
+    <row r="44" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D44">
+        <v>338</v>
+      </c>
+      <c r="E44" s="53">
+        <v>5619.0749999999998</v>
+      </c>
+      <c r="F44" s="53">
+        <v>5320</v>
+      </c>
+      <c r="G44" s="53">
+        <v>5705.5650000000005</v>
+      </c>
+      <c r="H44" s="53">
+        <v>16644.64</v>
       </c>
     </row>
   </sheetData>
@@ -5808,20 +6313,21 @@
     <mergeCell ref="K13:Q13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="K2:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="11:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="11:13" x14ac:dyDescent="0.25">
       <c r="K2">
         <f>103/240</f>
         <v>0.42916666666666664</v>

</xml_diff>

<commit_message>
fixed personal costings in costings summary
</commit_message>
<xml_diff>
--- a/Report/Costings summary.xlsx
+++ b/Report/Costings summary.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Documents\GitHub\CSC3600\Report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan2\Documents\GitHub\CSC3600\Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92C32216-CE54-4F47-A76B-7F9806BFBA41}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F4E2958-A1FA-4148-B41D-C3A5F595CF62}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9390" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,10 +22,15 @@
     <sheet name="Sheet1" sheetId="11" r:id="rId7"/>
     <sheet name="Sheet2" sheetId="12" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="179021" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -766,7 +771,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -863,6 +868,8 @@
     <xf numFmtId="10" fontId="3" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -902,17 +909,156 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="15">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
       </font>
     </dxf>
     <dxf>
@@ -1088,13 +1234,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>30.25</c:v>
+                  <c:v>26.75</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>33</c:v>
+                  <c:v>49.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>40</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>70</c:v>
@@ -1103,7 +1249,7 @@
                   <c:v>107.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>28</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>29.25</c:v>
@@ -2044,7 +2190,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:I16" totalsRowShown="0">
   <autoFilter ref="A1:I16" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Column1" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Column1" dataDxfId="14"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Initialising"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Discover and understand the details of the problem"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Create the project plan."/>
@@ -2062,7 +2208,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table13" displayName="Table13" ref="A1:I16" totalsRowShown="0">
   <autoFilter ref="A1:I16" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Column1" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Column1" dataDxfId="13"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Initialising"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Discover and understand the details of the problem"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Create the project plan."/>
@@ -2077,18 +2223,18 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table134" displayName="Table134" ref="A1:I16" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table134" displayName="Table134" ref="A1:I16" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
   <autoFilter ref="A1:I16" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Column1" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Initialising"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Discover and understand the details of the problem"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Create the project plan."/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Design Components"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Implement and Test"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Monitoring and Controlling"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Deploy"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="Weekly Total"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Column1" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Initialising" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Discover and understand the details of the problem" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Create the project plan." dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Design Components" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Implement and Test" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Monitoring and Controlling" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Deploy" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="Weekly Total" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2098,7 +2244,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table1345" displayName="Table1345" ref="A1:I16" totalsRowShown="0">
   <autoFilter ref="A1:I16" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Column1" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Column1" dataDxfId="12"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Initialising"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Discover and understand the details of the problem"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Create the project plan."/>
@@ -2116,7 +2262,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table13456" displayName="Table13456" ref="A1:I16" totalsRowShown="0">
   <autoFilter ref="A1:I16" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Week Number" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Week Number" dataDxfId="11"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Initialising"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Discover and understand the details of the problem"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Create the project plan."/>
@@ -2844,8 +2990,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2895,15 +3041,12 @@
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2">
-        <v>0.5</v>
-      </c>
       <c r="G2">
         <v>0.25</v>
       </c>
       <c r="I2">
         <f>SUM(B2:H2)</f>
-        <v>1.75</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -2911,17 +3054,14 @@
         <v>8</v>
       </c>
       <c r="B3">
-        <v>4</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G3">
-        <v>0.25</v>
+        <v>3.25</v>
       </c>
       <c r="I3">
         <f t="shared" ref="I3:I13" si="0">SUM(B3:H3)</f>
-        <v>6.25</v>
+        <v>4.25</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -2944,10 +3084,10 @@
         <v>10</v>
       </c>
       <c r="D5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G5">
-        <v>0.25</v>
+        <v>1.25</v>
       </c>
       <c r="I5">
         <f t="shared" si="0"/>
@@ -2959,10 +3099,10 @@
         <v>11</v>
       </c>
       <c r="D6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G6">
-        <v>0.25</v>
+        <v>2.25</v>
       </c>
       <c r="I6">
         <f t="shared" si="0"/>
@@ -2973,14 +3113,11 @@
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B7">
+      <c r="E7">
         <v>0.5</v>
       </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
       <c r="G7">
-        <v>0.25</v>
+        <v>1.25</v>
       </c>
       <c r="I7">
         <f t="shared" si="0"/>
@@ -2991,11 +3128,11 @@
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E8">
-        <v>11</v>
+      <c r="C8">
+        <v>10</v>
       </c>
       <c r="G8">
-        <v>0.25</v>
+        <v>1.25</v>
       </c>
       <c r="I8">
         <f t="shared" si="0"/>
@@ -3006,7 +3143,7 @@
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E9">
+      <c r="C9">
         <v>6</v>
       </c>
       <c r="F9">
@@ -3024,7 +3161,7 @@
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E10">
+      <c r="C10">
         <v>3</v>
       </c>
       <c r="F10">
@@ -3122,19 +3259,19 @@
       </c>
       <c r="B16" s="1">
         <f>SUM(B2:B15)</f>
-        <v>5.5</v>
+        <v>2</v>
       </c>
       <c r="C16" s="1">
         <f t="shared" ref="C16:G16" si="1">SUM(C2:C15)</f>
-        <v>4</v>
+        <v>20.5</v>
       </c>
       <c r="D16" s="1">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E16" s="1">
         <f t="shared" si="1"/>
-        <v>23.5</v>
+        <v>3</v>
       </c>
       <c r="F16" s="1">
         <f t="shared" si="1"/>
@@ -3142,7 +3279,7 @@
       </c>
       <c r="G16" s="1">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="H16" s="1">
         <f>SUM(H2:H15)</f>
@@ -3150,7 +3287,7 @@
       </c>
       <c r="I16" s="1">
         <f>SUM(I2:I15)</f>
-        <v>76.5</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -3167,46 +3304,48 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" customWidth="1"/>
-    <col min="3" max="3" width="45.85546875" customWidth="1"/>
-    <col min="4" max="4" width="22.7109375" customWidth="1"/>
-    <col min="5" max="6" width="19.7109375" customWidth="1"/>
-    <col min="7" max="7" width="25.7109375" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="55" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" style="55" customWidth="1"/>
+    <col min="3" max="3" width="45.85546875" style="55" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" style="55" customWidth="1"/>
+    <col min="5" max="6" width="19.7109375" style="55" customWidth="1"/>
+    <col min="7" max="7" width="25.7109375" style="55" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="55"/>
+    <col min="9" max="9" width="13.7109375" style="55" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="55"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="B1" s="55" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="55" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3214,13 +3353,13 @@
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="55">
         <v>3</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="55">
         <v>2.5</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="55">
         <f>SUM(B2:H2)</f>
         <v>5.5</v>
       </c>
@@ -3229,16 +3368,16 @@
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="55">
         <v>1</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="55">
         <v>5</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="55">
         <v>2</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="55">
         <f t="shared" ref="I3:I14" si="0">SUM(B3:H3)</f>
         <v>8</v>
       </c>
@@ -3247,10 +3386,10 @@
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="55">
         <v>9.5</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="55">
         <f t="shared" si="0"/>
         <v>9.5</v>
       </c>
@@ -3259,13 +3398,13 @@
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="55">
         <v>0.5</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="55">
         <v>6</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="55">
         <f t="shared" si="0"/>
         <v>6.5</v>
       </c>
@@ -3274,10 +3413,10 @@
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="55">
         <v>4</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="55">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
@@ -3286,13 +3425,13 @@
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="55">
         <v>0.5</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="55">
         <v>2</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="55">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
@@ -3301,19 +3440,19 @@
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="55">
         <v>1.5</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="55">
         <v>7</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="55">
         <v>3</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="55">
         <v>1</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="55">
         <f t="shared" si="0"/>
         <v>12.5</v>
       </c>
@@ -3322,16 +3461,16 @@
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="55">
         <v>2</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="55">
         <v>4</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="55">
         <v>1</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="55">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
@@ -3340,13 +3479,13 @@
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="55">
         <v>4</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="55">
         <v>2</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="55">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
@@ -3355,13 +3494,13 @@
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="55">
         <v>5</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="55">
         <v>1</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="55">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
@@ -3370,13 +3509,13 @@
       <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="55">
         <v>3.5</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="55">
         <v>0.5</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="55">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
@@ -3385,10 +3524,10 @@
       <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="55">
         <v>4</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="55">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
@@ -3397,10 +3536,10 @@
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="55">
         <v>2.5</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="55">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
@@ -3409,47 +3548,47 @@
       <c r="A15" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="55">
         <v>1.5</v>
       </c>
-      <c r="I15">
+      <c r="I15" s="55">
         <f>SUM(B15:H15)</f>
         <v>1.5</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" s="56">
         <f>SUM(B2:B15)</f>
         <v>8</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" s="56">
         <f t="shared" ref="C16:I16" si="1">SUM(C2:C15)</f>
         <v>9</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D16" s="56">
         <f t="shared" si="1"/>
         <v>15.5</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E16" s="56">
         <f t="shared" si="1"/>
         <v>28.5</v>
       </c>
-      <c r="F16" s="1">
+      <c r="F16" s="56">
         <f t="shared" si="1"/>
         <v>13.5</v>
       </c>
-      <c r="G16" s="1">
+      <c r="G16" s="56">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="H16" s="1">
+      <c r="H16" s="56">
         <f>SUM(H2:H15)</f>
         <v>4</v>
       </c>
-      <c r="I16" s="1">
+      <c r="I16" s="56">
         <f t="shared" si="1"/>
         <v>79.5</v>
       </c>
@@ -3457,8 +3596,9 @@
     <row r="17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -3898,7 +4038,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:Q32"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
@@ -3980,19 +4120,19 @@
       </c>
       <c r="B3">
         <f>Ryan!B16</f>
-        <v>5.5</v>
+        <v>2</v>
       </c>
       <c r="C3">
         <f>Ryan!C16</f>
-        <v>4</v>
+        <v>20.5</v>
       </c>
       <c r="D3">
         <f>Ryan!D16</f>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E3">
         <f>Ryan!E16</f>
-        <v>23.5</v>
+        <v>3</v>
       </c>
       <c r="F3">
         <f>Ryan!F16</f>
@@ -4000,7 +4140,7 @@
       </c>
       <c r="G3">
         <f>Ryan!G16</f>
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="H3">
         <f>Ryan!H16</f>
@@ -4008,7 +4148,7 @@
       </c>
       <c r="I3">
         <f>Ryan!I16</f>
-        <v>76.5</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -4091,19 +4231,19 @@
       </c>
       <c r="B6">
         <f>SUM(B2:B5)</f>
-        <v>30.25</v>
+        <v>26.75</v>
       </c>
       <c r="C6">
         <f t="shared" ref="C6:I6" si="0">SUM(C2:C5)</f>
-        <v>33</v>
+        <v>49.5</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
-        <v>71</v>
+        <v>50.5</v>
       </c>
       <c r="F6">
         <f t="shared" si="0"/>
@@ -4111,7 +4251,7 @@
       </c>
       <c r="G6">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="H6">
         <f t="shared" si="0"/>
@@ -4119,7 +4259,7 @@
       </c>
       <c r="I6">
         <f t="shared" si="0"/>
-        <v>325.5</v>
+        <v>323</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="30" x14ac:dyDescent="0.25">
@@ -4132,7 +4272,7 @@
       <c r="O7" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="P7" s="40" t="s">
+      <c r="P7" s="42" t="s">
         <v>53</v>
       </c>
       <c r="Q7" s="30" t="s">
@@ -4176,7 +4316,7 @@
       <c r="O8" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="P8" s="41"/>
+      <c r="P8" s="43"/>
       <c r="Q8" s="31" t="s">
         <v>55</v>
       </c>
@@ -4187,19 +4327,19 @@
       </c>
       <c r="B9" s="25">
         <f>B2/B$6</f>
-        <v>0.34710743801652894</v>
+        <v>0.3925233644859813</v>
       </c>
       <c r="C9" s="25">
         <f t="shared" ref="C9:H9" si="1">C2/C$6</f>
-        <v>0.39393939393939392</v>
+        <v>0.26262626262626265</v>
       </c>
       <c r="D9" s="25">
         <f t="shared" si="1"/>
-        <v>0.25</v>
+        <v>0.27027027027027029</v>
       </c>
       <c r="E9" s="25">
         <f t="shared" si="1"/>
-        <v>2.8169014084507043E-2</v>
+        <v>3.9603960396039604E-2</v>
       </c>
       <c r="F9" s="25">
         <f t="shared" si="1"/>
@@ -4207,7 +4347,7 @@
       </c>
       <c r="G9" s="25">
         <f t="shared" si="1"/>
-        <v>0.10714285714285714</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="H9" s="25">
         <f t="shared" si="1"/>
@@ -4221,7 +4361,7 @@
       </c>
       <c r="K9" s="25">
         <f>SUM(B9:J9)/9</f>
-        <v>0.27328681050504594</v>
+        <v>0.26461997583044589</v>
       </c>
       <c r="M9" s="32"/>
       <c r="N9" s="37">
@@ -4243,19 +4383,19 @@
       </c>
       <c r="B10" s="25">
         <f t="shared" ref="B10:H10" si="2">B3/B$6</f>
-        <v>0.18181818181818182</v>
+        <v>7.476635514018691E-2</v>
       </c>
       <c r="C10" s="25">
         <f t="shared" si="2"/>
-        <v>0.12121212121212122</v>
+        <v>0.41414141414141414</v>
       </c>
       <c r="D10" s="25">
         <f t="shared" si="2"/>
-        <v>0.17499999999999999</v>
+        <v>0.10810810810810811</v>
       </c>
       <c r="E10" s="25">
         <f t="shared" si="2"/>
-        <v>0.33098591549295775</v>
+        <v>5.9405940594059403E-2</v>
       </c>
       <c r="F10" s="25">
         <f t="shared" si="2"/>
@@ -4263,7 +4403,7 @@
       </c>
       <c r="G10" s="25">
         <f t="shared" si="2"/>
-        <v>0.39285714285714285</v>
+        <v>0.52777777777777779</v>
       </c>
       <c r="H10" s="25">
         <f t="shared" si="2"/>
@@ -4277,7 +4417,7 @@
       </c>
       <c r="K10" s="25">
         <f t="shared" ref="K10:K12" si="3">SUM(B10:J10)/9</f>
-        <v>0.2314496918083554</v>
+        <v>0.22948594007292686</v>
       </c>
       <c r="M10" s="32" t="s">
         <v>56</v>
@@ -4301,19 +4441,19 @@
       </c>
       <c r="B11" s="25">
         <f t="shared" ref="B11:H11" si="4">B4/B$6</f>
-        <v>0.26446280991735538</v>
+        <v>0.29906542056074764</v>
       </c>
       <c r="C11" s="25">
         <f t="shared" si="4"/>
-        <v>0.27272727272727271</v>
+        <v>0.18181818181818182</v>
       </c>
       <c r="D11" s="25">
         <f t="shared" si="4"/>
-        <v>0.38750000000000001</v>
+        <v>0.41891891891891891</v>
       </c>
       <c r="E11" s="25">
         <f t="shared" si="4"/>
-        <v>0.40140845070422537</v>
+        <v>0.5643564356435643</v>
       </c>
       <c r="F11" s="25">
         <f t="shared" si="4"/>
@@ -4321,7 +4461,7 @@
       </c>
       <c r="G11" s="25">
         <f t="shared" si="4"/>
-        <v>3.5714285714285712E-2</v>
+        <v>2.7777777777777776E-2</v>
       </c>
       <c r="H11" s="25">
         <f t="shared" si="4"/>
@@ -4335,7 +4475,7 @@
       </c>
       <c r="K11" s="25">
         <f t="shared" si="3"/>
-        <v>0.23775279631032545</v>
+        <v>0.25221100916099776</v>
       </c>
       <c r="M11" s="32" t="s">
         <v>57</v>
@@ -4359,19 +4499,19 @@
       </c>
       <c r="B12" s="25">
         <f t="shared" ref="B12:H12" si="5">B5/B$6</f>
-        <v>0.20661157024793389</v>
+        <v>0.23364485981308411</v>
       </c>
       <c r="C12" s="25">
         <f t="shared" si="5"/>
-        <v>0.21212121212121213</v>
+        <v>0.14141414141414141</v>
       </c>
       <c r="D12" s="25">
         <f t="shared" si="5"/>
-        <v>0.1875</v>
+        <v>0.20270270270270271</v>
       </c>
       <c r="E12" s="25">
         <f t="shared" si="5"/>
-        <v>0.23943661971830985</v>
+        <v>0.33663366336633666</v>
       </c>
       <c r="F12" s="25">
         <f t="shared" si="5"/>
@@ -4379,7 +4519,7 @@
       </c>
       <c r="G12" s="25">
         <f t="shared" si="5"/>
-        <v>0.4642857142857143</v>
+        <v>0.3611111111111111</v>
       </c>
       <c r="H12" s="25">
         <f t="shared" si="5"/>
@@ -4393,7 +4533,7 @@
       </c>
       <c r="K12" s="25">
         <f t="shared" si="3"/>
-        <v>0.25751070137627319</v>
+        <v>0.25368307493562942</v>
       </c>
       <c r="M12" s="32" t="s">
         <v>58</v>
@@ -4791,19 +4931,19 @@
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B31" s="54">
+      <c r="B31" s="41">
         <f>SUM(B22:B30)/9</f>
         <v>0.23144969180835545</v>
       </c>
-      <c r="C31" s="54">
+      <c r="C31" s="41">
         <f t="shared" ref="C31:E31" si="7">SUM(C22:C30)/9</f>
         <v>0.25751070137627319</v>
       </c>
-      <c r="D31" s="54">
+      <c r="D31" s="41">
         <f t="shared" si="7"/>
         <v>0.23775279631032545</v>
       </c>
-      <c r="E31" s="54">
+      <c r="E31" s="41">
         <f t="shared" si="7"/>
         <v>0.27328681050504594</v>
       </c>
@@ -4828,7 +4968,7 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4881,7 +5021,7 @@
       </c>
       <c r="C2">
         <f>Table1[[#This Row],[Discover and understand the details of the problem]]+Table13[[#This Row],[Discover and understand the details of the problem]]+Table134[[#This Row],[Discover and understand the details of the problem]]+Table1345[[#This Row],[Discover and understand the details of the problem]]</f>
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="D2">
         <f>Table1[[#This Row],[Create the project plan.]]+Table13[[#This Row],[Create the project plan.]]+Table134[[#This Row],[Create the project plan.]]+Table1345[[#This Row],[Create the project plan.]]</f>
@@ -4905,7 +5045,7 @@
       </c>
       <c r="I2">
         <f>SUM(B2:H2)</f>
-        <v>12</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -4914,11 +5054,11 @@
       </c>
       <c r="B3">
         <f>Table1[[#This Row],[Initialising]]+Table13[[#This Row],[Initialising]]+Table134[[#This Row],[Initialising]]+Table1345[[#This Row],[Initialising]]</f>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C3">
         <f>Table1[[#This Row],[Discover and understand the details of the problem]]+Table13[[#This Row],[Discover and understand the details of the problem]]+Table134[[#This Row],[Discover and understand the details of the problem]]+Table1345[[#This Row],[Discover and understand the details of the problem]]</f>
-        <v>5.5</v>
+        <v>3.5</v>
       </c>
       <c r="D3">
         <f>Table1[[#This Row],[Create the project plan.]]+Table13[[#This Row],[Create the project plan.]]+Table134[[#This Row],[Create the project plan.]]+Table1345[[#This Row],[Create the project plan.]]</f>
@@ -4934,7 +5074,7 @@
       </c>
       <c r="G3">
         <f>Table1[[#This Row],[Monitoring and Controlling]]+Table13[[#This Row],[Monitoring and Controlling]]+Table134[[#This Row],[Monitoring and Controlling]]+Table1345[[#This Row],[Monitoring and Controlling]]</f>
-        <v>0.5</v>
+        <v>3.5</v>
       </c>
       <c r="H3">
         <f>Table1[[#This Row],[Deploy]]+Table13[[#This Row],[Deploy]]+Table134[[#This Row],[Deploy]]+Table1345[[#This Row],[Deploy]]</f>
@@ -4942,7 +5082,7 @@
       </c>
       <c r="I3">
         <f t="shared" ref="I3:I14" si="0">SUM(B3:H3)</f>
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -4996,7 +5136,7 @@
       </c>
       <c r="D5">
         <f>Table1[[#This Row],[Create the project plan.]]+Table13[[#This Row],[Create the project plan.]]+Table134[[#This Row],[Create the project plan.]]+Table1345[[#This Row],[Create the project plan.]]</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E5">
         <f>Table1[[#This Row],[Design Components]]+Table13[[#This Row],[Design Components]]+Table134[[#This Row],[Design Components]]+Table1345[[#This Row],[Design Components]]</f>
@@ -5008,7 +5148,7 @@
       </c>
       <c r="G5">
         <f>Table1[[#This Row],[Monitoring and Controlling]]+Table13[[#This Row],[Monitoring and Controlling]]+Table134[[#This Row],[Monitoring and Controlling]]+Table1345[[#This Row],[Monitoring and Controlling]]</f>
-        <v>4.5</v>
+        <v>5.5</v>
       </c>
       <c r="H5">
         <f>Table1[[#This Row],[Deploy]]+Table13[[#This Row],[Deploy]]+Table134[[#This Row],[Deploy]]+Table1345[[#This Row],[Deploy]]</f>
@@ -5033,7 +5173,7 @@
       </c>
       <c r="D6">
         <f>Table1[[#This Row],[Create the project plan.]]+Table13[[#This Row],[Create the project plan.]]+Table134[[#This Row],[Create the project plan.]]+Table1345[[#This Row],[Create the project plan.]]</f>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E6">
         <f>Table1[[#This Row],[Design Components]]+Table13[[#This Row],[Design Components]]+Table134[[#This Row],[Design Components]]+Table1345[[#This Row],[Design Components]]</f>
@@ -5045,7 +5185,7 @@
       </c>
       <c r="G6">
         <f>Table1[[#This Row],[Monitoring and Controlling]]+Table13[[#This Row],[Monitoring and Controlling]]+Table134[[#This Row],[Monitoring and Controlling]]+Table1345[[#This Row],[Monitoring and Controlling]]</f>
-        <v>0.5</v>
+        <v>2.5</v>
       </c>
       <c r="H6">
         <f>Table1[[#This Row],[Deploy]]+Table13[[#This Row],[Deploy]]+Table134[[#This Row],[Deploy]]+Table1345[[#This Row],[Deploy]]</f>
@@ -5062,7 +5202,7 @@
       </c>
       <c r="B7">
         <f>Table1[[#This Row],[Initialising]]+Table13[[#This Row],[Initialising]]+Table134[[#This Row],[Initialising]]+Table1345[[#This Row],[Initialising]]</f>
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="C7">
         <f>Table1[[#This Row],[Discover and understand the details of the problem]]+Table13[[#This Row],[Discover and understand the details of the problem]]+Table134[[#This Row],[Discover and understand the details of the problem]]+Table1345[[#This Row],[Discover and understand the details of the problem]]</f>
@@ -5074,7 +5214,7 @@
       </c>
       <c r="E7">
         <f>Table1[[#This Row],[Design Components]]+Table13[[#This Row],[Design Components]]+Table134[[#This Row],[Design Components]]+Table1345[[#This Row],[Design Components]]</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="F7">
         <f>Table1[[#This Row],[Implement and Test]]+Table13[[#This Row],[Implement and Test]]+Table134[[#This Row],[Implement and Test]]+Table1345[[#This Row],[Implement and Test]]</f>
@@ -5082,7 +5222,7 @@
       </c>
       <c r="G7">
         <f>Table1[[#This Row],[Monitoring and Controlling]]+Table13[[#This Row],[Monitoring and Controlling]]+Table134[[#This Row],[Monitoring and Controlling]]+Table1345[[#This Row],[Monitoring and Controlling]]</f>
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
       <c r="H7">
         <f>Table1[[#This Row],[Deploy]]+Table13[[#This Row],[Deploy]]+Table134[[#This Row],[Deploy]]+Table1345[[#This Row],[Deploy]]</f>
@@ -5103,7 +5243,7 @@
       </c>
       <c r="C8">
         <f>Table1[[#This Row],[Discover and understand the details of the problem]]+Table13[[#This Row],[Discover and understand the details of the problem]]+Table134[[#This Row],[Discover and understand the details of the problem]]+Table1345[[#This Row],[Discover and understand the details of the problem]]</f>
-        <v>4.75</v>
+        <v>14.75</v>
       </c>
       <c r="D8">
         <f>Table1[[#This Row],[Create the project plan.]]+Table13[[#This Row],[Create the project plan.]]+Table134[[#This Row],[Create the project plan.]]+Table1345[[#This Row],[Create the project plan.]]</f>
@@ -5111,7 +5251,7 @@
       </c>
       <c r="E8">
         <f>Table1[[#This Row],[Design Components]]+Table13[[#This Row],[Design Components]]+Table134[[#This Row],[Design Components]]+Table1345[[#This Row],[Design Components]]</f>
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="F8">
         <f>Table1[[#This Row],[Implement and Test]]+Table13[[#This Row],[Implement and Test]]+Table134[[#This Row],[Implement and Test]]+Table1345[[#This Row],[Implement and Test]]</f>
@@ -5119,7 +5259,7 @@
       </c>
       <c r="G8">
         <f>Table1[[#This Row],[Monitoring and Controlling]]+Table13[[#This Row],[Monitoring and Controlling]]+Table134[[#This Row],[Monitoring and Controlling]]+Table1345[[#This Row],[Monitoring and Controlling]]</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H8">
         <f>Table1[[#This Row],[Deploy]]+Table13[[#This Row],[Deploy]]+Table134[[#This Row],[Deploy]]+Table1345[[#This Row],[Deploy]]</f>
@@ -5140,7 +5280,7 @@
       </c>
       <c r="C9">
         <f>Table1[[#This Row],[Discover and understand the details of the problem]]+Table13[[#This Row],[Discover and understand the details of the problem]]+Table134[[#This Row],[Discover and understand the details of the problem]]+Table1345[[#This Row],[Discover and understand the details of the problem]]</f>
-        <v>4.25</v>
+        <v>10.25</v>
       </c>
       <c r="D9">
         <f>Table1[[#This Row],[Create the project plan.]]+Table13[[#This Row],[Create the project plan.]]+Table134[[#This Row],[Create the project plan.]]+Table1345[[#This Row],[Create the project plan.]]</f>
@@ -5148,7 +5288,7 @@
       </c>
       <c r="E9">
         <f>Table1[[#This Row],[Design Components]]+Table13[[#This Row],[Design Components]]+Table134[[#This Row],[Design Components]]+Table1345[[#This Row],[Design Components]]</f>
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F9">
         <f>Table1[[#This Row],[Implement and Test]]+Table13[[#This Row],[Implement and Test]]+Table134[[#This Row],[Implement and Test]]+Table1345[[#This Row],[Implement and Test]]</f>
@@ -5177,7 +5317,7 @@
       </c>
       <c r="C10">
         <f>Table1[[#This Row],[Discover and understand the details of the problem]]+Table13[[#This Row],[Discover and understand the details of the problem]]+Table134[[#This Row],[Discover and understand the details of the problem]]+Table1345[[#This Row],[Discover and understand the details of the problem]]</f>
-        <v>2.25</v>
+        <v>5.25</v>
       </c>
       <c r="D10">
         <f>Table1[[#This Row],[Create the project plan.]]+Table13[[#This Row],[Create the project plan.]]+Table134[[#This Row],[Create the project plan.]]+Table1345[[#This Row],[Create the project plan.]]</f>
@@ -5185,7 +5325,7 @@
       </c>
       <c r="E10">
         <f>Table1[[#This Row],[Design Components]]+Table13[[#This Row],[Design Components]]+Table134[[#This Row],[Design Components]]+Table1345[[#This Row],[Design Components]]</f>
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F10">
         <f>Table1[[#This Row],[Implement and Test]]+Table13[[#This Row],[Implement and Test]]+Table134[[#This Row],[Implement and Test]]+Table1345[[#This Row],[Implement and Test]]</f>
@@ -5395,19 +5535,19 @@
       </c>
       <c r="B16" s="1">
         <f>SUM(B2:B15)</f>
-        <v>30.25</v>
+        <v>26.75</v>
       </c>
       <c r="C16" s="1">
         <f t="shared" ref="C16:H16" si="2">SUM(C2:C15)</f>
-        <v>33</v>
+        <v>49.5</v>
       </c>
       <c r="D16" s="1">
         <f t="shared" si="2"/>
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E16" s="1">
         <f t="shared" si="2"/>
-        <v>71</v>
+        <v>50.5</v>
       </c>
       <c r="F16" s="1">
         <f t="shared" si="2"/>
@@ -5415,7 +5555,7 @@
       </c>
       <c r="G16" s="1">
         <f t="shared" si="2"/>
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="H16" s="1">
         <f t="shared" si="2"/>
@@ -5423,7 +5563,7 @@
       </c>
       <c r="I16" s="1">
         <f>SUM(I2:I15)</f>
-        <v>339</v>
+        <v>336.5</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -5550,11 +5690,11 @@
       </c>
       <c r="C2" s="7">
         <f>'Total Hrs'!B16</f>
-        <v>30.25</v>
+        <v>26.75</v>
       </c>
       <c r="D2" s="10">
         <f>I2*D16</f>
-        <v>1167.5999999999999</v>
+        <v>997.32499999999993</v>
       </c>
       <c r="E2" s="10">
         <v>0</v>
@@ -5572,7 +5712,7 @@
       </c>
       <c r="I2">
         <f>C2-H2</f>
-        <v>24</v>
+        <v>20.5</v>
       </c>
       <c r="K2" s="6">
         <v>1</v>
@@ -5605,11 +5745,11 @@
       </c>
       <c r="C3" s="12">
         <f>'Total Hrs'!C16</f>
-        <v>33</v>
+        <v>49.5</v>
       </c>
       <c r="D3" s="14">
         <f>I3*D16</f>
-        <v>1264.8999999999999</v>
+        <v>2067.625</v>
       </c>
       <c r="E3" s="14">
         <v>0</v>
@@ -5627,7 +5767,7 @@
       </c>
       <c r="I3">
         <f t="shared" ref="I3:I8" si="1">C3-H3</f>
-        <v>26</v>
+        <v>42.5</v>
       </c>
       <c r="K3" s="11">
         <v>2</v>
@@ -5660,11 +5800,11 @@
       </c>
       <c r="C4" s="7">
         <f>'Total Hrs'!D16</f>
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D4" s="10">
         <f>I4*D16</f>
-        <v>1581.125</v>
+        <v>1435.175</v>
       </c>
       <c r="E4" s="10">
         <v>0</v>
@@ -5682,7 +5822,7 @@
       </c>
       <c r="I4">
         <f t="shared" si="1"/>
-        <v>32.5</v>
+        <v>29.5</v>
       </c>
       <c r="K4" s="6">
         <v>3</v>
@@ -5824,11 +5964,11 @@
       </c>
       <c r="C7" s="12">
         <f>'Total Hrs'!G16</f>
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="D7" s="14">
         <f>I7*D16</f>
-        <v>729.75</v>
+        <v>1118.95</v>
       </c>
       <c r="E7" s="14">
         <v>0</v>
@@ -5846,7 +5986,7 @@
       </c>
       <c r="I7">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="K7" s="11">
         <v>6</v>
@@ -5926,17 +6066,17 @@
       </c>
     </row>
     <row r="9" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="45" t="s">
+      <c r="A9" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="46"/>
+      <c r="B9" s="48"/>
       <c r="C9" s="13">
         <f>SUM(C2:C8)</f>
-        <v>338</v>
+        <v>356</v>
       </c>
       <c r="D9" s="16">
         <f>SUM(D2:D8)</f>
-        <v>5619.0749999999998</v>
+        <v>6494.7749999999996</v>
       </c>
       <c r="E9" s="16">
         <f>SUM(E2:E8)</f>
@@ -5948,12 +6088,12 @@
       </c>
       <c r="G9" s="16">
         <f>SUM(D9:F9)</f>
-        <v>16644.64</v>
-      </c>
-      <c r="K9" s="45" t="s">
+        <v>17520.34</v>
+      </c>
+      <c r="K9" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="L9" s="46"/>
+      <c r="L9" s="48"/>
       <c r="M9" s="13">
         <v>377</v>
       </c>
@@ -5971,115 +6111,115 @@
       </c>
     </row>
     <row r="10" spans="1:17" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="47" t="s">
+      <c r="A10" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="48"/>
-      <c r="C10" s="48"/>
-      <c r="D10" s="48"/>
-      <c r="E10" s="48"/>
-      <c r="F10" s="48"/>
-      <c r="G10" s="49"/>
+      <c r="B10" s="50"/>
+      <c r="C10" s="50"/>
+      <c r="D10" s="50"/>
+      <c r="E10" s="50"/>
+      <c r="F10" s="50"/>
+      <c r="G10" s="51"/>
       <c r="H10">
         <v>3400</v>
       </c>
       <c r="I10" s="9">
         <f>G9+H10</f>
-        <v>20044.64</v>
-      </c>
-      <c r="K10" s="47" t="s">
+        <v>20920.34</v>
+      </c>
+      <c r="K10" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="L10" s="48"/>
-      <c r="M10" s="48"/>
-      <c r="N10" s="48"/>
-      <c r="O10" s="48"/>
-      <c r="P10" s="48"/>
-      <c r="Q10" s="49"/>
+      <c r="L10" s="50"/>
+      <c r="M10" s="50"/>
+      <c r="N10" s="50"/>
+      <c r="O10" s="50"/>
+      <c r="P10" s="50"/>
+      <c r="Q10" s="51"/>
     </row>
     <row r="11" spans="1:17" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="50" t="s">
+      <c r="A11" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="51"/>
-      <c r="C11" s="51"/>
-      <c r="D11" s="51"/>
-      <c r="E11" s="51"/>
-      <c r="F11" s="51"/>
-      <c r="G11" s="52"/>
+      <c r="B11" s="53"/>
+      <c r="C11" s="53"/>
+      <c r="D11" s="53"/>
+      <c r="E11" s="53"/>
+      <c r="F11" s="53"/>
+      <c r="G11" s="54"/>
       <c r="I11" s="9">
         <f>O22-I10</f>
-        <v>84.360000000000582</v>
-      </c>
-      <c r="K11" s="50" t="s">
+        <v>-791.34000000000015</v>
+      </c>
+      <c r="K11" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="L11" s="51"/>
-      <c r="M11" s="51"/>
-      <c r="N11" s="51"/>
-      <c r="O11" s="51"/>
-      <c r="P11" s="51"/>
-      <c r="Q11" s="52"/>
+      <c r="L11" s="53"/>
+      <c r="M11" s="53"/>
+      <c r="N11" s="53"/>
+      <c r="O11" s="53"/>
+      <c r="P11" s="53"/>
+      <c r="Q11" s="54"/>
     </row>
     <row r="12" spans="1:17" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="50" t="s">
+      <c r="A12" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="51"/>
-      <c r="C12" s="51"/>
-      <c r="D12" s="51"/>
-      <c r="E12" s="51"/>
-      <c r="F12" s="51"/>
-      <c r="G12" s="52"/>
-      <c r="K12" s="50" t="s">
+      <c r="B12" s="53"/>
+      <c r="C12" s="53"/>
+      <c r="D12" s="53"/>
+      <c r="E12" s="53"/>
+      <c r="F12" s="53"/>
+      <c r="G12" s="54"/>
+      <c r="K12" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="L12" s="51"/>
-      <c r="M12" s="51"/>
-      <c r="N12" s="51"/>
-      <c r="O12" s="51"/>
-      <c r="P12" s="51"/>
-      <c r="Q12" s="52"/>
+      <c r="L12" s="53"/>
+      <c r="M12" s="53"/>
+      <c r="N12" s="53"/>
+      <c r="O12" s="53"/>
+      <c r="P12" s="53"/>
+      <c r="Q12" s="54"/>
     </row>
     <row r="13" spans="1:17" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="50" t="s">
+      <c r="A13" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="51"/>
-      <c r="C13" s="51"/>
-      <c r="D13" s="51"/>
-      <c r="E13" s="51"/>
-      <c r="F13" s="51"/>
-      <c r="G13" s="52"/>
-      <c r="K13" s="50" t="s">
+      <c r="B13" s="53"/>
+      <c r="C13" s="53"/>
+      <c r="D13" s="53"/>
+      <c r="E13" s="53"/>
+      <c r="F13" s="53"/>
+      <c r="G13" s="54"/>
+      <c r="K13" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="L13" s="51"/>
-      <c r="M13" s="51"/>
-      <c r="N13" s="51"/>
-      <c r="O13" s="51"/>
-      <c r="P13" s="51"/>
-      <c r="Q13" s="52"/>
+      <c r="L13" s="53"/>
+      <c r="M13" s="53"/>
+      <c r="N13" s="53"/>
+      <c r="O13" s="53"/>
+      <c r="P13" s="53"/>
+      <c r="Q13" s="54"/>
     </row>
     <row r="14" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="42" t="s">
+      <c r="A14" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="43"/>
-      <c r="C14" s="43"/>
-      <c r="D14" s="43"/>
-      <c r="E14" s="43"/>
-      <c r="F14" s="43"/>
-      <c r="G14" s="44"/>
-      <c r="K14" s="42" t="s">
+      <c r="B14" s="45"/>
+      <c r="C14" s="45"/>
+      <c r="D14" s="45"/>
+      <c r="E14" s="45"/>
+      <c r="F14" s="45"/>
+      <c r="G14" s="46"/>
+      <c r="K14" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="L14" s="43"/>
-      <c r="M14" s="43"/>
-      <c r="N14" s="43"/>
-      <c r="O14" s="43"/>
-      <c r="P14" s="43"/>
-      <c r="Q14" s="44"/>
+      <c r="L14" s="45"/>
+      <c r="M14" s="45"/>
+      <c r="N14" s="45"/>
+      <c r="O14" s="45"/>
+      <c r="P14" s="45"/>
+      <c r="Q14" s="46"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D15" s="9"/>
@@ -6111,7 +6251,7 @@
     <row r="19" spans="4:15" x14ac:dyDescent="0.25">
       <c r="N19" s="9">
         <f>3400+G9</f>
-        <v>20044.64</v>
+        <v>20920.34</v>
       </c>
     </row>
     <row r="20" spans="4:15" x14ac:dyDescent="0.25">
@@ -6157,7 +6297,7 @@
       </c>
     </row>
     <row r="29" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D29" s="53">
+      <c r="D29" s="40">
         <v>84.360000000000582</v>
       </c>
     </row>
@@ -6165,16 +6305,16 @@
       <c r="D37">
         <v>30.25</v>
       </c>
-      <c r="E37" s="53">
+      <c r="E37" s="40">
         <v>1167.5999999999999</v>
       </c>
-      <c r="F37" s="53">
-        <v>0</v>
-      </c>
-      <c r="G37" s="53">
+      <c r="F37" s="40">
+        <v>0</v>
+      </c>
+      <c r="G37" s="40">
         <v>505.81250000000006</v>
       </c>
-      <c r="H37" s="53">
+      <c r="H37" s="40">
         <v>3403.2</v>
       </c>
     </row>
@@ -6182,16 +6322,16 @@
       <c r="D38">
         <v>33</v>
       </c>
-      <c r="E38" s="53">
+      <c r="E38" s="40">
         <v>1264.8999999999999</v>
       </c>
-      <c r="F38" s="53">
-        <v>0</v>
-      </c>
-      <c r="G38" s="53">
+      <c r="F38" s="40">
+        <v>0</v>
+      </c>
+      <c r="G38" s="40">
         <v>566.51</v>
       </c>
-      <c r="H38" s="53">
+      <c r="H38" s="40">
         <v>4537.6000000000004</v>
       </c>
     </row>
@@ -6199,16 +6339,16 @@
       <c r="D39">
         <v>40</v>
       </c>
-      <c r="E39" s="53">
+      <c r="E39" s="40">
         <v>1581.125</v>
       </c>
-      <c r="F39" s="53">
-        <v>0</v>
-      </c>
-      <c r="G39" s="53">
+      <c r="F39" s="40">
+        <v>0</v>
+      </c>
+      <c r="G39" s="40">
         <v>606.97500000000002</v>
       </c>
-      <c r="H39" s="53">
+      <c r="H39" s="40">
         <v>7260.16</v>
       </c>
     </row>
@@ -6216,16 +6356,16 @@
       <c r="D40">
         <v>70</v>
       </c>
-      <c r="E40" s="53">
-        <v>0</v>
-      </c>
-      <c r="F40" s="53">
+      <c r="E40" s="40">
+        <v>0</v>
+      </c>
+      <c r="F40" s="40">
         <v>1855</v>
       </c>
-      <c r="G40" s="53">
+      <c r="G40" s="40">
         <v>1375.8100000000002</v>
       </c>
-      <c r="H40" s="53">
+      <c r="H40" s="40">
         <v>1680</v>
       </c>
     </row>
@@ -6233,16 +6373,16 @@
       <c r="D41">
         <v>107.5</v>
       </c>
-      <c r="E41" s="53">
-        <v>0</v>
-      </c>
-      <c r="F41" s="53">
+      <c r="E41" s="40">
+        <v>0</v>
+      </c>
+      <c r="F41" s="40">
         <v>3465</v>
       </c>
-      <c r="G41" s="53">
+      <c r="G41" s="40">
         <v>687.90500000000009</v>
       </c>
-      <c r="H41" s="53">
+      <c r="H41" s="40">
         <v>25200</v>
       </c>
     </row>
@@ -6250,16 +6390,16 @@
       <c r="D42">
         <v>28</v>
       </c>
-      <c r="E42" s="53">
+      <c r="E42" s="40">
         <v>729.75</v>
       </c>
-      <c r="F42" s="53">
-        <v>0</v>
-      </c>
-      <c r="G42" s="53">
+      <c r="F42" s="40">
+        <v>0</v>
+      </c>
+      <c r="G42" s="40">
         <v>1052.0900000000001</v>
       </c>
-      <c r="H42" s="53">
+      <c r="H42" s="40">
         <v>4764.4799999999996</v>
       </c>
     </row>
@@ -6267,16 +6407,16 @@
       <c r="D43">
         <v>29.25</v>
       </c>
-      <c r="E43" s="53">
+      <c r="E43" s="40">
         <v>875.69999999999993</v>
       </c>
-      <c r="F43" s="53">
-        <v>0</v>
-      </c>
-      <c r="G43" s="53">
+      <c r="F43" s="40">
+        <v>0</v>
+      </c>
+      <c r="G43" s="40">
         <v>910.46250000000009</v>
       </c>
-      <c r="H43" s="53">
+      <c r="H43" s="40">
         <v>8394.56</v>
       </c>
     </row>
@@ -6284,16 +6424,16 @@
       <c r="D44">
         <v>338</v>
       </c>
-      <c r="E44" s="53">
+      <c r="E44" s="40">
         <v>5619.0749999999998</v>
       </c>
-      <c r="F44" s="53">
+      <c r="F44" s="40">
         <v>5320</v>
       </c>
-      <c r="G44" s="53">
+      <c r="G44" s="40">
         <v>5705.5650000000005</v>
       </c>
-      <c r="H44" s="53">
+      <c r="H44" s="40">
         <v>16644.64</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Corrected error in costings
</commit_message>
<xml_diff>
--- a/Report/Costings summary.xlsx
+++ b/Report/Costings summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Documents\GitHub\CSC3600\Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FEF15C1-A5C3-4E49-8BAE-9B8373EF1F21}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88FE5138-961F-47E2-8B4F-77040DDB44DD}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9390" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="51">
   <si>
     <t>Initialising</t>
   </si>
@@ -264,55 +264,16 @@
     <t>Isaac</t>
   </si>
   <si>
-    <t>MAIN</t>
+    <t>`</t>
   </si>
   <si>
-    <t>TASKS</t>
+    <t>Column2</t>
   </si>
   <si>
-    <t>RYAN</t>
+    <t>Labour</t>
   </si>
   <si>
-    <t>GEORGE</t>
-  </si>
-  <si>
-    <t>ISAAC</t>
-  </si>
-  <si>
-    <t>HERTWECK</t>
-  </si>
-  <si>
-    <t>ANDREW JOHNSTON</t>
-  </si>
-  <si>
-    <t>GREGORY</t>
-  </si>
-  <si>
-    <t>JONES</t>
-  </si>
-  <si>
-    <t>Research</t>
-  </si>
-  <si>
-    <t>Discussions</t>
-  </si>
-  <si>
-    <t>Meetings</t>
-  </si>
-  <si>
-    <t>Design</t>
-  </si>
-  <si>
-    <t>Documentation</t>
-  </si>
-  <si>
-    <t>Implementation</t>
-  </si>
-  <si>
-    <t>Monitor and Control</t>
-  </si>
-  <si>
-    <t>TOTAL</t>
+    <t>Equipment</t>
   </si>
 </sst>
 </file>
@@ -381,7 +342,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -411,14 +372,8 @@
         <bgColor theme="4"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFD4E1ED"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="30">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -636,137 +591,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </right>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
-      <bottom style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFFFFFFF"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color rgb="FFFFFFFF"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFFFFFFF"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFFFFFFF"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color rgb="FFFFFFFF"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFFFFFFF"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FFFFFFFF"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color rgb="FFFFFFFF"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFFFFFFF"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color rgb="FFFFFFFF"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FFFFFFFF"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FFFFFFFF"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFFFFFFF"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFFFFFFF"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FFFFFFFF"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFFFFFFF"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FFFFFFFF"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FFFFFFFF"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFFFFFFF"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFFFFFFF"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FFFFFFFF"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -819,60 +649,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="4" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="6" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="6" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="3" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="3" fillId="3" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="3" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -2236,9 +2016,9 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table1345" displayName="Table1345" ref="A1:I16" totalsRowShown="0">
-  <autoFilter ref="A1:I16" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
-  <tableColumns count="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table1345" displayName="Table1345" ref="A1:J16" totalsRowShown="0">
+  <autoFilter ref="A1:J16" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+  <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Column1" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Initialising"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Discover and understand the details of the problem"/>
@@ -2248,6 +2028,7 @@
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="Monitoring and Controlling"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="Deploy"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0300-000009000000}" name="Weekly Total"/>
+    <tableColumn id="10" xr3:uid="{C751530F-B7BA-46F9-9B8F-822B0B688CE0}" name="Column2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2537,7 +2318,7 @@
   <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2998,7 +2779,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3311,48 +3092,48 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="42" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" style="42" customWidth="1"/>
-    <col min="3" max="3" width="45.85546875" style="42" customWidth="1"/>
-    <col min="4" max="4" width="22.7109375" style="42" customWidth="1"/>
-    <col min="5" max="6" width="19.7109375" style="42" customWidth="1"/>
-    <col min="7" max="7" width="25.7109375" style="42" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="42"/>
-    <col min="9" max="9" width="13.7109375" style="42" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="42"/>
+    <col min="1" max="1" width="11.42578125" style="26" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" style="26" customWidth="1"/>
+    <col min="3" max="3" width="45.85546875" style="26" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" style="26" customWidth="1"/>
+    <col min="5" max="6" width="19.7109375" style="26" customWidth="1"/>
+    <col min="7" max="7" width="25.7109375" style="26" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="26"/>
+    <col min="9" max="9" width="13.7109375" style="26" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="26"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="42" t="s">
+      <c r="B1" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="42" t="s">
+      <c r="D1" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="42" t="s">
+      <c r="E1" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="42" t="s">
+      <c r="F1" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="42" t="s">
+      <c r="G1" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="42" t="s">
+      <c r="H1" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="42" t="s">
+      <c r="I1" s="26" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3360,13 +3141,13 @@
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="42">
+      <c r="B2" s="26">
         <v>3</v>
       </c>
-      <c r="C2" s="42">
+      <c r="C2" s="26">
         <v>2.5</v>
       </c>
-      <c r="I2" s="42">
+      <c r="I2" s="26">
         <f>SUM(B2:H2)</f>
         <v>5.5</v>
       </c>
@@ -3375,16 +3156,16 @@
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="42">
+      <c r="C3" s="26">
         <v>1</v>
       </c>
-      <c r="E3" s="42">
+      <c r="E3" s="26">
         <v>5</v>
       </c>
-      <c r="F3" s="42">
+      <c r="F3" s="26">
         <v>2</v>
       </c>
-      <c r="I3" s="42">
+      <c r="I3" s="26">
         <f t="shared" ref="I3:I14" si="0">SUM(B3:H3)</f>
         <v>8</v>
       </c>
@@ -3393,10 +3174,10 @@
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="42">
+      <c r="D4" s="26">
         <v>9.5</v>
       </c>
-      <c r="I4" s="42">
+      <c r="I4" s="26">
         <f t="shared" si="0"/>
         <v>9.5</v>
       </c>
@@ -3405,13 +3186,13 @@
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="42">
+      <c r="B5" s="26">
         <v>0.5</v>
       </c>
-      <c r="D5" s="42">
+      <c r="D5" s="26">
         <v>6</v>
       </c>
-      <c r="I5" s="42">
+      <c r="I5" s="26">
         <f t="shared" si="0"/>
         <v>6.5</v>
       </c>
@@ -3420,10 +3201,10 @@
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="42">
+      <c r="B6" s="26">
         <v>4</v>
       </c>
-      <c r="I6" s="42">
+      <c r="I6" s="26">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
@@ -3432,13 +3213,13 @@
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="42">
+      <c r="B7" s="26">
         <v>0.5</v>
       </c>
-      <c r="C7" s="42">
+      <c r="C7" s="26">
         <v>2</v>
       </c>
-      <c r="I7" s="42">
+      <c r="I7" s="26">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
@@ -3447,19 +3228,19 @@
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="42">
+      <c r="C8" s="26">
         <v>1.5</v>
       </c>
-      <c r="E8" s="42">
+      <c r="E8" s="26">
         <v>7</v>
       </c>
-      <c r="F8" s="42">
+      <c r="F8" s="26">
         <v>3</v>
       </c>
-      <c r="G8" s="42">
+      <c r="G8" s="26">
         <v>1</v>
       </c>
-      <c r="I8" s="42">
+      <c r="I8" s="26">
         <f t="shared" si="0"/>
         <v>12.5</v>
       </c>
@@ -3468,16 +3249,16 @@
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="42">
+      <c r="C9" s="26">
         <v>2</v>
       </c>
-      <c r="E9" s="42">
+      <c r="E9" s="26">
         <v>4</v>
       </c>
-      <c r="F9" s="42">
+      <c r="F9" s="26">
         <v>1</v>
       </c>
-      <c r="I9" s="42">
+      <c r="I9" s="26">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
@@ -3486,13 +3267,13 @@
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="42">
+      <c r="E10" s="26">
         <v>4</v>
       </c>
-      <c r="F10" s="42">
+      <c r="F10" s="26">
         <v>2</v>
       </c>
-      <c r="I10" s="42">
+      <c r="I10" s="26">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
@@ -3501,13 +3282,13 @@
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="42">
+      <c r="E11" s="26">
         <v>5</v>
       </c>
-      <c r="F11" s="42">
+      <c r="F11" s="26">
         <v>1</v>
       </c>
-      <c r="I11" s="42">
+      <c r="I11" s="26">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
@@ -3516,13 +3297,13 @@
       <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E12" s="42">
+      <c r="E12" s="26">
         <v>3.5</v>
       </c>
-      <c r="F12" s="42">
+      <c r="F12" s="26">
         <v>0.5</v>
       </c>
-      <c r="I12" s="42">
+      <c r="I12" s="26">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
@@ -3531,10 +3312,10 @@
       <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F13" s="42">
+      <c r="F13" s="26">
         <v>4</v>
       </c>
-      <c r="I13" s="42">
+      <c r="I13" s="26">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
@@ -3543,10 +3324,10 @@
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H14" s="42">
+      <c r="H14" s="26">
         <v>2.5</v>
       </c>
-      <c r="I14" s="42">
+      <c r="I14" s="26">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
@@ -3555,47 +3336,47 @@
       <c r="A15" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="H15" s="42">
+      <c r="H15" s="26">
         <v>1.5</v>
       </c>
-      <c r="I15" s="42">
+      <c r="I15" s="26">
         <f>SUM(B15:H15)</f>
         <v>1.5</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="43" t="s">
+      <c r="A16" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="43">
+      <c r="B16" s="27">
         <f>SUM(B2:B15)</f>
         <v>8</v>
       </c>
-      <c r="C16" s="43">
+      <c r="C16" s="27">
         <f t="shared" ref="C16:I16" si="1">SUM(C2:C15)</f>
         <v>9</v>
       </c>
-      <c r="D16" s="43">
+      <c r="D16" s="27">
         <f t="shared" si="1"/>
         <v>15.5</v>
       </c>
-      <c r="E16" s="43">
+      <c r="E16" s="27">
         <f t="shared" si="1"/>
         <v>28.5</v>
       </c>
-      <c r="F16" s="43">
+      <c r="F16" s="27">
         <f t="shared" si="1"/>
         <v>13.5</v>
       </c>
-      <c r="G16" s="43">
+      <c r="G16" s="27">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="H16" s="43">
+      <c r="H16" s="27">
         <f>SUM(H2:H15)</f>
         <v>4</v>
       </c>
-      <c r="I16" s="43">
+      <c r="I16" s="27">
         <f t="shared" si="1"/>
         <v>79.5</v>
       </c>
@@ -3612,10 +3393,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3630,7 +3411,7 @@
     <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -3658,8 +3439,11 @@
       <c r="I1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -3673,8 +3457,11 @@
         <f>SUM(B2:H2)</f>
         <v>2.25</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -3688,8 +3475,11 @@
         <f>SUM(B3:H3)</f>
         <v>1.75</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -3706,8 +3496,11 @@
         <f>SUM(B4:H4)</f>
         <v>3.25</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
@@ -3724,8 +3517,11 @@
         <f t="shared" ref="I4:I15" si="0">SUM(B5:H5)</f>
         <v>7.5</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
@@ -3742,8 +3538,11 @@
         <f t="shared" si="0"/>
         <v>3.5</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -3760,8 +3559,11 @@
         <f t="shared" si="0"/>
         <v>3.5</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -3778,8 +3580,11 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -3799,8 +3604,11 @@
         <f t="shared" si="0"/>
         <v>4.5</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
@@ -3820,8 +3628,11 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
@@ -3841,8 +3652,11 @@
         <f t="shared" si="0"/>
         <v>5.5</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
@@ -3862,8 +3676,11 @@
         <f t="shared" si="0"/>
         <v>6.5</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
@@ -3883,8 +3700,11 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
@@ -3898,8 +3718,11 @@
         <f t="shared" si="0"/>
         <v>5.5</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>41</v>
       </c>
@@ -3913,8 +3736,11 @@
         <f t="shared" si="0"/>
         <v>7.75</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>21</v>
       </c>
@@ -4043,19 +3869,18 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:Q43"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="8" max="8" width="13.42578125" customWidth="1"/>
-    <col min="9" max="9" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
         <v>42</v>
       </c>
@@ -4080,11 +3905,8 @@
       <c r="H1" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="24" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>43</v>
       </c>
@@ -4116,12 +3938,8 @@
         <f>Greg!H16</f>
         <v>6</v>
       </c>
-      <c r="I2">
-        <f>Greg!I16</f>
-        <v>107</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>44</v>
       </c>
@@ -4153,12 +3971,8 @@
         <f>Ryan!H16</f>
         <v>5</v>
       </c>
-      <c r="I3">
-        <f>Ryan!I16</f>
-        <v>74</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>45</v>
       </c>
@@ -4190,12 +4004,8 @@
         <f>Andrew!H16</f>
         <v>4</v>
       </c>
-      <c r="I4">
-        <f>Andrew!I16</f>
-        <v>79.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>46</v>
       </c>
@@ -4227,12 +4037,8 @@
         <f>Isaac!H16</f>
         <v>11.25</v>
       </c>
-      <c r="I5">
-        <f>Isaac!I16</f>
-        <v>70.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -4241,7 +4047,7 @@
         <v>26.75</v>
       </c>
       <c r="C6">
-        <f t="shared" ref="C6:I6" si="0">SUM(C2:C5)</f>
+        <f t="shared" ref="C6:H6" si="0">SUM(C2:C5)</f>
         <v>49.5</v>
       </c>
       <c r="D6">
@@ -4264,29 +4070,8 @@
         <f t="shared" si="0"/>
         <v>26.25</v>
       </c>
-      <c r="I6">
-        <f t="shared" si="0"/>
-        <v>331</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" ht="30" x14ac:dyDescent="0.25">
-      <c r="M7" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="N7" s="28" t="s">
-        <v>49</v>
-      </c>
-      <c r="O7" s="28" t="s">
-        <v>51</v>
-      </c>
-      <c r="P7" s="44" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q7" s="30" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
         <v>42</v>
       </c>
@@ -4311,839 +4096,325 @@
       <c r="H8" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="I8" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="M8" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="N8" s="29" t="s">
-        <v>50</v>
-      </c>
-      <c r="O8" s="29" t="s">
-        <v>52</v>
-      </c>
-      <c r="P8" s="45"/>
-      <c r="Q8" s="31" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>43</v>
       </c>
-      <c r="B9" s="25">
+      <c r="B9" s="24">
         <f>B2/B$6</f>
         <v>0.3925233644859813</v>
       </c>
-      <c r="C9" s="25">
+      <c r="C9" s="24">
         <f t="shared" ref="C9:H9" si="1">C2/C$6</f>
         <v>0.26262626262626265</v>
       </c>
-      <c r="D9" s="25">
+      <c r="D9" s="24">
         <f t="shared" si="1"/>
         <v>0.27027027027027029</v>
       </c>
-      <c r="E9" s="25">
+      <c r="E9" s="24">
         <f t="shared" si="1"/>
         <v>3.9603960396039604E-2</v>
       </c>
-      <c r="F9" s="25">
+      <c r="F9" s="24">
         <f t="shared" si="1"/>
         <v>0.60465116279069764</v>
       </c>
-      <c r="G9" s="25">
+      <c r="G9" s="24">
         <f t="shared" si="1"/>
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="H9" s="25">
+      <c r="H9" s="24">
         <f t="shared" si="1"/>
         <v>0.22857142857142856</v>
       </c>
-      <c r="I9" s="25">
-        <v>0.25</v>
-      </c>
-      <c r="J9" s="25">
-        <v>0.25</v>
-      </c>
-      <c r="K9" s="25">
-        <f>SUM(B9:J9)/9</f>
-        <v>0.26461997583044589</v>
-      </c>
-      <c r="M9" s="32"/>
-      <c r="N9" s="37">
-        <v>0.154</v>
-      </c>
-      <c r="O9" s="38">
-        <v>0.214</v>
-      </c>
-      <c r="P9" s="38">
-        <v>0.27400000000000002</v>
-      </c>
-      <c r="Q9" s="39">
-        <v>0.35899999999999999</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="25">
+      <c r="B10" s="24">
         <f t="shared" ref="B10:H10" si="2">B3/B$6</f>
         <v>7.476635514018691E-2</v>
       </c>
-      <c r="C10" s="25">
+      <c r="C10" s="24">
         <f t="shared" si="2"/>
         <v>0.41414141414141414</v>
       </c>
-      <c r="D10" s="25">
+      <c r="D10" s="24">
         <f t="shared" si="2"/>
         <v>0.10810810810810811</v>
       </c>
-      <c r="E10" s="25">
+      <c r="E10" s="24">
         <f t="shared" si="2"/>
         <v>5.9405940594059403E-2</v>
       </c>
-      <c r="F10" s="25">
+      <c r="F10" s="24">
         <f t="shared" si="2"/>
         <v>0.19069767441860466</v>
       </c>
-      <c r="G10" s="25">
+      <c r="G10" s="24">
         <f t="shared" si="2"/>
         <v>0.52777777777777779</v>
       </c>
-      <c r="H10" s="25">
+      <c r="H10" s="24">
         <f t="shared" si="2"/>
         <v>0.19047619047619047</v>
       </c>
-      <c r="I10" s="25">
-        <v>0.25</v>
-      </c>
-      <c r="J10" s="25">
-        <v>0.25</v>
-      </c>
-      <c r="K10" s="25">
-        <f t="shared" ref="K10:K12" si="3">SUM(B10:J10)/9</f>
-        <v>0.22948594007292686</v>
-      </c>
-      <c r="M10" s="32" t="s">
-        <v>56</v>
-      </c>
-      <c r="N10" s="33">
-        <v>7.9000000000000001E-2</v>
-      </c>
-      <c r="O10" s="33">
-        <v>0.222</v>
-      </c>
-      <c r="P10" s="33">
-        <v>0.28599999999999998</v>
-      </c>
-      <c r="Q10" s="33">
-        <v>0.41299999999999998</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>45</v>
       </c>
-      <c r="B11" s="25">
-        <f t="shared" ref="B11:H11" si="4">B4/B$6</f>
+      <c r="B11" s="24">
+        <f t="shared" ref="B11:H11" si="3">B4/B$6</f>
         <v>0.29906542056074764</v>
       </c>
-      <c r="C11" s="25">
-        <f t="shared" si="4"/>
+      <c r="C11" s="24">
+        <f t="shared" si="3"/>
         <v>0.18181818181818182</v>
       </c>
-      <c r="D11" s="25">
-        <f t="shared" si="4"/>
+      <c r="D11" s="24">
+        <f t="shared" si="3"/>
         <v>0.41891891891891891</v>
       </c>
-      <c r="E11" s="25">
-        <f t="shared" si="4"/>
+      <c r="E11" s="24">
+        <f t="shared" si="3"/>
         <v>0.5643564356435643</v>
       </c>
-      <c r="F11" s="25">
-        <f t="shared" si="4"/>
+      <c r="F11" s="24">
+        <f t="shared" si="3"/>
         <v>0.12558139534883722</v>
       </c>
-      <c r="G11" s="25">
-        <f t="shared" si="4"/>
+      <c r="G11" s="24">
+        <f t="shared" si="3"/>
         <v>2.7777777777777776E-2</v>
       </c>
-      <c r="H11" s="25">
-        <f t="shared" si="4"/>
+      <c r="H11" s="24">
+        <f t="shared" si="3"/>
         <v>0.15238095238095239</v>
       </c>
-      <c r="I11" s="25">
-        <v>0.25</v>
-      </c>
-      <c r="J11" s="25">
-        <v>0.25</v>
-      </c>
-      <c r="K11" s="25">
-        <f t="shared" si="3"/>
-        <v>0.25221100916099776</v>
-      </c>
-      <c r="M11" s="32" t="s">
-        <v>57</v>
-      </c>
-      <c r="N11" s="34">
-        <v>0.25</v>
-      </c>
-      <c r="O11" s="34">
-        <v>0.25</v>
-      </c>
-      <c r="P11" s="34">
-        <v>0.25</v>
-      </c>
-      <c r="Q11" s="34">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="25">
-        <f t="shared" ref="B12:H12" si="5">B5/B$6</f>
+      <c r="B12" s="24">
+        <f t="shared" ref="B12:H12" si="4">B5/B$6</f>
         <v>0.23364485981308411</v>
       </c>
-      <c r="C12" s="25">
+      <c r="C12" s="24">
+        <f t="shared" si="4"/>
+        <v>0.14141414141414141</v>
+      </c>
+      <c r="D12" s="24">
+        <f t="shared" si="4"/>
+        <v>0.20270270270270271</v>
+      </c>
+      <c r="E12" s="24">
+        <f t="shared" si="4"/>
+        <v>0.33663366336633666</v>
+      </c>
+      <c r="F12" s="24">
+        <f t="shared" si="4"/>
+        <v>7.9069767441860464E-2</v>
+      </c>
+      <c r="G12" s="24">
+        <f t="shared" si="4"/>
+        <v>0.3611111111111111</v>
+      </c>
+      <c r="H12" s="24">
+        <f t="shared" si="4"/>
+        <v>0.42857142857142855</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="24"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" t="s">
+        <v>45</v>
+      </c>
+      <c r="E18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="24">
+        <v>7.476635514018691E-2</v>
+      </c>
+      <c r="C19" s="24">
+        <v>0.23364485981308411</v>
+      </c>
+      <c r="D19" s="24">
+        <v>0.29906542056074764</v>
+      </c>
+      <c r="E19" s="24">
+        <v>0.3925233644859813</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20" s="24">
+        <v>0.10810810810810811</v>
+      </c>
+      <c r="C20" s="24">
+        <v>0.20270270270270271</v>
+      </c>
+      <c r="D20" s="24">
+        <v>0.41891891891891891</v>
+      </c>
+      <c r="E20" s="24">
+        <v>0.27027027027027029</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" s="24">
+        <v>0.41414141414141414</v>
+      </c>
+      <c r="C21" s="24">
+        <v>0.14141414141414141</v>
+      </c>
+      <c r="D21" s="24">
+        <v>0.18181818181818182</v>
+      </c>
+      <c r="E21" s="24">
+        <v>0.26262626262626265</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="24">
+        <v>0.25</v>
+      </c>
+      <c r="C22" s="24">
+        <v>0.25</v>
+      </c>
+      <c r="D22" s="24">
+        <v>0.25</v>
+      </c>
+      <c r="E22" s="24">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="24">
+        <v>0.25</v>
+      </c>
+      <c r="C23" s="24">
+        <v>0.25</v>
+      </c>
+      <c r="D23" s="24">
+        <v>0.25</v>
+      </c>
+      <c r="E23" s="24">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" s="24">
+        <v>5.9405940594059403E-2</v>
+      </c>
+      <c r="C24" s="24">
+        <v>0.33663366336633666</v>
+      </c>
+      <c r="D24" s="24">
+        <v>0.5643564356435643</v>
+      </c>
+      <c r="E24" s="24">
+        <v>3.9603960396039604E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" s="24">
+        <v>0.19069767441860466</v>
+      </c>
+      <c r="C25" s="24">
+        <v>7.9069767441860464E-2</v>
+      </c>
+      <c r="D25" s="24">
+        <v>0.12558139534883722</v>
+      </c>
+      <c r="E25" s="24">
+        <v>0.60465116279069764</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" s="24">
+        <v>0.52777777777777779</v>
+      </c>
+      <c r="C26" s="24">
+        <v>0.3611111111111111</v>
+      </c>
+      <c r="D26" s="24">
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="E26" s="24">
+        <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" s="24">
+        <v>0.19047619047619047</v>
+      </c>
+      <c r="C27" s="24">
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="D27" s="24">
+        <v>0.15238095238095239</v>
+      </c>
+      <c r="E27" s="24">
+        <v>0.22857142857142856</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="24">
+        <f>SUM(B19:B27)/9</f>
+        <v>0.22948594007292686</v>
+      </c>
+      <c r="C28" s="24">
+        <f t="shared" ref="C28:E28" si="5">SUM(C19:C27)/9</f>
+        <v>0.25368307493562947</v>
+      </c>
+      <c r="D28" s="24">
         <f t="shared" si="5"/>
-        <v>0.14141414141414141</v>
-      </c>
-      <c r="D12" s="25">
+        <v>0.25221100916099776</v>
+      </c>
+      <c r="E28" s="24">
         <f t="shared" si="5"/>
-        <v>0.20270270270270271</v>
-      </c>
-      <c r="E12" s="25">
-        <f t="shared" si="5"/>
-        <v>0.33663366336633666</v>
-      </c>
-      <c r="F12" s="25">
-        <f t="shared" si="5"/>
-        <v>7.9069767441860464E-2</v>
-      </c>
-      <c r="G12" s="25">
-        <f t="shared" si="5"/>
-        <v>0.3611111111111111</v>
-      </c>
-      <c r="H12" s="25">
-        <f t="shared" si="5"/>
-        <v>0.42857142857142855</v>
-      </c>
-      <c r="I12" s="25">
-        <v>0.25</v>
-      </c>
-      <c r="J12" s="25">
-        <v>0.25</v>
-      </c>
-      <c r="K12" s="25">
-        <f t="shared" si="3"/>
-        <v>0.25368307493562942</v>
-      </c>
-      <c r="M12" s="32" t="s">
-        <v>58</v>
-      </c>
-      <c r="N12" s="34">
-        <v>0.25</v>
-      </c>
-      <c r="O12" s="34">
-        <v>0.25</v>
-      </c>
-      <c r="P12" s="34">
-        <v>0.25</v>
-      </c>
-      <c r="Q12" s="34">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="M13" s="32" t="s">
-        <v>59</v>
-      </c>
-      <c r="N13" s="36">
-        <v>0.32100000000000001</v>
-      </c>
-      <c r="O13" s="36">
-        <v>0.24299999999999999</v>
-      </c>
-      <c r="P13" s="36">
-        <v>0.40699999999999997</v>
-      </c>
-      <c r="Q13" s="36">
-        <v>2.9000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="M14" s="32" t="s">
-        <v>60</v>
-      </c>
-      <c r="N14" s="35"/>
-      <c r="O14" s="35"/>
-      <c r="P14" s="35"/>
-      <c r="Q14" s="35"/>
-    </row>
-    <row r="15" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="25">
-        <v>0.3925233644859813</v>
-      </c>
-      <c r="C15" s="25">
-        <v>0.26262626262626265</v>
-      </c>
-      <c r="D15" s="25">
-        <v>0.27027027027027029</v>
-      </c>
-      <c r="E15" s="25">
-        <v>3.9603960396039604E-2</v>
-      </c>
-      <c r="F15" s="25">
-        <v>0.60465116279069764</v>
-      </c>
-      <c r="G15" s="25">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="H15" s="25">
-        <v>0.22857142857142856</v>
-      </c>
-      <c r="I15" s="25">
-        <v>0.25</v>
-      </c>
-      <c r="J15" s="25">
-        <v>0.25</v>
-      </c>
-      <c r="K15">
-        <v>0.27328681050504594</v>
-      </c>
-      <c r="M15" s="32" t="s">
-        <v>61</v>
-      </c>
-      <c r="N15" s="36">
-        <v>0.187</v>
-      </c>
-      <c r="O15" s="36">
-        <v>7.9000000000000001E-2</v>
-      </c>
-      <c r="P15" s="36">
-        <v>0.126</v>
-      </c>
-      <c r="Q15" s="36">
-        <v>0.60699999999999998</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="25">
-        <v>7.476635514018691E-2</v>
-      </c>
-      <c r="C16" s="25">
-        <v>0.41414141414141414</v>
-      </c>
-      <c r="D16" s="25">
-        <v>0.10810810810810811</v>
-      </c>
-      <c r="E16" s="25">
-        <v>5.9405940594059403E-2</v>
-      </c>
-      <c r="F16" s="25">
-        <v>0.19069767441860466</v>
-      </c>
-      <c r="G16" s="25">
-        <v>0.52777777777777779</v>
-      </c>
-      <c r="H16" s="25">
-        <v>0.19047619047619047</v>
-      </c>
-      <c r="I16" s="25">
-        <v>0.25</v>
-      </c>
-      <c r="J16" s="25">
-        <v>0.25</v>
-      </c>
-      <c r="K16">
-        <v>0.2314496918083554</v>
-      </c>
-      <c r="M16" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="N16" s="33">
-        <v>0.26100000000000001</v>
-      </c>
-      <c r="O16" s="33">
-        <v>0.39100000000000001</v>
-      </c>
-      <c r="P16" s="33">
-        <v>0.13900000000000001</v>
-      </c>
-      <c r="Q16" s="33">
-        <v>0.20899999999999999</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="25">
-        <v>0.29906542056074764</v>
-      </c>
-      <c r="C17" s="25">
-        <v>0.18181818181818182</v>
-      </c>
-      <c r="D17" s="25">
-        <v>0.41891891891891891</v>
-      </c>
-      <c r="E17" s="25">
-        <v>0.5643564356435643</v>
-      </c>
-      <c r="F17" s="25">
-        <v>0.12558139534883722</v>
-      </c>
-      <c r="G17" s="25">
-        <v>2.7777777777777776E-2</v>
-      </c>
-      <c r="H17" s="25">
-        <v>0.15238095238095239</v>
-      </c>
-      <c r="I17" s="25">
-        <v>0.25</v>
-      </c>
-      <c r="J17" s="25">
-        <v>0.25</v>
-      </c>
-      <c r="K17">
-        <v>0.23775279631032545</v>
-      </c>
-      <c r="M17" s="32" t="s">
-        <v>62</v>
-      </c>
-      <c r="N17" s="36">
-        <v>0.32</v>
-      </c>
-      <c r="O17" s="36">
-        <v>0.52</v>
-      </c>
-      <c r="P17" s="36">
-        <v>0.04</v>
-      </c>
-      <c r="Q17" s="36">
-        <v>0.12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="25">
-        <v>0.23364485981308411</v>
-      </c>
-      <c r="C18" s="25">
-        <v>0.14141414141414141</v>
-      </c>
-      <c r="D18" s="25">
-        <v>0.20270270270270271</v>
-      </c>
-      <c r="E18" s="25">
-        <v>0.33663366336633666</v>
-      </c>
-      <c r="F18" s="25">
-        <v>7.9069767441860464E-2</v>
-      </c>
-      <c r="G18" s="25">
-        <v>0.3611111111111111</v>
-      </c>
-      <c r="H18" s="25">
-        <v>0.42857142857142855</v>
-      </c>
-      <c r="I18" s="25">
-        <v>0.25</v>
-      </c>
-      <c r="J18" s="25">
-        <v>0.25</v>
-      </c>
-      <c r="K18">
-        <v>0.25751070137627319</v>
-      </c>
-      <c r="M18" s="32" t="s">
-        <v>63</v>
-      </c>
-      <c r="N18" s="33">
-        <f t="shared" ref="N18:P18" si="6">SUM(N9:N17)</f>
-        <v>1.8220000000000003</v>
-      </c>
-      <c r="O18" s="33">
-        <f t="shared" si="6"/>
-        <v>2.1689999999999996</v>
-      </c>
-      <c r="P18" s="33">
-        <f t="shared" si="6"/>
-        <v>1.772</v>
-      </c>
-      <c r="Q18" s="33">
-        <f>SUM(Q9:Q17)</f>
-        <v>2.2370000000000001</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>44</v>
-      </c>
-      <c r="C21" t="s">
-        <v>46</v>
-      </c>
-      <c r="D21" t="s">
-        <v>45</v>
-      </c>
-      <c r="E21" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A22" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="B22" s="25">
-        <v>0.18181818181818199</v>
-      </c>
-      <c r="C22" s="25">
-        <v>0.20661157024793389</v>
-      </c>
-      <c r="D22" s="25">
-        <v>0.26446280991735538</v>
-      </c>
-      <c r="E22" s="25">
-        <v>0.34710743801652894</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A23" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="B23" s="25">
-        <v>0.17499999999999999</v>
-      </c>
-      <c r="C23" s="25">
-        <v>0.1875</v>
-      </c>
-      <c r="D23" s="25">
-        <v>0.38750000000000001</v>
-      </c>
-      <c r="E23" s="25">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A24" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="B24" s="25">
-        <v>0.12121212121212122</v>
-      </c>
-      <c r="C24" s="25">
-        <v>0.21212121212121213</v>
-      </c>
-      <c r="D24" s="25">
-        <v>0.27272727272727271</v>
-      </c>
-      <c r="E24" s="25">
-        <v>0.39393939393939392</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B25">
-        <v>0.25</v>
-      </c>
-      <c r="C25">
-        <v>0.25</v>
-      </c>
-      <c r="D25">
-        <v>0.25</v>
-      </c>
-      <c r="E25">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B26">
-        <v>0.25</v>
-      </c>
-      <c r="C26">
-        <v>0.25</v>
-      </c>
-      <c r="D26">
-        <v>0.25</v>
-      </c>
-      <c r="E26">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A27" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="B27" s="25">
-        <v>0.33098591549295775</v>
-      </c>
-      <c r="C27" s="25">
-        <v>0.23943661971830985</v>
-      </c>
-      <c r="D27" s="25">
-        <v>0.40140845070422537</v>
-      </c>
-      <c r="E27" s="25">
-        <v>2.8169014084507043E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A28" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="B28" s="25">
-        <v>0.19069767441860466</v>
-      </c>
-      <c r="C28" s="25">
-        <v>7.9069767441860464E-2</v>
-      </c>
-      <c r="D28" s="25">
-        <v>0.12558139534883722</v>
-      </c>
-      <c r="E28" s="25">
-        <v>0.60465116279069764</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A29" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="B29" s="25">
-        <v>0.39285714285714285</v>
-      </c>
-      <c r="C29" s="25">
-        <v>0.4642857142857143</v>
-      </c>
-      <c r="D29" s="25">
-        <v>3.5714285714285712E-2</v>
-      </c>
-      <c r="E29" s="25">
-        <v>0.10714285714285714</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A30" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="B30" s="25">
-        <v>0.19047619047619047</v>
-      </c>
-      <c r="C30" s="25">
-        <v>0.42857142857142855</v>
-      </c>
-      <c r="D30" s="25">
-        <v>0.15238095238095239</v>
-      </c>
-      <c r="E30" s="25">
-        <v>0.22857142857142856</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B31" s="41">
-        <f>SUM(B22:B30)/9</f>
-        <v>0.23144969180835545</v>
-      </c>
-      <c r="C31" s="41">
-        <f t="shared" ref="C31:E31" si="7">SUM(C22:C30)/9</f>
-        <v>0.25751070137627319</v>
-      </c>
-      <c r="D31" s="41">
-        <f t="shared" si="7"/>
-        <v>0.23775279631032545</v>
-      </c>
-      <c r="E31" s="41">
-        <f t="shared" si="7"/>
-        <v>0.27328681050504594</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B32" s="25"/>
-      <c r="C32" s="25"/>
-      <c r="D32" s="25"/>
-      <c r="E32" s="25"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
-        <v>44</v>
-      </c>
-      <c r="C33" t="s">
-        <v>46</v>
-      </c>
-      <c r="D33" t="s">
-        <v>45</v>
-      </c>
-      <c r="E33" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="B34" s="25">
-        <v>7.476635514018691E-2</v>
-      </c>
-      <c r="C34" s="25">
-        <v>0.23364485981308411</v>
-      </c>
-      <c r="D34" s="25">
-        <v>0.29906542056074764</v>
-      </c>
-      <c r="E34" s="25">
-        <v>0.3925233644859813</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="B35" s="25">
-        <v>0.10810810810810811</v>
-      </c>
-      <c r="C35" s="25">
-        <v>0.20270270270270271</v>
-      </c>
-      <c r="D35" s="25">
-        <v>0.41891891891891891</v>
-      </c>
-      <c r="E35" s="25">
-        <v>0.27027027027027029</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="B36" s="25">
-        <v>0.41414141414141414</v>
-      </c>
-      <c r="C36" s="25">
-        <v>0.14141414141414141</v>
-      </c>
-      <c r="D36" s="25">
-        <v>0.18181818181818182</v>
-      </c>
-      <c r="E36" s="25">
-        <v>0.26262626262626265</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B37" s="25">
-        <v>0.25</v>
-      </c>
-      <c r="C37" s="25">
-        <v>0.25</v>
-      </c>
-      <c r="D37" s="25">
-        <v>0.25</v>
-      </c>
-      <c r="E37" s="25">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B38" s="25">
-        <v>0.25</v>
-      </c>
-      <c r="C38" s="25">
-        <v>0.25</v>
-      </c>
-      <c r="D38" s="25">
-        <v>0.25</v>
-      </c>
-      <c r="E38" s="25">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="B39" s="25">
-        <v>5.9405940594059403E-2</v>
-      </c>
-      <c r="C39" s="25">
-        <v>0.33663366336633666</v>
-      </c>
-      <c r="D39" s="25">
-        <v>0.5643564356435643</v>
-      </c>
-      <c r="E39" s="25">
-        <v>3.9603960396039604E-2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="B40" s="25">
-        <v>0.19069767441860466</v>
-      </c>
-      <c r="C40" s="25">
-        <v>7.9069767441860464E-2</v>
-      </c>
-      <c r="D40" s="25">
-        <v>0.12558139534883722</v>
-      </c>
-      <c r="E40" s="25">
-        <v>0.60465116279069764</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="B41" s="25">
-        <v>0.52777777777777779</v>
-      </c>
-      <c r="C41" s="25">
-        <v>0.3611111111111111</v>
-      </c>
-      <c r="D41" s="25">
-        <v>2.7777777777777776E-2</v>
-      </c>
-      <c r="E41" s="25">
-        <v>8.3333333333333329E-2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="B42" s="25">
-        <v>0.19047619047619047</v>
-      </c>
-      <c r="C42" s="25">
-        <v>0.42857142857142855</v>
-      </c>
-      <c r="D42" s="25">
-        <v>0.15238095238095239</v>
-      </c>
-      <c r="E42" s="25">
-        <v>0.22857142857142856</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B43" s="25">
-        <f>SUM(B34:B42)/9</f>
-        <v>0.22948594007292686</v>
-      </c>
-      <c r="C43" s="25">
-        <f t="shared" ref="C43:E43" si="8">SUM(C34:C42)/9</f>
-        <v>0.25368307493562947</v>
-      </c>
-      <c r="D43" s="25">
-        <f t="shared" si="8"/>
-        <v>0.25221100916099776</v>
-      </c>
-      <c r="E43" s="25">
-        <f t="shared" si="8"/>
         <v>0.26461997583044594</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="P7:P8"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -5154,7 +4425,7 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5797,7 +5068,7 @@
   <dimension ref="A1:Q44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5890,7 +5161,8 @@
         <v>505.81250000000006</v>
       </c>
       <c r="G2" s="10">
-        <v>3403.2</v>
+        <f>D2+E2+F2</f>
+        <v>1503.1375</v>
       </c>
       <c r="H2">
         <f>Isaac!B16</f>
@@ -5944,15 +5216,16 @@
         <f t="shared" ref="F3:F8" si="0">H3*F$16</f>
         <v>566.51</v>
       </c>
-      <c r="G3" s="14">
-        <v>4537.6000000000004</v>
+      <c r="G3" s="10">
+        <f t="shared" ref="G3:G8" si="1">D3+E3+F3</f>
+        <v>2634.1350000000002</v>
       </c>
       <c r="H3">
         <f>Isaac!C16</f>
         <v>7</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I8" si="1">C3-H3</f>
+        <f t="shared" ref="I3:I8" si="2">C3-H3</f>
         <v>42.5</v>
       </c>
       <c r="K3" s="11">
@@ -6000,14 +5273,15 @@
         <v>606.97500000000002</v>
       </c>
       <c r="G4" s="10">
-        <v>7260.16</v>
+        <f t="shared" si="1"/>
+        <v>2042.15</v>
       </c>
       <c r="H4">
         <f>Isaac!D16</f>
         <v>7.5</v>
       </c>
       <c r="I4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>29.5</v>
       </c>
       <c r="K4" s="6">
@@ -6047,22 +5321,22 @@
       </c>
       <c r="E5" s="14">
         <f>I5*E16</f>
-        <v>1855</v>
+        <v>2450</v>
       </c>
       <c r="F5" s="14">
         <f t="shared" si="0"/>
-        <v>1375.8100000000002</v>
-      </c>
-      <c r="G5" s="14">
-        <v>1680</v>
+        <v>0</v>
+      </c>
+      <c r="G5" s="10">
+        <f t="shared" si="1"/>
+        <v>2450</v>
       </c>
       <c r="H5">
-        <f>Isaac!E16</f>
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="I5">
-        <f t="shared" si="1"/>
-        <v>53</v>
+        <f t="shared" si="2"/>
+        <v>70</v>
       </c>
       <c r="K5" s="11">
         <v>4</v>
@@ -6102,22 +5376,22 @@
       </c>
       <c r="E6" s="10">
         <f>I6*E16</f>
-        <v>3465</v>
+        <v>3762.5</v>
       </c>
       <c r="F6" s="10">
         <f t="shared" si="0"/>
-        <v>687.90500000000009</v>
+        <v>0</v>
       </c>
       <c r="G6" s="10">
-        <v>25200</v>
+        <f t="shared" si="1"/>
+        <v>3762.5</v>
       </c>
       <c r="H6">
-        <f>Isaac!F16</f>
-        <v>8.5</v>
+        <v>0</v>
       </c>
       <c r="I6">
-        <f t="shared" si="1"/>
-        <v>99</v>
+        <f t="shared" si="2"/>
+        <v>107.5</v>
       </c>
       <c r="K6" s="6">
         <v>5</v>
@@ -6163,15 +5437,16 @@
         <f t="shared" si="0"/>
         <v>1052.0900000000001</v>
       </c>
-      <c r="G7" s="14">
-        <v>4764.4799999999996</v>
+      <c r="G7" s="10">
+        <f t="shared" si="1"/>
+        <v>2171.04</v>
       </c>
       <c r="H7">
         <f>Isaac!G16</f>
         <v>13</v>
       </c>
       <c r="I7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>23</v>
       </c>
       <c r="K7" s="11">
@@ -6219,14 +5494,15 @@
         <v>910.46250000000009</v>
       </c>
       <c r="G8" s="10">
-        <v>8394.56</v>
+        <f t="shared" si="1"/>
+        <v>1786.1624999999999</v>
       </c>
       <c r="H8">
         <f>Isaac!H16</f>
         <v>11.25</v>
       </c>
       <c r="I8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="K8" s="6">
@@ -6252,10 +5528,10 @@
       </c>
     </row>
     <row r="9" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="49" t="s">
+      <c r="A9" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="50"/>
+      <c r="B9" s="32"/>
       <c r="C9" s="13">
         <f>SUM(C2:C8)</f>
         <v>356</v>
@@ -6266,20 +5542,20 @@
       </c>
       <c r="E9" s="16">
         <f>SUM(E2:E8)</f>
-        <v>5320</v>
+        <v>6212.5</v>
       </c>
       <c r="F9" s="16">
         <f>SUM(F2:F8)</f>
-        <v>5705.5650000000005</v>
+        <v>3641.8500000000004</v>
       </c>
       <c r="G9" s="16">
         <f>SUM(D9:F9)</f>
-        <v>17520.34</v>
-      </c>
-      <c r="K9" s="49" t="s">
+        <v>16349.125</v>
+      </c>
+      <c r="K9" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="L9" s="50"/>
+      <c r="L9" s="32"/>
       <c r="M9" s="13">
         <v>377</v>
       </c>
@@ -6297,115 +5573,115 @@
       </c>
     </row>
     <row r="10" spans="1:17" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="51" t="s">
+      <c r="A10" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="52"/>
-      <c r="C10" s="52"/>
-      <c r="D10" s="52"/>
-      <c r="E10" s="52"/>
-      <c r="F10" s="52"/>
-      <c r="G10" s="53"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
+      <c r="G10" s="35"/>
       <c r="H10">
         <v>3400</v>
       </c>
       <c r="I10" s="9">
         <f>G9+H10</f>
-        <v>20920.34</v>
-      </c>
-      <c r="K10" s="51" t="s">
+        <v>19749.125</v>
+      </c>
+      <c r="K10" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="L10" s="52"/>
-      <c r="M10" s="52"/>
-      <c r="N10" s="52"/>
-      <c r="O10" s="52"/>
-      <c r="P10" s="52"/>
-      <c r="Q10" s="53"/>
+      <c r="L10" s="34"/>
+      <c r="M10" s="34"/>
+      <c r="N10" s="34"/>
+      <c r="O10" s="34"/>
+      <c r="P10" s="34"/>
+      <c r="Q10" s="35"/>
     </row>
     <row r="11" spans="1:17" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="54" t="s">
+      <c r="A11" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="55"/>
-      <c r="C11" s="55"/>
-      <c r="D11" s="55"/>
-      <c r="E11" s="55"/>
-      <c r="F11" s="55"/>
-      <c r="G11" s="56"/>
+      <c r="B11" s="37"/>
+      <c r="C11" s="37"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="38"/>
       <c r="I11" s="9">
         <f>O22-I10</f>
-        <v>-791.34000000000015</v>
-      </c>
-      <c r="K11" s="54" t="s">
+        <v>379.875</v>
+      </c>
+      <c r="K11" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="L11" s="55"/>
-      <c r="M11" s="55"/>
-      <c r="N11" s="55"/>
-      <c r="O11" s="55"/>
-      <c r="P11" s="55"/>
-      <c r="Q11" s="56"/>
+      <c r="L11" s="37"/>
+      <c r="M11" s="37"/>
+      <c r="N11" s="37"/>
+      <c r="O11" s="37"/>
+      <c r="P11" s="37"/>
+      <c r="Q11" s="38"/>
     </row>
     <row r="12" spans="1:17" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="54" t="s">
+      <c r="A12" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="55"/>
-      <c r="C12" s="55"/>
-      <c r="D12" s="55"/>
-      <c r="E12" s="55"/>
-      <c r="F12" s="55"/>
-      <c r="G12" s="56"/>
-      <c r="K12" s="54" t="s">
+      <c r="B12" s="37"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="38"/>
+      <c r="K12" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="L12" s="55"/>
-      <c r="M12" s="55"/>
-      <c r="N12" s="55"/>
-      <c r="O12" s="55"/>
-      <c r="P12" s="55"/>
-      <c r="Q12" s="56"/>
+      <c r="L12" s="37"/>
+      <c r="M12" s="37"/>
+      <c r="N12" s="37"/>
+      <c r="O12" s="37"/>
+      <c r="P12" s="37"/>
+      <c r="Q12" s="38"/>
     </row>
     <row r="13" spans="1:17" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="54" t="s">
+      <c r="A13" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="55"/>
-      <c r="C13" s="55"/>
-      <c r="D13" s="55"/>
-      <c r="E13" s="55"/>
-      <c r="F13" s="55"/>
-      <c r="G13" s="56"/>
-      <c r="K13" s="54" t="s">
+      <c r="B13" s="37"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="37"/>
+      <c r="G13" s="38"/>
+      <c r="K13" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="L13" s="55"/>
-      <c r="M13" s="55"/>
-      <c r="N13" s="55"/>
-      <c r="O13" s="55"/>
-      <c r="P13" s="55"/>
-      <c r="Q13" s="56"/>
+      <c r="L13" s="37"/>
+      <c r="M13" s="37"/>
+      <c r="N13" s="37"/>
+      <c r="O13" s="37"/>
+      <c r="P13" s="37"/>
+      <c r="Q13" s="38"/>
     </row>
     <row r="14" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="46" t="s">
+      <c r="A14" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="47"/>
-      <c r="C14" s="47"/>
-      <c r="D14" s="47"/>
-      <c r="E14" s="47"/>
-      <c r="F14" s="47"/>
-      <c r="G14" s="48"/>
-      <c r="K14" s="46" t="s">
+      <c r="B14" s="29"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="30"/>
+      <c r="K14" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="L14" s="47"/>
-      <c r="M14" s="47"/>
-      <c r="N14" s="47"/>
-      <c r="O14" s="47"/>
-      <c r="P14" s="47"/>
-      <c r="Q14" s="48"/>
+      <c r="L14" s="29"/>
+      <c r="M14" s="29"/>
+      <c r="N14" s="29"/>
+      <c r="O14" s="29"/>
+      <c r="P14" s="29"/>
+      <c r="Q14" s="30"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D15" s="9"/>
@@ -6428,34 +5704,47 @@
         <v>377</v>
       </c>
     </row>
-    <row r="17" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="F17" t="s">
+        <v>47</v>
+      </c>
       <c r="M17">
         <f>M9-M16</f>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:15" x14ac:dyDescent="0.25">
       <c r="N19" s="9">
         <f>3400+G9</f>
-        <v>20920.34</v>
-      </c>
-    </row>
-    <row r="20" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="G20" s="9"/>
+        <v>19749.125</v>
+      </c>
+    </row>
+    <row r="20" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="G20" s="9">
+        <f>SUM(G2:G8)</f>
+        <v>16349.125000000002</v>
+      </c>
       <c r="O20" s="9">
         <f>Q9/4</f>
         <v>16729</v>
       </c>
     </row>
-    <row r="21" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>49</v>
+      </c>
       <c r="D21" s="20">
-        <v>17520.34</v>
+        <f>G9</f>
+        <v>16349.125</v>
       </c>
       <c r="O21" s="18">
         <v>3400</v>
       </c>
     </row>
-    <row r="22" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>50</v>
+      </c>
       <c r="D22" s="9">
         <v>3400</v>
       </c>
@@ -6464,26 +5753,33 @@
         <v>20129</v>
       </c>
     </row>
-    <row r="23" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>21</v>
+      </c>
       <c r="D23" s="9">
         <f>D21+D22</f>
-        <v>20920.34</v>
-      </c>
-    </row>
-    <row r="25" spans="4:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="26" spans="4:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>19749.125</v>
+      </c>
+    </row>
+    <row r="25" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D26" s="21">
         <v>20129</v>
       </c>
     </row>
-    <row r="27" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:15" x14ac:dyDescent="0.25">
       <c r="D27" s="9">
         <f>D26-D23</f>
-        <v>-791.34000000000015</v>
-      </c>
-    </row>
-    <row r="29" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D29" s="40">
+        <v>379.875</v>
+      </c>
+      <c r="E27">
+        <f>D27/D26</f>
+        <v>1.8872025435938199E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="D29" s="25">
         <v>84.360000000000582</v>
       </c>
     </row>
@@ -6491,16 +5787,16 @@
       <c r="D37">
         <v>30.25</v>
       </c>
-      <c r="E37" s="40">
+      <c r="E37" s="25">
         <v>1167.5999999999999</v>
       </c>
-      <c r="F37" s="40">
-        <v>0</v>
-      </c>
-      <c r="G37" s="40">
+      <c r="F37" s="25">
+        <v>0</v>
+      </c>
+      <c r="G37" s="25">
         <v>505.81250000000006</v>
       </c>
-      <c r="H37" s="40">
+      <c r="H37" s="25">
         <v>3403.2</v>
       </c>
     </row>
@@ -6508,16 +5804,16 @@
       <c r="D38">
         <v>33</v>
       </c>
-      <c r="E38" s="40">
+      <c r="E38" s="25">
         <v>1264.8999999999999</v>
       </c>
-      <c r="F38" s="40">
-        <v>0</v>
-      </c>
-      <c r="G38" s="40">
+      <c r="F38" s="25">
+        <v>0</v>
+      </c>
+      <c r="G38" s="25">
         <v>566.51</v>
       </c>
-      <c r="H38" s="40">
+      <c r="H38" s="25">
         <v>4537.6000000000004</v>
       </c>
     </row>
@@ -6525,16 +5821,16 @@
       <c r="D39">
         <v>40</v>
       </c>
-      <c r="E39" s="40">
+      <c r="E39" s="25">
         <v>1581.125</v>
       </c>
-      <c r="F39" s="40">
-        <v>0</v>
-      </c>
-      <c r="G39" s="40">
+      <c r="F39" s="25">
+        <v>0</v>
+      </c>
+      <c r="G39" s="25">
         <v>606.97500000000002</v>
       </c>
-      <c r="H39" s="40">
+      <c r="H39" s="25">
         <v>7260.16</v>
       </c>
     </row>
@@ -6542,16 +5838,16 @@
       <c r="D40">
         <v>70</v>
       </c>
-      <c r="E40" s="40">
-        <v>0</v>
-      </c>
-      <c r="F40" s="40">
+      <c r="E40" s="25">
+        <v>0</v>
+      </c>
+      <c r="F40" s="25">
         <v>1855</v>
       </c>
-      <c r="G40" s="40">
+      <c r="G40" s="25">
         <v>1375.8100000000002</v>
       </c>
-      <c r="H40" s="40">
+      <c r="H40" s="25">
         <v>1680</v>
       </c>
     </row>
@@ -6559,16 +5855,16 @@
       <c r="D41">
         <v>107.5</v>
       </c>
-      <c r="E41" s="40">
-        <v>0</v>
-      </c>
-      <c r="F41" s="40">
+      <c r="E41" s="25">
+        <v>0</v>
+      </c>
+      <c r="F41" s="25">
         <v>3465</v>
       </c>
-      <c r="G41" s="40">
+      <c r="G41" s="25">
         <v>687.90500000000009</v>
       </c>
-      <c r="H41" s="40">
+      <c r="H41" s="25">
         <v>25200</v>
       </c>
     </row>
@@ -6576,16 +5872,16 @@
       <c r="D42">
         <v>28</v>
       </c>
-      <c r="E42" s="40">
+      <c r="E42" s="25">
         <v>729.75</v>
       </c>
-      <c r="F42" s="40">
-        <v>0</v>
-      </c>
-      <c r="G42" s="40">
+      <c r="F42" s="25">
+        <v>0</v>
+      </c>
+      <c r="G42" s="25">
         <v>1052.0900000000001</v>
       </c>
-      <c r="H42" s="40">
+      <c r="H42" s="25">
         <v>4764.4799999999996</v>
       </c>
     </row>
@@ -6593,16 +5889,16 @@
       <c r="D43">
         <v>29.25</v>
       </c>
-      <c r="E43" s="40">
+      <c r="E43" s="25">
         <v>875.69999999999993</v>
       </c>
-      <c r="F43" s="40">
-        <v>0</v>
-      </c>
-      <c r="G43" s="40">
+      <c r="F43" s="25">
+        <v>0</v>
+      </c>
+      <c r="G43" s="25">
         <v>910.46250000000009</v>
       </c>
-      <c r="H43" s="40">
+      <c r="H43" s="25">
         <v>8394.56</v>
       </c>
     </row>
@@ -6610,16 +5906,16 @@
       <c r="D44">
         <v>338</v>
       </c>
-      <c r="E44" s="40">
+      <c r="E44" s="25">
         <v>5619.0749999999998</v>
       </c>
-      <c r="F44" s="40">
+      <c r="F44" s="25">
         <v>5320</v>
       </c>
-      <c r="G44" s="40">
+      <c r="G44" s="25">
         <v>5705.5650000000005</v>
       </c>
-      <c r="H44" s="40">
+      <c r="H44" s="25">
         <v>16644.64</v>
       </c>
     </row>

</xml_diff>